<commit_message>
Run-hour warning for unit, compressor and EXV (not tested); bios and app revision;
</commit_message>
<xml_diff>
--- a/BZ172Lab/BZ172Lab Notes.xlsx
+++ b/BZ172Lab/BZ172Lab Notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BZ\Projects\PLC61131Repos\BZ172Lab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E485F0-FB36-4DD3-8C94-23464026ECB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{429236A4-2469-4FED-ABBE-8E18830E7CB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="4" r:id="rId1"/>
@@ -43,16 +43,16 @@
     <definedName name="CP_ID">Requirements!$B$159</definedName>
     <definedName name="CW_ID">Requirements!$B$87</definedName>
     <definedName name="EC_ID">Requirements!$B$95</definedName>
-    <definedName name="frs.all">Requirements!$B$3:$E$207</definedName>
-    <definedName name="frs.id">Requirements!$B$2:$B$207</definedName>
+    <definedName name="frs.all">Requirements!$B$3:$E$208</definedName>
+    <definedName name="frs.id">Requirements!$B$2:$B$208</definedName>
     <definedName name="FRS.Level" localSheetId="5">[1]Requirements!$D$4:$D$176</definedName>
-    <definedName name="FRS.Level">Requirements!$C$3:$C$207</definedName>
-    <definedName name="frs.requirement">Requirements!$E$2:$E$207</definedName>
+    <definedName name="FRS.Level">Requirements!$C$3:$C$208</definedName>
+    <definedName name="frs.requirement">Requirements!$E$2:$E$208</definedName>
     <definedName name="FRS.Status" localSheetId="5">[1]Requirements!$E$4:$E$176</definedName>
-    <definedName name="FRS.Status">Requirements!$D$3:$D$207</definedName>
-    <definedName name="FRSList">Requirements!$B$2:$F$203</definedName>
+    <definedName name="FRS.Status">Requirements!$D$3:$D$208</definedName>
+    <definedName name="FRSList">Requirements!$B$2:$F$204</definedName>
     <definedName name="GF_ID">Requirements!$B$3</definedName>
-    <definedName name="GP_ID">Requirements!$B$194</definedName>
+    <definedName name="GP_ID">Requirements!$B$195</definedName>
     <definedName name="notifications" localSheetId="5">OFFSET([2]Settings!$C$1,1,0,MATCH(REPT("z",255),[2]Settings!$C:$C),1)</definedName>
     <definedName name="notifications">OFFSET([3]Settings!$C$1,1,0,MATCH(REPT("z",255),[3]Settings!$C:$C),1)</definedName>
     <definedName name="priorities" localSheetId="5">[4]Settings!$A$2:$A$6</definedName>
@@ -171,7 +171,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2148" uniqueCount="840">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2151" uniqueCount="841">
   <si>
     <t>Author</t>
   </si>
@@ -2411,12 +2411,6 @@
     <t>EEV working time (EEVRunHours) should be traced with a percision of an hour.</t>
   </si>
   <si>
-    <t>Warning[51] : EEV Lifecycle
-    Entry  : EEVRunHours &gt;  EEVRunHours_cfg.
-    Exit      : EEVRunHours &lt; EEVRunHours_cfg.
-EEVRunHours is from [8736, 65535] with default 20208</t>
-  </si>
-  <si>
     <t>A binary hardware input (RSS) can override 'ON' status of the unit by putting it into 'OFF'.</t>
   </si>
   <si>
@@ -2488,12 +2482,6 @@
     <t>Fan status should be polled periodically?</t>
   </si>
   <si>
-    <t>Warning[70] : Compressor Lifecycle
-    Entry  : CompRunHours &gt;  CompRunHours_cfg.
-    Exit      : CompRunHours &lt; CompRunHours_cfg.
-CompRunHours is from [8736, 65535] with default 20208</t>
-  </si>
-  <si>
     <t>1.0 version</t>
   </si>
   <si>
@@ -2526,14 +2514,6 @@
   </si>
   <si>
     <t>RS485-1 (CN19) is the customer interface of data exchange by working as a MODBUS slave. By default, the communication parameters are 19200 8-E-1 and the address is 7.</t>
-  </si>
-  <si>
-    <t>BIOS (bzBIOSVersion) and application (bzAppVersion) version can be read from MODBUS.</t>
-  </si>
-  <si>
-    <t>Serial NO. and Model NO. can be preserved permanently.
-Serial NO (bzSerialNO) is string type with max length of 16 bytes
-Model NO (bzModelNO) is string type with max length of 16 bytes</t>
   </si>
   <si>
     <t>DDF overall design</t>
@@ -3216,6 +3196,37 @@
   </si>
   <si>
     <t>BZ172Lab</t>
+  </si>
+  <si>
+    <t>Warning[101] : Unit Lifecycle
+    Entry  : bzUnitRunhourLog is greater than bzUnitRunhourThresholdCfg.
+    Exit      : bzUnitRunhourLog is less than bzUnitRunhourThresholdCfg.
+bzUnitRunhourThresholdCfg is from [8736, 65535] with default 20208</t>
+  </si>
+  <si>
+    <t>Warning[51] : EEV Lifecycle
+    Entry  : bzEEVRunHourLog &gt;  bzEEVRunHourThresholdCfg.
+    Exit      : bzEEVRunHourLog &lt; bzEEVRunHourThresholdCfg.
+bzEEVRunHourThresholdCfg is from [8736, 65535] with default 20208</t>
+  </si>
+  <si>
+    <t>Warning[70] : Compressor Lifecycle
+    Entry  : bzCompressorRunHourLog &gt;  bzCompressorRunHourThresholdCfg.
+    Exit      : bzCompressorRunHourLog &lt; bzCompressorRunHourThresholdCfg.
+bzCompressorRunHourThresholdCfg is from [8736, 65535] with default 20208</t>
+  </si>
+  <si>
+    <t>Serial NO. and Model NO. can be preserved permanently.
+Serial NO (bzSerialNO) is string type with max length of 15 bytes
+Model NO (bzModelNO) is string type with max length of 15 bytes</t>
+  </si>
+  <si>
+    <t>BIOS (bzBIOSVersion) and application (bzAppVersion) version can be read from MODBUS.
+Max length of version string is 8
+The format of application version is YYMM.xxx where
+YY  is two-digit year, 20 for 2020 for example
+MM is the  acronym of the month that it is released. (JN,FB,MR,AP,MY,JN,JL,AG,SP,OT,NV,DC)
+and xxx is ordinal number for the release times in the specific month</t>
   </si>
 </sst>
 </file>
@@ -4887,16 +4898,46 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="10" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="11" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="18" xfId="11" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="10" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
@@ -4910,36 +4951,6 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="15" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="11" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="18" xfId="11" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="2" borderId="1" xfId="12" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4977,151 +4988,6 @@
   </cellStyles>
   <dxfs count="132">
     <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="hair">
-          <color indexed="64"/>
-        </left>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yy;@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="hair">
-          <color indexed="64"/>
-        </left>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top style="hair">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="hair">
-          <color indexed="64"/>
-        </left>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top style="hair">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="hair">
-          <color indexed="64"/>
-        </left>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top style="hair">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="hair">
-          <color indexed="64"/>
-        </left>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top style="hair">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="hair">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="hair">
-          <color indexed="64"/>
-        </left>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <bgColor rgb="FF92D050"/>
@@ -5148,243 +5014,6 @@
           <bgColor rgb="FF00B0F0"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="hair">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="hair">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="hair">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="hair">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="hair">
-          <color indexed="64"/>
-        </left>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top style="hair">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="hair">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="hair">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top style="hair">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="hair">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="hair">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="hair">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="hair">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top style="hair">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="hair">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="hair">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="hair">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="hair">
-          <color indexed="64"/>
-        </left>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top style="hair">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="hair">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="hair">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top style="hair">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="hair">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="hair">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="double">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -5421,152 +5050,6 @@
         <i val="0"/>
         <color rgb="FFFF0000"/>
       </font>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="hair">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="hair">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="hair">
-          <color indexed="64"/>
-        </left>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top style="hair">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="hair">
-          <color indexed="64"/>
-        </left>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top style="hair">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="hair">
-          <color indexed="64"/>
-        </left>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top style="hair">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top style="hair">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color rgb="FF3F3F3F"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="3"/>
-        <name val="Cambria"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFCC99"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF7F7F7F"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF7F7F7F"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -6048,6 +5531,534 @@
         <b val="0"/>
         <i/>
       </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="hair">
+          <color indexed="64"/>
+        </left>
+        <right/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yy;@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="hair">
+          <color indexed="64"/>
+        </left>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top style="hair">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="hair">
+          <color indexed="64"/>
+        </left>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top style="hair">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="hair">
+          <color indexed="64"/>
+        </left>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top style="hair">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="hair">
+          <color indexed="64"/>
+        </left>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top style="hair">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="hair">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="hair">
+          <color indexed="64"/>
+        </left>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="hair">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="hair">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="hair">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="hair">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="hair">
+          <color indexed="64"/>
+        </left>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top style="hair">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="hair">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="hair">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top style="hair">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="hair">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="hair">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="hair">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="hair">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top style="hair">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="hair">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="hair">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="hair">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="hair">
+          <color indexed="64"/>
+        </left>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top style="hair">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="hair">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="hair">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top style="hair">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="hair">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="hair">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="double">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="hair">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="hair">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="hair">
+          <color indexed="64"/>
+        </left>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top style="hair">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="hair">
+          <color indexed="64"/>
+        </left>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top style="hair">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="hair">
+          <color indexed="64"/>
+        </left>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top style="hair">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top style="hair">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color rgb="FF3F3F3F"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="3"/>
+        <name val="Cambria"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFCC99"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF7F7F7F"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF7F7F7F"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -8486,51 +8497,51 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DA4C32D8-628E-4DC9-877D-4ED51980429C}" name="Table2" displayName="Table2" ref="B2:F200" totalsRowShown="0" headerRowDxfId="38" tableBorderDxfId="37">
-  <autoFilter ref="B2:F200" xr:uid="{CDEA0ADE-0555-4D01-8A61-CFA14708222C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DA4C32D8-628E-4DC9-877D-4ED51980429C}" name="Table2" displayName="Table2" ref="B2:F201" totalsRowShown="0" headerRowDxfId="129" tableBorderDxfId="128">
+  <autoFilter ref="B2:F201" xr:uid="{CDEA0ADE-0555-4D01-8A61-CFA14708222C}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{EEC440CC-C59E-404F-9916-B7B335C0A1FA}" name="ID" dataDxfId="36"/>
-    <tableColumn id="2" xr3:uid="{0D454755-1962-49B9-A9AE-DE3621F55672}" name="LEVEL" dataDxfId="35"/>
-    <tableColumn id="3" xr3:uid="{9BA24605-273E-4985-933B-06818CBA9537}" name="STATUS" dataDxfId="34"/>
-    <tableColumn id="4" xr3:uid="{53754EA4-50A6-4DD8-9232-D08866425BE4}" name="REQUIREMENT" dataDxfId="33"/>
-    <tableColumn id="5" xr3:uid="{1B4BE84A-D954-4677-AFFC-A0D5CAB7D3BA}" name="COMMENT" dataDxfId="32"/>
+    <tableColumn id="1" xr3:uid="{EEC440CC-C59E-404F-9916-B7B335C0A1FA}" name="ID" dataDxfId="127"/>
+    <tableColumn id="2" xr3:uid="{0D454755-1962-49B9-A9AE-DE3621F55672}" name="LEVEL" dataDxfId="126"/>
+    <tableColumn id="3" xr3:uid="{9BA24605-273E-4985-933B-06818CBA9537}" name="STATUS" dataDxfId="125"/>
+    <tableColumn id="4" xr3:uid="{53754EA4-50A6-4DD8-9232-D08866425BE4}" name="REQUIREMENT" dataDxfId="124"/>
+    <tableColumn id="5" xr3:uid="{1B4BE84A-D954-4677-AFFC-A0D5CAB7D3BA}" name="COMMENT" dataDxfId="123"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AAF4E3A6-1435-4943-A0FB-7E69B9E573B3}" name="Table1" displayName="Table1" ref="B2:K86" totalsRowShown="0" headerRowDxfId="28" headerRowBorderDxfId="27" tableBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AAF4E3A6-1435-4943-A0FB-7E69B9E573B3}" name="Table1" displayName="Table1" ref="B2:K86" totalsRowShown="0" headerRowDxfId="122" headerRowBorderDxfId="121" tableBorderDxfId="120">
   <autoFilter ref="B2:K86" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{BA3BC7BB-ECE4-462B-8824-97F388F144C5}" name="ID" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{C7FEB3E5-CB44-4B6C-9037-3D4D80F11092}" name="Task" dataDxfId="24"/>
-    <tableColumn id="6" xr3:uid="{DA8AC2B3-0FDD-4A71-9D23-75C65B931AE5}" name="Due" dataDxfId="23"/>
-    <tableColumn id="11" xr3:uid="{79F1150C-F5DC-407D-B8EC-D7D0577E0197}" name="Days" dataDxfId="22">
+    <tableColumn id="1" xr3:uid="{BA3BC7BB-ECE4-462B-8824-97F388F144C5}" name="ID" dataDxfId="119"/>
+    <tableColumn id="2" xr3:uid="{C7FEB3E5-CB44-4B6C-9037-3D4D80F11092}" name="Task" dataDxfId="118"/>
+    <tableColumn id="6" xr3:uid="{DA8AC2B3-0FDD-4A71-9D23-75C65B931AE5}" name="Due" dataDxfId="117"/>
+    <tableColumn id="11" xr3:uid="{79F1150C-F5DC-407D-B8EC-D7D0577E0197}" name="Days" dataDxfId="116">
       <calculatedColumnFormula>IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{9690982A-833C-4E42-9ED5-2EFA892551CE}" name="PRI" dataDxfId="21"/>
-    <tableColumn id="7" xr3:uid="{94174600-EB70-4A9B-9222-C70BB59D0A17}" name="BL" dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{89F020A6-CB77-4228-B7A9-9FA1CA50D659}" name="PROG" dataDxfId="19"/>
-    <tableColumn id="8" xr3:uid="{62190683-A6A8-4A1D-8C2C-F4AA5A1AA84F}" name="Owners" dataDxfId="18"/>
-    <tableColumn id="9" xr3:uid="{212AD8CC-8A46-4EF1-A572-52656BE74CC0}" name="Prerequisites" dataDxfId="17"/>
-    <tableColumn id="10" xr3:uid="{47B4D71F-1414-4149-9932-EF0D1879BE1E}" name="Deliverables" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{9690982A-833C-4E42-9ED5-2EFA892551CE}" name="PRI" dataDxfId="115"/>
+    <tableColumn id="7" xr3:uid="{94174600-EB70-4A9B-9222-C70BB59D0A17}" name="BL" dataDxfId="114"/>
+    <tableColumn id="4" xr3:uid="{89F020A6-CB77-4228-B7A9-9FA1CA50D659}" name="PROG" dataDxfId="113"/>
+    <tableColumn id="8" xr3:uid="{62190683-A6A8-4A1D-8C2C-F4AA5A1AA84F}" name="Owners" dataDxfId="112"/>
+    <tableColumn id="9" xr3:uid="{212AD8CC-8A46-4EF1-A572-52656BE74CC0}" name="Prerequisites" dataDxfId="111"/>
+    <tableColumn id="10" xr3:uid="{47B4D71F-1414-4149-9932-EF0D1879BE1E}" name="Deliverables" dataDxfId="110"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="VerificationTable" displayName="VerificationTable" ref="B9:I29" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="VerificationTable" displayName="VerificationTable" ref="B9:I29" totalsRowShown="0" headerRowDxfId="109" headerRowBorderDxfId="108" tableBorderDxfId="107" totalsRowBorderDxfId="106">
   <tableColumns count="8">
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="NO." dataDxfId="7"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Issue_x000a_Description" dataDxfId="6"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Category" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Found_x000a_Version" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Repaired _x000a_Version" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Last_x000a_Date" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Status" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Comment" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="NO." dataDxfId="105"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Issue_x000a_Description" dataDxfId="104"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Category" dataDxfId="103"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Found_x000a_Version" dataDxfId="102"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Repaired _x000a_Version" dataDxfId="101"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Last_x000a_Date" dataDxfId="100"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Status" dataDxfId="99"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Comment" dataDxfId="98"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8860,7 +8871,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="D4:O22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D10" sqref="D10:O13"/>
     </sheetView>
   </sheetViews>
@@ -8871,7 +8882,7 @@
   <sheetData>
     <row r="4" spans="4:15">
       <c r="D4" s="207" t="s">
-        <v>839</v>
+        <v>835</v>
       </c>
       <c r="E4" s="207"/>
       <c r="F4" s="207"/>
@@ -9017,7 +9028,7 @@
       </c>
       <c r="E21" s="205"/>
       <c r="F21" s="206" t="s">
-        <v>769</v>
+        <v>765</v>
       </c>
       <c r="G21" s="206"/>
       <c r="H21" s="206"/>
@@ -9029,7 +9040,7 @@
       </c>
       <c r="F22" s="204">
         <f ca="1">TODAY()</f>
-        <v>44245</v>
+        <v>44249</v>
       </c>
       <c r="G22" s="204"/>
       <c r="H22" s="204"/>
@@ -9428,16 +9439,16 @@
   </mergeCells>
   <phoneticPr fontId="22" type="noConversion"/>
   <conditionalFormatting sqref="H10:H29">
-    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"As Design"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"Close"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>"Fixed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9713,7 +9724,7 @@
   <dimension ref="E3:F17"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -9753,7 +9764,7 @@
         <v>44221</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
     </row>
     <row r="7" spans="5:6">
@@ -9761,7 +9772,7 @@
         <v>44237</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>816</v>
+        <v>812</v>
       </c>
     </row>
     <row r="8" spans="5:6">
@@ -9825,34 +9836,34 @@
   </cols>
   <sheetData>
     <row r="2" spans="4:7">
-      <c r="D2" s="226">
+      <c r="D2" s="216">
         <f ca="1">TODAY()</f>
-        <v>44245</v>
-      </c>
-      <c r="E2" s="226"/>
-      <c r="F2" s="226"/>
+        <v>44249</v>
+      </c>
+      <c r="E2" s="216"/>
+      <c r="F2" s="216"/>
     </row>
     <row r="3" spans="4:7">
-      <c r="D3" s="227"/>
-      <c r="E3" s="227"/>
-      <c r="F3" s="227"/>
+      <c r="D3" s="217"/>
+      <c r="E3" s="217"/>
+      <c r="F3" s="217"/>
     </row>
     <row r="4" spans="4:7">
-      <c r="D4" s="225" t="s">
+      <c r="D4" s="215" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="225"/>
+      <c r="E4" s="215"/>
       <c r="F4" s="27">
         <f>COUNTIF(FRS.Level, D4)</f>
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G4" s="26"/>
     </row>
     <row r="5" spans="4:7">
-      <c r="D5" s="225" t="s">
+      <c r="D5" s="215" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="225"/>
+      <c r="E5" s="215"/>
       <c r="F5" s="27">
         <f>COUNTIF(FRS.Level, D5)</f>
         <v>7</v>
@@ -9860,10 +9871,10 @@
       <c r="G5" s="26"/>
     </row>
     <row r="6" spans="4:7">
-      <c r="D6" s="225" t="s">
+      <c r="D6" s="215" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="225"/>
+      <c r="E6" s="215"/>
       <c r="F6" s="27">
         <f>COUNTIF(FRS.Level, D6)</f>
         <v>5</v>
@@ -9871,10 +9882,10 @@
       <c r="G6" s="26"/>
     </row>
     <row r="7" spans="4:7">
-      <c r="D7" s="225" t="s">
+      <c r="D7" s="215" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="225"/>
+      <c r="E7" s="215"/>
       <c r="F7" s="27">
         <f>COUNTIF(FRS.Level, D7)</f>
         <v>0</v>
@@ -9886,139 +9897,139 @@
       <c r="E8" s="25"/>
       <c r="F8" s="27">
         <f>SUM(F4:F7)</f>
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="G8" s="26"/>
     </row>
     <row r="10" spans="4:7">
-      <c r="D10" s="225" t="s">
+      <c r="D10" s="215" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="225"/>
+      <c r="E10" s="215"/>
       <c r="F10" s="27">
         <f t="shared" ref="F10:F16" si="0">COUNTIF(FRS.Status,D10)</f>
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="4:7">
-      <c r="D11" s="225" t="s">
+      <c r="D11" s="215" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="225"/>
+      <c r="E11" s="215"/>
       <c r="F11" s="27">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="4:7">
-      <c r="D12" s="225" t="s">
+      <c r="D12" s="215" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="225"/>
+      <c r="E12" s="215"/>
       <c r="F12" s="27">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="4:7">
-      <c r="D13" s="225" t="s">
+      <c r="D13" s="215" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="225"/>
+      <c r="E13" s="215"/>
       <c r="F13" s="27">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
     <row r="14" spans="4:7">
-      <c r="D14" s="225" t="s">
+      <c r="D14" s="215" t="s">
         <v>24</v>
       </c>
-      <c r="E14" s="225"/>
+      <c r="E14" s="215"/>
       <c r="F14" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="4:7">
-      <c r="D15" s="225" t="s">
+      <c r="D15" s="215" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="225"/>
+      <c r="E15" s="215"/>
       <c r="F15" s="27">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="4:7">
-      <c r="D16" s="225" t="s">
+      <c r="D16" s="215" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="225"/>
+      <c r="E16" s="215"/>
       <c r="F16" s="27">
         <f t="shared" si="0"/>
-        <v>75</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="4:19" ht="20.25" thickBot="1">
-      <c r="D18" s="217" t="s">
+      <c r="D18" s="227" t="s">
         <v>46</v>
       </c>
-      <c r="E18" s="217"/>
-      <c r="F18" s="217"/>
-      <c r="G18" s="217"/>
-      <c r="H18" s="216" t="s">
+      <c r="E18" s="227"/>
+      <c r="F18" s="227"/>
+      <c r="G18" s="227"/>
+      <c r="H18" s="226" t="s">
         <v>47</v>
       </c>
-      <c r="I18" s="216"/>
-      <c r="J18" s="216"/>
-      <c r="K18" s="216"/>
-      <c r="L18" s="216"/>
-      <c r="M18" s="216"/>
-      <c r="N18" s="216"/>
-      <c r="O18" s="216"/>
-      <c r="P18" s="216"/>
-      <c r="Q18" s="216"/>
+      <c r="I18" s="226"/>
+      <c r="J18" s="226"/>
+      <c r="K18" s="226"/>
+      <c r="L18" s="226"/>
+      <c r="M18" s="226"/>
+      <c r="N18" s="226"/>
+      <c r="O18" s="226"/>
+      <c r="P18" s="226"/>
+      <c r="Q18" s="226"/>
     </row>
     <row r="19" spans="4:19" ht="15.75" thickTop="1">
-      <c r="D19" s="210" t="s">
+      <c r="D19" s="223" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="210"/>
-      <c r="F19" s="210" t="s">
+      <c r="E19" s="223"/>
+      <c r="F19" s="223" t="s">
         <v>2</v>
       </c>
-      <c r="G19" s="210"/>
-      <c r="H19" s="210" t="s">
+      <c r="G19" s="223"/>
+      <c r="H19" s="223" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="210"/>
-      <c r="J19" s="210" t="s">
+      <c r="I19" s="223"/>
+      <c r="J19" s="223" t="s">
         <v>18</v>
       </c>
-      <c r="K19" s="210"/>
-      <c r="L19" s="210" t="s">
+      <c r="K19" s="223"/>
+      <c r="L19" s="223" t="s">
         <v>15</v>
       </c>
-      <c r="M19" s="210"/>
-      <c r="N19" s="210" t="s">
+      <c r="M19" s="223"/>
+      <c r="N19" s="223" t="s">
         <v>21</v>
       </c>
-      <c r="O19" s="210"/>
-      <c r="P19" s="210" t="s">
+      <c r="O19" s="223"/>
+      <c r="P19" s="223" t="s">
         <v>29</v>
       </c>
-      <c r="Q19" s="210"/>
+      <c r="Q19" s="223"/>
     </row>
     <row r="20" spans="4:19">
-      <c r="D20" s="211">
+      <c r="D20" s="210">
         <v>44221</v>
       </c>
-      <c r="E20" s="212"/>
-      <c r="F20" s="220" t="s">
+      <c r="E20" s="211"/>
+      <c r="F20" s="212" t="s">
         <v>109</v>
       </c>
-      <c r="G20" s="220"/>
+      <c r="G20" s="212"/>
       <c r="H20" s="213">
         <v>8</v>
       </c>
@@ -10035,21 +10046,21 @@
         <v>0</v>
       </c>
       <c r="O20" s="213"/>
-      <c r="P20" s="214">
+      <c r="P20" s="224">
         <v>0</v>
       </c>
-      <c r="Q20" s="215"/>
+      <c r="Q20" s="225"/>
       <c r="S20" s="28"/>
     </row>
     <row r="21" spans="4:19">
-      <c r="D21" s="211">
+      <c r="D21" s="210">
         <v>44237</v>
       </c>
-      <c r="E21" s="212"/>
-      <c r="F21" s="220" t="s">
-        <v>769</v>
-      </c>
-      <c r="G21" s="220"/>
+      <c r="E21" s="211"/>
+      <c r="F21" s="212" t="s">
+        <v>765</v>
+      </c>
+      <c r="G21" s="212"/>
       <c r="H21" s="213">
         <v>9</v>
       </c>
@@ -10069,17 +10080,17 @@
       <c r="P21" s="213">
         <v>56</v>
       </c>
-      <c r="Q21" s="223"/>
+      <c r="Q21" s="214"/>
     </row>
     <row r="22" spans="4:19">
-      <c r="D22" s="211">
+      <c r="D22" s="210">
         <v>44256</v>
       </c>
-      <c r="E22" s="212"/>
-      <c r="F22" s="220" t="s">
-        <v>833</v>
-      </c>
-      <c r="G22" s="220"/>
+      <c r="E22" s="211"/>
+      <c r="F22" s="212" t="s">
+        <v>829</v>
+      </c>
+      <c r="G22" s="212"/>
       <c r="H22" s="213"/>
       <c r="I22" s="213"/>
       <c r="J22" s="213"/>
@@ -10089,13 +10100,13 @@
       <c r="N22" s="213"/>
       <c r="O22" s="213"/>
       <c r="P22" s="213"/>
-      <c r="Q22" s="223"/>
+      <c r="Q22" s="214"/>
     </row>
     <row r="23" spans="4:19">
-      <c r="D23" s="211"/>
-      <c r="E23" s="212"/>
-      <c r="F23" s="220"/>
-      <c r="G23" s="220"/>
+      <c r="D23" s="210"/>
+      <c r="E23" s="211"/>
+      <c r="F23" s="212"/>
+      <c r="G23" s="212"/>
       <c r="H23" s="213"/>
       <c r="I23" s="213"/>
       <c r="J23" s="213"/>
@@ -10105,13 +10116,13 @@
       <c r="N23" s="213"/>
       <c r="O23" s="213"/>
       <c r="P23" s="213"/>
-      <c r="Q23" s="223"/>
+      <c r="Q23" s="214"/>
     </row>
     <row r="24" spans="4:19">
-      <c r="D24" s="211"/>
-      <c r="E24" s="212"/>
-      <c r="F24" s="220"/>
-      <c r="G24" s="220"/>
+      <c r="D24" s="210"/>
+      <c r="E24" s="211"/>
+      <c r="F24" s="212"/>
+      <c r="G24" s="212"/>
       <c r="H24" s="213"/>
       <c r="I24" s="213"/>
       <c r="J24" s="213"/>
@@ -10121,13 +10132,13 @@
       <c r="N24" s="213"/>
       <c r="O24" s="213"/>
       <c r="P24" s="213"/>
-      <c r="Q24" s="223"/>
+      <c r="Q24" s="214"/>
     </row>
     <row r="25" spans="4:19">
-      <c r="D25" s="211"/>
-      <c r="E25" s="212"/>
-      <c r="F25" s="220"/>
-      <c r="G25" s="220"/>
+      <c r="D25" s="210"/>
+      <c r="E25" s="211"/>
+      <c r="F25" s="212"/>
+      <c r="G25" s="212"/>
       <c r="H25" s="213"/>
       <c r="I25" s="213"/>
       <c r="J25" s="213"/>
@@ -10137,13 +10148,13 @@
       <c r="N25" s="213"/>
       <c r="O25" s="213"/>
       <c r="P25" s="213"/>
-      <c r="Q25" s="223"/>
+      <c r="Q25" s="214"/>
     </row>
     <row r="26" spans="4:19">
-      <c r="D26" s="211"/>
-      <c r="E26" s="212"/>
-      <c r="F26" s="220"/>
-      <c r="G26" s="220"/>
+      <c r="D26" s="210"/>
+      <c r="E26" s="211"/>
+      <c r="F26" s="212"/>
+      <c r="G26" s="212"/>
       <c r="H26" s="213"/>
       <c r="I26" s="213"/>
       <c r="J26" s="213"/>
@@ -10153,13 +10164,13 @@
       <c r="N26" s="213"/>
       <c r="O26" s="213"/>
       <c r="P26" s="213"/>
-      <c r="Q26" s="223"/>
+      <c r="Q26" s="214"/>
     </row>
     <row r="27" spans="4:19">
-      <c r="D27" s="211"/>
-      <c r="E27" s="212"/>
-      <c r="F27" s="220"/>
-      <c r="G27" s="220"/>
+      <c r="D27" s="210"/>
+      <c r="E27" s="211"/>
+      <c r="F27" s="212"/>
+      <c r="G27" s="212"/>
       <c r="H27" s="213"/>
       <c r="I27" s="213"/>
       <c r="J27" s="213"/>
@@ -10169,13 +10180,13 @@
       <c r="N27" s="213"/>
       <c r="O27" s="213"/>
       <c r="P27" s="213"/>
-      <c r="Q27" s="223"/>
+      <c r="Q27" s="214"/>
     </row>
     <row r="28" spans="4:19">
-      <c r="D28" s="211"/>
-      <c r="E28" s="212"/>
-      <c r="F28" s="220"/>
-      <c r="G28" s="220"/>
+      <c r="D28" s="210"/>
+      <c r="E28" s="211"/>
+      <c r="F28" s="212"/>
+      <c r="G28" s="212"/>
       <c r="H28" s="213"/>
       <c r="I28" s="213"/>
       <c r="J28" s="213"/>
@@ -10185,13 +10196,13 @@
       <c r="N28" s="213"/>
       <c r="O28" s="213"/>
       <c r="P28" s="213"/>
-      <c r="Q28" s="223"/>
+      <c r="Q28" s="214"/>
     </row>
     <row r="29" spans="4:19">
-      <c r="D29" s="211"/>
-      <c r="E29" s="212"/>
-      <c r="F29" s="220"/>
-      <c r="G29" s="220"/>
+      <c r="D29" s="210"/>
+      <c r="E29" s="211"/>
+      <c r="F29" s="212"/>
+      <c r="G29" s="212"/>
       <c r="H29" s="213"/>
       <c r="I29" s="213"/>
       <c r="J29" s="213"/>
@@ -10201,13 +10212,13 @@
       <c r="N29" s="213"/>
       <c r="O29" s="213"/>
       <c r="P29" s="213"/>
-      <c r="Q29" s="223"/>
+      <c r="Q29" s="214"/>
     </row>
     <row r="30" spans="4:19">
-      <c r="D30" s="211"/>
-      <c r="E30" s="212"/>
-      <c r="F30" s="220"/>
-      <c r="G30" s="220"/>
+      <c r="D30" s="210"/>
+      <c r="E30" s="211"/>
+      <c r="F30" s="212"/>
+      <c r="G30" s="212"/>
       <c r="H30" s="213"/>
       <c r="I30" s="213"/>
       <c r="J30" s="213"/>
@@ -10217,13 +10228,13 @@
       <c r="N30" s="213"/>
       <c r="O30" s="213"/>
       <c r="P30" s="213"/>
-      <c r="Q30" s="223"/>
+      <c r="Q30" s="214"/>
     </row>
     <row r="31" spans="4:19">
-      <c r="D31" s="211"/>
-      <c r="E31" s="212"/>
-      <c r="F31" s="220"/>
-      <c r="G31" s="220"/>
+      <c r="D31" s="210"/>
+      <c r="E31" s="211"/>
+      <c r="F31" s="212"/>
+      <c r="G31" s="212"/>
       <c r="H31" s="213"/>
       <c r="I31" s="213"/>
       <c r="J31" s="213"/>
@@ -10233,13 +10244,13 @@
       <c r="N31" s="213"/>
       <c r="O31" s="213"/>
       <c r="P31" s="213"/>
-      <c r="Q31" s="223"/>
+      <c r="Q31" s="214"/>
     </row>
     <row r="32" spans="4:19">
-      <c r="D32" s="211"/>
-      <c r="E32" s="212"/>
-      <c r="F32" s="220"/>
-      <c r="G32" s="220"/>
+      <c r="D32" s="210"/>
+      <c r="E32" s="211"/>
+      <c r="F32" s="212"/>
+      <c r="G32" s="212"/>
       <c r="H32" s="213"/>
       <c r="I32" s="213"/>
       <c r="J32" s="213"/>
@@ -10249,13 +10260,13 @@
       <c r="N32" s="213"/>
       <c r="O32" s="213"/>
       <c r="P32" s="213"/>
-      <c r="Q32" s="223"/>
+      <c r="Q32" s="214"/>
     </row>
     <row r="33" spans="4:17">
-      <c r="D33" s="211"/>
-      <c r="E33" s="212"/>
-      <c r="F33" s="220"/>
-      <c r="G33" s="220"/>
+      <c r="D33" s="210"/>
+      <c r="E33" s="211"/>
+      <c r="F33" s="212"/>
+      <c r="G33" s="212"/>
       <c r="H33" s="213"/>
       <c r="I33" s="213"/>
       <c r="J33" s="213"/>
@@ -10265,13 +10276,13 @@
       <c r="N33" s="213"/>
       <c r="O33" s="213"/>
       <c r="P33" s="213"/>
-      <c r="Q33" s="223"/>
+      <c r="Q33" s="214"/>
     </row>
     <row r="34" spans="4:17">
-      <c r="D34" s="211"/>
-      <c r="E34" s="212"/>
-      <c r="F34" s="220"/>
-      <c r="G34" s="220"/>
+      <c r="D34" s="210"/>
+      <c r="E34" s="211"/>
+      <c r="F34" s="212"/>
+      <c r="G34" s="212"/>
       <c r="H34" s="213"/>
       <c r="I34" s="213"/>
       <c r="J34" s="213"/>
@@ -10281,13 +10292,13 @@
       <c r="N34" s="213"/>
       <c r="O34" s="213"/>
       <c r="P34" s="213"/>
-      <c r="Q34" s="223"/>
+      <c r="Q34" s="214"/>
     </row>
     <row r="35" spans="4:17">
-      <c r="D35" s="211"/>
-      <c r="E35" s="212"/>
-      <c r="F35" s="220"/>
-      <c r="G35" s="220"/>
+      <c r="D35" s="210"/>
+      <c r="E35" s="211"/>
+      <c r="F35" s="212"/>
+      <c r="G35" s="212"/>
       <c r="H35" s="213"/>
       <c r="I35" s="213"/>
       <c r="J35" s="213"/>
@@ -10297,13 +10308,13 @@
       <c r="N35" s="213"/>
       <c r="O35" s="213"/>
       <c r="P35" s="213"/>
-      <c r="Q35" s="223"/>
+      <c r="Q35" s="214"/>
     </row>
     <row r="36" spans="4:17">
-      <c r="D36" s="211"/>
-      <c r="E36" s="212"/>
-      <c r="F36" s="220"/>
-      <c r="G36" s="220"/>
+      <c r="D36" s="210"/>
+      <c r="E36" s="211"/>
+      <c r="F36" s="212"/>
+      <c r="G36" s="212"/>
       <c r="H36" s="213"/>
       <c r="I36" s="213"/>
       <c r="J36" s="213"/>
@@ -10313,13 +10324,13 @@
       <c r="N36" s="213"/>
       <c r="O36" s="213"/>
       <c r="P36" s="213"/>
-      <c r="Q36" s="223"/>
+      <c r="Q36" s="214"/>
     </row>
     <row r="37" spans="4:17">
-      <c r="D37" s="211"/>
-      <c r="E37" s="212"/>
-      <c r="F37" s="220"/>
-      <c r="G37" s="220"/>
+      <c r="D37" s="210"/>
+      <c r="E37" s="211"/>
+      <c r="F37" s="212"/>
+      <c r="G37" s="212"/>
       <c r="H37" s="213"/>
       <c r="I37" s="213"/>
       <c r="J37" s="213"/>
@@ -10329,13 +10340,13 @@
       <c r="N37" s="213"/>
       <c r="O37" s="213"/>
       <c r="P37" s="213"/>
-      <c r="Q37" s="223"/>
+      <c r="Q37" s="214"/>
     </row>
     <row r="38" spans="4:17">
-      <c r="D38" s="211"/>
-      <c r="E38" s="212"/>
-      <c r="F38" s="220"/>
-      <c r="G38" s="220"/>
+      <c r="D38" s="210"/>
+      <c r="E38" s="211"/>
+      <c r="F38" s="212"/>
+      <c r="G38" s="212"/>
       <c r="H38" s="213"/>
       <c r="I38" s="213"/>
       <c r="J38" s="213"/>
@@ -10345,13 +10356,13 @@
       <c r="N38" s="213"/>
       <c r="O38" s="213"/>
       <c r="P38" s="213"/>
-      <c r="Q38" s="223"/>
+      <c r="Q38" s="214"/>
     </row>
     <row r="39" spans="4:17">
-      <c r="D39" s="211"/>
-      <c r="E39" s="212"/>
-      <c r="F39" s="220"/>
-      <c r="G39" s="220"/>
+      <c r="D39" s="210"/>
+      <c r="E39" s="211"/>
+      <c r="F39" s="212"/>
+      <c r="G39" s="212"/>
       <c r="H39" s="213"/>
       <c r="I39" s="213"/>
       <c r="J39" s="213"/>
@@ -10361,23 +10372,23 @@
       <c r="N39" s="213"/>
       <c r="O39" s="213"/>
       <c r="P39" s="213"/>
-      <c r="Q39" s="223"/>
+      <c r="Q39" s="214"/>
     </row>
     <row r="40" spans="4:17">
-      <c r="D40" s="218"/>
-      <c r="E40" s="219"/>
-      <c r="F40" s="221"/>
-      <c r="G40" s="221"/>
-      <c r="H40" s="222"/>
-      <c r="I40" s="222"/>
-      <c r="J40" s="222"/>
-      <c r="K40" s="222"/>
-      <c r="L40" s="222"/>
-      <c r="M40" s="222"/>
-      <c r="N40" s="222"/>
-      <c r="O40" s="222"/>
-      <c r="P40" s="222"/>
-      <c r="Q40" s="224"/>
+      <c r="D40" s="221"/>
+      <c r="E40" s="222"/>
+      <c r="F40" s="220"/>
+      <c r="G40" s="220"/>
+      <c r="H40" s="218"/>
+      <c r="I40" s="218"/>
+      <c r="J40" s="218"/>
+      <c r="K40" s="218"/>
+      <c r="L40" s="218"/>
+      <c r="M40" s="218"/>
+      <c r="N40" s="218"/>
+      <c r="O40" s="218"/>
+      <c r="P40" s="218"/>
+      <c r="Q40" s="219"/>
     </row>
     <row r="41" spans="4:17">
       <c r="D41" s="24"/>
@@ -10385,71 +10396,85 @@
     </row>
   </sheetData>
   <mergeCells count="168">
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="J34:K34"/>
-    <mergeCell ref="L34:M34"/>
-    <mergeCell ref="N34:O34"/>
-    <mergeCell ref="P34:Q34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="J35:K35"/>
-    <mergeCell ref="L35:M35"/>
-    <mergeCell ref="N35:O35"/>
-    <mergeCell ref="P35:Q35"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="L31:M31"/>
-    <mergeCell ref="N31:O31"/>
-    <mergeCell ref="P31:Q31"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="L29:M29"/>
-    <mergeCell ref="N29:O29"/>
-    <mergeCell ref="P29:Q29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="N30:O30"/>
-    <mergeCell ref="P30:Q30"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D2:F3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="P38:Q38"/>
-    <mergeCell ref="P39:Q39"/>
-    <mergeCell ref="P40:Q40"/>
-    <mergeCell ref="P26:Q26"/>
-    <mergeCell ref="P27:Q27"/>
-    <mergeCell ref="P28:Q28"/>
-    <mergeCell ref="P32:Q32"/>
-    <mergeCell ref="P33:Q33"/>
-    <mergeCell ref="P36:Q36"/>
-    <mergeCell ref="P21:Q21"/>
-    <mergeCell ref="P22:Q22"/>
-    <mergeCell ref="P23:Q23"/>
-    <mergeCell ref="P24:Q24"/>
-    <mergeCell ref="P25:Q25"/>
-    <mergeCell ref="N33:O33"/>
-    <mergeCell ref="N36:O36"/>
-    <mergeCell ref="N37:O37"/>
-    <mergeCell ref="P37:Q37"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="H18:Q18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="D18:G18"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="L40:M40"/>
+    <mergeCell ref="L26:M26"/>
+    <mergeCell ref="L27:M27"/>
+    <mergeCell ref="L28:M28"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="L33:M33"/>
+    <mergeCell ref="L36:M36"/>
+    <mergeCell ref="N40:O40"/>
+    <mergeCell ref="J33:K33"/>
+    <mergeCell ref="J36:K36"/>
+    <mergeCell ref="J37:K37"/>
+    <mergeCell ref="J38:K38"/>
+    <mergeCell ref="J39:K39"/>
+    <mergeCell ref="J40:K40"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="J32:K32"/>
     <mergeCell ref="J21:K21"/>
     <mergeCell ref="J22:K22"/>
     <mergeCell ref="L21:M21"/>
@@ -10474,85 +10499,71 @@
     <mergeCell ref="J23:K23"/>
     <mergeCell ref="J24:K24"/>
     <mergeCell ref="J25:K25"/>
-    <mergeCell ref="L40:M40"/>
-    <mergeCell ref="L26:M26"/>
-    <mergeCell ref="L27:M27"/>
-    <mergeCell ref="L28:M28"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="L33:M33"/>
-    <mergeCell ref="L36:M36"/>
-    <mergeCell ref="N40:O40"/>
-    <mergeCell ref="J33:K33"/>
-    <mergeCell ref="J36:K36"/>
-    <mergeCell ref="J37:K37"/>
-    <mergeCell ref="J38:K38"/>
-    <mergeCell ref="J39:K39"/>
-    <mergeCell ref="J40:K40"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="H40:I40"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="P19:Q19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="H18:Q18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="D18:G18"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="P22:Q22"/>
+    <mergeCell ref="P23:Q23"/>
+    <mergeCell ref="P24:Q24"/>
+    <mergeCell ref="P25:Q25"/>
+    <mergeCell ref="N33:O33"/>
+    <mergeCell ref="N36:O36"/>
+    <mergeCell ref="N37:O37"/>
+    <mergeCell ref="P37:Q37"/>
+    <mergeCell ref="P38:Q38"/>
+    <mergeCell ref="P39:Q39"/>
+    <mergeCell ref="P40:Q40"/>
+    <mergeCell ref="P26:Q26"/>
+    <mergeCell ref="P27:Q27"/>
+    <mergeCell ref="P28:Q28"/>
+    <mergeCell ref="P32:Q32"/>
+    <mergeCell ref="P33:Q33"/>
+    <mergeCell ref="P36:Q36"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D2:F3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="L31:M31"/>
+    <mergeCell ref="N31:O31"/>
+    <mergeCell ref="P31:Q31"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="N29:O29"/>
+    <mergeCell ref="P29:Q29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="N30:O30"/>
+    <mergeCell ref="P30:Q30"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="L34:M34"/>
+    <mergeCell ref="N34:O34"/>
+    <mergeCell ref="P34:Q34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="J35:K35"/>
+    <mergeCell ref="L35:M35"/>
+    <mergeCell ref="N35:O35"/>
+    <mergeCell ref="P35:Q35"/>
   </mergeCells>
   <phoneticPr fontId="22" type="noConversion"/>
   <dataValidations disablePrompts="1" count="1">
@@ -10574,13 +10585,13 @@
   <sheetPr codeName="Sheet5">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:F208"/>
+  <dimension ref="B1:F209"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B39" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E42" sqref="E42"/>
+      <selection pane="bottomRight" activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -10648,7 +10659,7 @@
         <v>29</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="F5" s="33"/>
     </row>
@@ -10744,11 +10755,11 @@
         <v>18</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>716</v>
+        <v>839</v>
       </c>
       <c r="F11" s="33"/>
     </row>
-    <row r="12" spans="2:6" ht="30" outlineLevel="1">
+    <row r="12" spans="2:6" ht="135" outlineLevel="1">
       <c r="B12" s="30" t="str">
         <f t="shared" si="0"/>
         <v>GF.009</v>
@@ -10757,10 +10768,10 @@
         <v>35</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>715</v>
+        <v>840</v>
       </c>
       <c r="F12" s="33"/>
     </row>
@@ -10792,7 +10803,7 @@
         <v>29</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>770</v>
+        <v>766</v>
       </c>
       <c r="F14" s="33">
         <v>9960</v>
@@ -10826,7 +10837,7 @@
         <v>29</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>771</v>
+        <v>767</v>
       </c>
       <c r="F16" s="33">
         <v>10160</v>
@@ -10860,7 +10871,7 @@
         <v>29</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>764</v>
+        <v>760</v>
       </c>
       <c r="F18" s="33"/>
     </row>
@@ -10876,7 +10887,7 @@
         <v>29</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="F19" s="33"/>
     </row>
@@ -10892,7 +10903,7 @@
         <v>21</v>
       </c>
       <c r="E20" s="21" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="F20" s="92"/>
     </row>
@@ -10908,7 +10919,7 @@
         <v>29</v>
       </c>
       <c r="E21" s="21" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="F21" s="92"/>
     </row>
@@ -10924,7 +10935,7 @@
         <v>29</v>
       </c>
       <c r="E22" s="21" t="s">
-        <v>834</v>
+        <v>830</v>
       </c>
       <c r="F22" s="92"/>
     </row>
@@ -10940,7 +10951,7 @@
         <v>29</v>
       </c>
       <c r="E23" s="21" t="s">
-        <v>838</v>
+        <v>834</v>
       </c>
       <c r="F23" s="92"/>
     </row>
@@ -10956,7 +10967,7 @@
         <v>29</v>
       </c>
       <c r="E24" s="21" t="s">
-        <v>837</v>
+        <v>833</v>
       </c>
       <c r="F24" s="92"/>
     </row>
@@ -11220,7 +11231,7 @@
         <v>29</v>
       </c>
       <c r="E41" s="23" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
       <c r="F41" s="32">
         <f t="shared" ref="F41:F46" si="2">WARNING_BASE + MID(E41, SEARCH("[",E41) + 1, SEARCH("]",E41) - SEARCH("[",E41) - 1)</f>
@@ -11239,7 +11250,7 @@
         <v>29</v>
       </c>
       <c r="E42" s="23" t="s">
-        <v>836</v>
+        <v>832</v>
       </c>
       <c r="F42" s="32">
         <f t="shared" si="2"/>
@@ -11277,7 +11288,7 @@
         <v>29</v>
       </c>
       <c r="E44" s="23" t="s">
-        <v>799</v>
+        <v>795</v>
       </c>
       <c r="F44" s="32">
         <f t="shared" si="2"/>
@@ -11469,7 +11480,7 @@
         <v>29</v>
       </c>
       <c r="E58" s="102" t="s">
-        <v>801</v>
+        <v>797</v>
       </c>
       <c r="F58" s="32"/>
     </row>
@@ -11485,7 +11496,7 @@
         <v>29</v>
       </c>
       <c r="E59" s="193" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
       <c r="F59" s="92"/>
     </row>
@@ -11501,7 +11512,7 @@
         <v>29</v>
       </c>
       <c r="E60" s="193" t="s">
-        <v>803</v>
+        <v>799</v>
       </c>
       <c r="F60" s="92"/>
     </row>
@@ -11517,7 +11528,7 @@
         <v>29</v>
       </c>
       <c r="E61" s="16" t="s">
-        <v>784</v>
+        <v>780</v>
       </c>
       <c r="F61" s="32"/>
     </row>
@@ -11533,7 +11544,7 @@
         <v>29</v>
       </c>
       <c r="E62" s="21" t="s">
-        <v>819</v>
+        <v>815</v>
       </c>
       <c r="F62" s="92"/>
     </row>
@@ -11565,7 +11576,7 @@
         <v>29</v>
       </c>
       <c r="E64" s="16" t="s">
-        <v>818</v>
+        <v>814</v>
       </c>
       <c r="F64" s="32"/>
     </row>
@@ -11581,7 +11592,7 @@
         <v>29</v>
       </c>
       <c r="E65" s="16" t="s">
-        <v>817</v>
+        <v>813</v>
       </c>
       <c r="F65" s="32"/>
     </row>
@@ -11597,7 +11608,7 @@
         <v>29</v>
       </c>
       <c r="E66" s="21" t="s">
-        <v>835</v>
+        <v>831</v>
       </c>
       <c r="F66" s="92"/>
     </row>
@@ -12089,7 +12100,7 @@
         <v>21</v>
       </c>
       <c r="E100" s="21" t="s">
-        <v>782</v>
+        <v>778</v>
       </c>
       <c r="F100" s="32"/>
     </row>
@@ -12105,7 +12116,7 @@
         <v>29</v>
       </c>
       <c r="E101" s="21" t="s">
-        <v>820</v>
+        <v>816</v>
       </c>
       <c r="F101" s="92"/>
     </row>
@@ -12121,7 +12132,7 @@
         <v>29</v>
       </c>
       <c r="E102" s="21" t="s">
-        <v>821</v>
+        <v>817</v>
       </c>
       <c r="F102" s="92"/>
     </row>
@@ -12137,7 +12148,7 @@
         <v>29</v>
       </c>
       <c r="E103" s="21" t="s">
-        <v>822</v>
+        <v>818</v>
       </c>
       <c r="F103" s="92"/>
     </row>
@@ -12153,7 +12164,7 @@
         <v>29</v>
       </c>
       <c r="E104" s="21" t="s">
-        <v>829</v>
+        <v>825</v>
       </c>
       <c r="F104" s="92"/>
     </row>
@@ -12166,7 +12177,7 @@
         <v>35</v>
       </c>
       <c r="D105" s="14" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="E105" s="21" t="s">
         <v>687</v>
@@ -12182,7 +12193,7 @@
         <v>35</v>
       </c>
       <c r="D106" s="20" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="E106" s="21" t="s">
         <v>653</v>
@@ -12233,10 +12244,10 @@
         <v>35</v>
       </c>
       <c r="D109" s="20" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="E109" s="193" t="s">
-        <v>688</v>
+        <v>837</v>
       </c>
       <c r="F109" s="32">
         <f t="shared" si="7"/>
@@ -12433,7 +12444,7 @@
         <v>21</v>
       </c>
       <c r="E122" s="21" t="s">
-        <v>781</v>
+        <v>777</v>
       </c>
       <c r="F122" s="32"/>
     </row>
@@ -12449,7 +12460,7 @@
         <v>29</v>
       </c>
       <c r="E123" s="21" t="s">
-        <v>805</v>
+        <v>801</v>
       </c>
       <c r="F123" s="32"/>
     </row>
@@ -12481,7 +12492,7 @@
         <v>29</v>
       </c>
       <c r="E125" s="193" t="s">
-        <v>806</v>
+        <v>802</v>
       </c>
       <c r="F125" s="32">
         <f t="shared" ref="F125" si="8">WARNING_BASE + MID(E125, SEARCH("[",E125) + 1, SEARCH("]",E125) - SEARCH("[",E125) - 1)</f>
@@ -12525,7 +12536,7 @@
         <v>15</v>
       </c>
       <c r="E129" s="16" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="F129" s="92"/>
     </row>
@@ -12541,7 +12552,7 @@
         <v>15</v>
       </c>
       <c r="E130" s="21" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="F130" s="92"/>
     </row>
@@ -12573,7 +12584,7 @@
         <v>21</v>
       </c>
       <c r="E132" s="21" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="F132" s="92"/>
     </row>
@@ -12589,7 +12600,7 @@
         <v>29</v>
       </c>
       <c r="E133" s="21" t="s">
-        <v>828</v>
+        <v>824</v>
       </c>
       <c r="F133" s="92"/>
     </row>
@@ -12605,7 +12616,7 @@
         <v>29</v>
       </c>
       <c r="E134" s="21" t="s">
-        <v>823</v>
+        <v>819</v>
       </c>
       <c r="F134" s="92"/>
     </row>
@@ -12621,7 +12632,7 @@
         <v>29</v>
       </c>
       <c r="E135" s="21" t="s">
-        <v>826</v>
+        <v>822</v>
       </c>
       <c r="F135" s="92"/>
     </row>
@@ -12637,7 +12648,7 @@
         <v>29</v>
       </c>
       <c r="E136" s="21" t="s">
-        <v>824</v>
+        <v>820</v>
       </c>
       <c r="F136" s="92"/>
     </row>
@@ -12653,7 +12664,7 @@
         <v>29</v>
       </c>
       <c r="E137" s="21" t="s">
-        <v>825</v>
+        <v>821</v>
       </c>
       <c r="F137" s="92"/>
     </row>
@@ -12669,7 +12680,7 @@
         <v>29</v>
       </c>
       <c r="E138" s="21" t="s">
-        <v>804</v>
+        <v>800</v>
       </c>
       <c r="F138" s="92"/>
     </row>
@@ -12685,7 +12696,7 @@
         <v>18</v>
       </c>
       <c r="E139" s="21" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="F139" s="92"/>
     </row>
@@ -12701,7 +12712,7 @@
         <v>18</v>
       </c>
       <c r="E140" s="21" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="F140" s="92"/>
     </row>
@@ -12717,7 +12728,7 @@
         <v>18</v>
       </c>
       <c r="E141" s="21" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="F141" s="92"/>
     </row>
@@ -12733,7 +12744,7 @@
         <v>15</v>
       </c>
       <c r="E142" s="21" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="F142" s="92"/>
     </row>
@@ -12749,7 +12760,7 @@
         <v>18</v>
       </c>
       <c r="E143" s="21" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="F143" s="92"/>
     </row>
@@ -12765,7 +12776,7 @@
         <v>18</v>
       </c>
       <c r="E144" s="21" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="F144" s="92"/>
     </row>
@@ -12781,7 +12792,7 @@
         <v>18</v>
       </c>
       <c r="E145" s="21" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="F145" s="92"/>
     </row>
@@ -12797,7 +12808,7 @@
         <v>18</v>
       </c>
       <c r="E146" s="16" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="F146" s="32">
         <f>ALARM_BASE + MID(E146, SEARCH("[",E146) + 1, SEARCH("]",E146) - SEARCH("[",E146) - 1)</f>
@@ -12829,10 +12840,10 @@
         <v>35</v>
       </c>
       <c r="D148" s="20" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="E148" s="21" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F148" s="92"/>
     </row>
@@ -12845,10 +12856,10 @@
         <v>35</v>
       </c>
       <c r="D149" s="20" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="E149" s="193" t="s">
-        <v>706</v>
+        <v>838</v>
       </c>
       <c r="F149" s="32">
         <f t="shared" ref="F149" si="10">WARNING_BASE + MID(E149, SEARCH("[",E149) + 1, SEARCH("]",E149) - SEARCH("[",E149) - 1)</f>
@@ -12899,7 +12910,7 @@
         <v>15</v>
       </c>
       <c r="E154" s="16" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="F154" s="92"/>
     </row>
@@ -12915,7 +12926,7 @@
         <v>15</v>
       </c>
       <c r="E155" s="21" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="F155" s="92"/>
     </row>
@@ -12979,7 +12990,7 @@
         <v>29</v>
       </c>
       <c r="E161" s="21" t="s">
-        <v>790</v>
+        <v>786</v>
       </c>
       <c r="F161" s="92"/>
     </row>
@@ -12995,7 +13006,7 @@
         <v>29</v>
       </c>
       <c r="E162" s="21" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
       <c r="F162" s="92"/>
     </row>
@@ -13027,7 +13038,7 @@
         <v>29</v>
       </c>
       <c r="E164" s="21" t="s">
-        <v>789</v>
+        <v>785</v>
       </c>
       <c r="F164" s="32">
         <f>ALARM_BASE + MID(E164, SEARCH("[",E164) + 1, SEARCH("]",E164) - SEARCH("[",E164) - 1)</f>
@@ -13062,7 +13073,7 @@
         <v>29</v>
       </c>
       <c r="E166" s="193" t="s">
-        <v>795</v>
+        <v>791</v>
       </c>
       <c r="F166" s="32">
         <f t="shared" ref="F166" si="12">WARNING_BASE + MID(E166, SEARCH("[",E166) + 1, SEARCH("]",E166) - SEARCH("[",E166) - 1)</f>
@@ -13122,7 +13133,7 @@
         <v>29</v>
       </c>
       <c r="E171" s="21" t="s">
-        <v>776</v>
+        <v>772</v>
       </c>
       <c r="F171" s="92"/>
     </row>
@@ -13154,7 +13165,7 @@
         <v>29</v>
       </c>
       <c r="E173" s="21" t="s">
-        <v>775</v>
+        <v>771</v>
       </c>
       <c r="F173" s="92"/>
     </row>
@@ -13185,7 +13196,7 @@
     </row>
     <row r="177" spans="2:6" ht="210" outlineLevel="1">
       <c r="B177" s="91" t="str">
-        <f t="shared" ref="B177:B191" si="13">_xlfn.CONCAT(UO_ID,".",TEXT(ROW()-ROW(UO_ID), "000"))</f>
+        <f t="shared" ref="B177:B192" si="13">_xlfn.CONCAT(UO_ID,".",TEXT(ROW()-ROW(UO_ID), "000"))</f>
         <v>UO.001</v>
       </c>
       <c r="C177" s="20" t="s">
@@ -13195,7 +13206,7 @@
         <v>29</v>
       </c>
       <c r="E177" s="21" t="s">
-        <v>792</v>
+        <v>788</v>
       </c>
       <c r="F177" s="92"/>
     </row>
@@ -13211,7 +13222,7 @@
         <v>29</v>
       </c>
       <c r="E178" s="21" t="s">
-        <v>765</v>
+        <v>761</v>
       </c>
       <c r="F178" s="92"/>
     </row>
@@ -13227,7 +13238,7 @@
         <v>29</v>
       </c>
       <c r="E179" s="21" t="s">
-        <v>794</v>
+        <v>790</v>
       </c>
       <c r="F179" s="92"/>
     </row>
@@ -13243,7 +13254,7 @@
         <v>29</v>
       </c>
       <c r="E180" s="21" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="F180" s="92"/>
     </row>
@@ -13259,7 +13270,7 @@
         <v>29</v>
       </c>
       <c r="E181" s="21" t="s">
-        <v>766</v>
+        <v>762</v>
       </c>
       <c r="F181" s="92"/>
     </row>
@@ -13275,7 +13286,7 @@
         <v>29</v>
       </c>
       <c r="E182" s="21" t="s">
-        <v>793</v>
+        <v>789</v>
       </c>
       <c r="F182" s="92"/>
     </row>
@@ -13291,7 +13302,7 @@
         <v>29</v>
       </c>
       <c r="E183" s="21" t="s">
-        <v>767</v>
+        <v>763</v>
       </c>
       <c r="F183" s="92"/>
     </row>
@@ -13307,7 +13318,7 @@
         <v>29</v>
       </c>
       <c r="E184" s="21" t="s">
-        <v>768</v>
+        <v>764</v>
       </c>
       <c r="F184" s="92"/>
     </row>
@@ -13323,7 +13334,7 @@
         <v>29</v>
       </c>
       <c r="E185" s="21" t="s">
-        <v>778</v>
+        <v>774</v>
       </c>
       <c r="F185" s="92"/>
     </row>
@@ -13339,14 +13350,14 @@
         <v>29</v>
       </c>
       <c r="E186" s="193" t="s">
-        <v>779</v>
+        <v>775</v>
       </c>
       <c r="F186" s="32">
-        <f t="shared" ref="F186" si="14">WARNING_BASE + MID(E186, SEARCH("[",E186) + 1, SEARCH("]",E186) - SEARCH("[",E186) - 1)</f>
+        <f t="shared" ref="F186:F187" si="14">WARNING_BASE + MID(E186, SEARCH("[",E186) + 1, SEARCH("]",E186) - SEARCH("[",E186) - 1)</f>
         <v>10060</v>
       </c>
     </row>
-    <row r="187" spans="2:6" outlineLevel="1">
+    <row r="187" spans="2:6" ht="75" outlineLevel="1">
       <c r="B187" s="91" t="str">
         <f t="shared" si="13"/>
         <v>UO.011</v>
@@ -13357,12 +13368,15 @@
       <c r="D187" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="E187" s="21" t="s">
-        <v>690</v>
-      </c>
-      <c r="F187" s="92"/>
-    </row>
-    <row r="188" spans="2:6" ht="45" outlineLevel="1">
+      <c r="E187" s="193" t="s">
+        <v>836</v>
+      </c>
+      <c r="F187" s="32">
+        <f t="shared" si="14"/>
+        <v>10061</v>
+      </c>
+    </row>
+    <row r="188" spans="2:6" outlineLevel="1">
       <c r="B188" s="91" t="str">
         <f t="shared" si="13"/>
         <v>UO.012</v>
@@ -13374,12 +13388,9 @@
         <v>29</v>
       </c>
       <c r="E188" s="21" t="s">
-        <v>788</v>
-      </c>
-      <c r="F188" s="32">
-        <f>ALARM_BASE + MID(E188, SEARCH("[",E188) + 1, SEARCH("]",E188) - SEARCH("[",E188) - 1)</f>
-        <v>10260</v>
-      </c>
+        <v>689</v>
+      </c>
+      <c r="F188" s="92"/>
     </row>
     <row r="189" spans="2:6" ht="45" outlineLevel="1">
       <c r="B189" s="91" t="str">
@@ -13393,11 +13404,11 @@
         <v>29</v>
       </c>
       <c r="E189" s="21" t="s">
-        <v>691</v>
+        <v>784</v>
       </c>
       <c r="F189" s="32">
         <f>ALARM_BASE + MID(E189, SEARCH("[",E189) + 1, SEARCH("]",E189) - SEARCH("[",E189) - 1)</f>
-        <v>10261</v>
+        <v>10260</v>
       </c>
     </row>
     <row r="190" spans="2:6" ht="45" outlineLevel="1">
@@ -13412,14 +13423,14 @@
         <v>29</v>
       </c>
       <c r="E190" s="21" t="s">
-        <v>814</v>
+        <v>690</v>
       </c>
       <c r="F190" s="32">
         <f>ALARM_BASE + MID(E190, SEARCH("[",E190) + 1, SEARCH("]",E190) - SEARCH("[",E190) - 1)</f>
-        <v>10262</v>
-      </c>
-    </row>
-    <row r="191" spans="2:6" ht="90" outlineLevel="1">
+        <v>10261</v>
+      </c>
+    </row>
+    <row r="191" spans="2:6" ht="45" outlineLevel="1">
       <c r="B191" s="91" t="str">
         <f t="shared" si="13"/>
         <v>UO.015</v>
@@ -13431,19 +13442,31 @@
         <v>29</v>
       </c>
       <c r="E191" s="21" t="s">
-        <v>815</v>
+        <v>810</v>
       </c>
       <c r="F191" s="32">
         <f>ALARM_BASE + MID(E191, SEARCH("[",E191) + 1, SEARCH("]",E191) - SEARCH("[",E191) - 1)</f>
+        <v>10262</v>
+      </c>
+    </row>
+    <row r="192" spans="2:6" ht="90" outlineLevel="1">
+      <c r="B192" s="91" t="str">
+        <f t="shared" si="13"/>
+        <v>UO.016</v>
+      </c>
+      <c r="C192" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D192" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="E192" s="21" t="s">
+        <v>811</v>
+      </c>
+      <c r="F192" s="32">
+        <f>ALARM_BASE + MID(E192, SEARCH("[",E192) + 1, SEARCH("]",E192) - SEARCH("[",E192) - 1)</f>
         <v>10263</v>
       </c>
-    </row>
-    <row r="192" spans="2:6" outlineLevel="1">
-      <c r="B192" s="91"/>
-      <c r="C192" s="20"/>
-      <c r="D192" s="20"/>
-      <c r="E192" s="21"/>
-      <c r="F192" s="92"/>
     </row>
     <row r="193" spans="2:6" outlineLevel="1">
       <c r="B193" s="91"/>
@@ -13452,29 +13475,29 @@
       <c r="E193" s="21"/>
       <c r="F193" s="92"/>
     </row>
-    <row r="194" spans="2:6">
-      <c r="B194" s="18" t="s">
+    <row r="194" spans="2:6" outlineLevel="1">
+      <c r="B194" s="91"/>
+      <c r="C194" s="20"/>
+      <c r="D194" s="20"/>
+      <c r="E194" s="21"/>
+      <c r="F194" s="92"/>
+    </row>
+    <row r="195" spans="2:6">
+      <c r="B195" s="18" t="s">
         <v>201</v>
       </c>
-      <c r="C194" s="19"/>
-      <c r="D194" s="19"/>
-      <c r="E194" s="96" t="s">
+      <c r="C195" s="19"/>
+      <c r="D195" s="19"/>
+      <c r="E195" s="96" t="s">
         <v>202</v>
       </c>
-      <c r="F194" s="97"/>
-    </row>
-    <row r="195" spans="2:6" outlineLevel="1">
-      <c r="B195" s="91" t="str">
+      <c r="F195" s="97"/>
+    </row>
+    <row r="196" spans="2:6" outlineLevel="1">
+      <c r="B196" s="91" t="str">
         <f>_xlfn.CONCAT(GP_ID,".",TEXT(ROW()-ROW(GP_ID), "000"))</f>
         <v>GP.001</v>
       </c>
-      <c r="C195" s="20"/>
-      <c r="D195" s="20"/>
-      <c r="E195" s="21"/>
-      <c r="F195" s="92"/>
-    </row>
-    <row r="196" spans="2:6" outlineLevel="1">
-      <c r="B196" s="91"/>
       <c r="C196" s="20"/>
       <c r="D196" s="20"/>
       <c r="E196" s="21"/>
@@ -13501,19 +13524,19 @@
       <c r="E199" s="21"/>
       <c r="F199" s="92"/>
     </row>
-    <row r="200" spans="2:6">
-      <c r="B200" s="189"/>
-      <c r="C200" s="190"/>
-      <c r="D200" s="190"/>
-      <c r="E200" s="191"/>
-      <c r="F200" s="192"/>
-    </row>
-    <row r="201" spans="2:6" outlineLevel="1">
-      <c r="B201" s="91"/>
-      <c r="C201" s="20"/>
-      <c r="D201" s="20"/>
-      <c r="E201" s="21"/>
-      <c r="F201" s="92"/>
+    <row r="200" spans="2:6" outlineLevel="1">
+      <c r="B200" s="91"/>
+      <c r="C200" s="20"/>
+      <c r="D200" s="20"/>
+      <c r="E200" s="21"/>
+      <c r="F200" s="92"/>
+    </row>
+    <row r="201" spans="2:6">
+      <c r="B201" s="189"/>
+      <c r="C201" s="190"/>
+      <c r="D201" s="190"/>
+      <c r="E201" s="191"/>
+      <c r="F201" s="192"/>
     </row>
     <row r="202" spans="2:6" outlineLevel="1">
       <c r="B202" s="91"/>
@@ -13550,357 +13573,364 @@
       <c r="E206" s="21"/>
       <c r="F206" s="92"/>
     </row>
-    <row r="207" spans="2:6">
-      <c r="B207" s="228" t="s">
+    <row r="207" spans="2:6" outlineLevel="1">
+      <c r="B207" s="91"/>
+      <c r="C207" s="20"/>
+      <c r="D207" s="20"/>
+      <c r="E207" s="21"/>
+      <c r="F207" s="92"/>
+    </row>
+    <row r="208" spans="2:6">
+      <c r="B208" s="228" t="s">
         <v>106</v>
       </c>
-      <c r="C207" s="228"/>
-      <c r="D207" s="228"/>
-      <c r="E207" s="228"/>
-      <c r="F207" s="228"/>
-    </row>
-    <row r="208" spans="2:6">
-      <c r="B208" s="22"/>
-      <c r="C208" s="22"/>
-      <c r="D208" s="22"/>
-      <c r="E208" s="22"/>
-      <c r="F208" s="22"/>
+      <c r="C208" s="228"/>
+      <c r="D208" s="228"/>
+      <c r="E208" s="228"/>
+      <c r="F208" s="228"/>
+    </row>
+    <row r="209" spans="2:6">
+      <c r="B209" s="22"/>
+      <c r="C209" s="22"/>
+      <c r="D209" s="22"/>
+      <c r="E209" s="22"/>
+      <c r="F209" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B207:F207"/>
+    <mergeCell ref="B208:F208"/>
   </mergeCells>
   <phoneticPr fontId="22" type="noConversion"/>
-  <conditionalFormatting sqref="E195:E199 E170:E175 E201:E206 E2:E16 E92:E119 E122:E127 E160:E168 E154:E158 E177:E193 E18:E86 E129:E152">
-    <cfRule type="expression" dxfId="129" priority="93">
+  <conditionalFormatting sqref="E196:E200 E170:E175 E202:E207 E2:E16 E92:E119 E122:E127 E160:E168 E154:E158 E177:E194 E18:E86 E129:E152">
+    <cfRule type="expression" dxfId="97" priority="93">
       <formula>$C2="Nice to have"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="128" priority="98">
+    <cfRule type="expression" dxfId="96" priority="98">
       <formula>$C2="Deprecated"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D195:D199 D170:D175 D201:D206 D122:D127 D3:D16 D92:D119 D160:D168 D154:D158 D177:D193 D18:D86 D129:D152">
-    <cfRule type="cellIs" dxfId="127" priority="92" operator="equal">
+  <conditionalFormatting sqref="D196:D200 D170:D175 D202:D207 D122:D127 D3:D16 D92:D119 D160:D168 D154:D158 D177:D194 D18:D86 D129:D152">
+    <cfRule type="cellIs" dxfId="95" priority="92" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="126" priority="94" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="94" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="125" priority="95" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="95" operator="equal">
       <formula>"Approved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="124" priority="96" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="96" operator="equal">
       <formula>"On Hold"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="123" priority="97" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="97" operator="equal">
       <formula>"Pending Approval"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E128">
-    <cfRule type="expression" dxfId="122" priority="86">
+    <cfRule type="expression" dxfId="90" priority="86">
       <formula>$C128="Nice to have"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="121" priority="91">
+    <cfRule type="expression" dxfId="89" priority="91">
       <formula>$C128="Deprecated"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D128">
-    <cfRule type="cellIs" dxfId="120" priority="85" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="85" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="119" priority="87" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="87" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="118" priority="88" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="88" operator="equal">
       <formula>"Approved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="117" priority="89" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="89" operator="equal">
       <formula>"On Hold"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="116" priority="90" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="90" operator="equal">
       <formula>"Pending Approval"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E153">
-    <cfRule type="expression" dxfId="115" priority="79">
+    <cfRule type="expression" dxfId="83" priority="79">
       <formula>$C153="Nice to have"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="114" priority="84">
+    <cfRule type="expression" dxfId="82" priority="84">
       <formula>$C153="Deprecated"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D153">
-    <cfRule type="cellIs" dxfId="113" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="78" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="112" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="80" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="111" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="81" operator="equal">
       <formula>"Approved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="110" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="82" operator="equal">
       <formula>"On Hold"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="109" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="83" operator="equal">
       <formula>"Pending Approval"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E159">
-    <cfRule type="expression" dxfId="108" priority="72">
+    <cfRule type="expression" dxfId="76" priority="72">
       <formula>$C159="Nice to have"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="107" priority="77">
+    <cfRule type="expression" dxfId="75" priority="77">
       <formula>$C159="Deprecated"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D159">
-    <cfRule type="cellIs" dxfId="106" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="71" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="105" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="73" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="104" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="74" operator="equal">
       <formula>"Approved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="103" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="75" operator="equal">
       <formula>"On Hold"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="102" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="76" operator="equal">
       <formula>"Pending Approval"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E176">
-    <cfRule type="expression" dxfId="101" priority="65">
+    <cfRule type="expression" dxfId="69" priority="65">
       <formula>$C176="Nice to have"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="100" priority="70">
+    <cfRule type="expression" dxfId="68" priority="70">
       <formula>$C176="Deprecated"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D176">
-    <cfRule type="cellIs" dxfId="99" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="64" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="98" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="66" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="97" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="67" operator="equal">
       <formula>"Approved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="68" operator="equal">
       <formula>"On Hold"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="95" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="69" operator="equal">
       <formula>"Pending Approval"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E194">
-    <cfRule type="expression" dxfId="94" priority="58">
-      <formula>$C194="Nice to have"</formula>
+  <conditionalFormatting sqref="E195">
+    <cfRule type="expression" dxfId="62" priority="58">
+      <formula>$C195="Nice to have"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="93" priority="63">
-      <formula>$C194="Deprecated"</formula>
+    <cfRule type="expression" dxfId="61" priority="63">
+      <formula>$C195="Deprecated"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D194">
-    <cfRule type="cellIs" dxfId="92" priority="57" operator="equal">
+  <conditionalFormatting sqref="D195">
+    <cfRule type="cellIs" dxfId="60" priority="57" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="91" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="59" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="60" operator="equal">
       <formula>"Approved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="89" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="61" operator="equal">
       <formula>"On Hold"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="62" operator="equal">
       <formula>"Pending Approval"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E200">
-    <cfRule type="expression" dxfId="87" priority="51">
-      <formula>$C200="Nice to have"</formula>
+  <conditionalFormatting sqref="E201">
+    <cfRule type="expression" dxfId="55" priority="51">
+      <formula>$C201="Nice to have"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="86" priority="56">
-      <formula>$C200="Deprecated"</formula>
+    <cfRule type="expression" dxfId="54" priority="56">
+      <formula>$C201="Deprecated"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D200">
-    <cfRule type="cellIs" dxfId="85" priority="50" operator="equal">
+  <conditionalFormatting sqref="D201">
+    <cfRule type="cellIs" dxfId="53" priority="50" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="52" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="83" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="53" operator="equal">
       <formula>"Approved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="54" operator="equal">
       <formula>"On Hold"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="55" operator="equal">
       <formula>"Pending Approval"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E169">
-    <cfRule type="expression" dxfId="80" priority="37">
+    <cfRule type="expression" dxfId="48" priority="37">
       <formula>$C169="Nice to have"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="79" priority="42">
+    <cfRule type="expression" dxfId="47" priority="42">
       <formula>$C169="Deprecated"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D169">
-    <cfRule type="cellIs" dxfId="78" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="36" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="38" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="39" operator="equal">
       <formula>"Approved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="40" operator="equal">
       <formula>"On Hold"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="41" operator="equal">
       <formula>"Pending Approval"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E120">
-    <cfRule type="expression" dxfId="73" priority="30">
+    <cfRule type="expression" dxfId="41" priority="30">
       <formula>$C120="Nice to have"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="35">
+    <cfRule type="expression" dxfId="40" priority="35">
       <formula>$C120="Deprecated"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D120">
-    <cfRule type="cellIs" dxfId="71" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="29" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="31" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="32" operator="equal">
       <formula>"Approved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="33" operator="equal">
       <formula>"On Hold"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="34" operator="equal">
       <formula>"Pending Approval"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E121">
-    <cfRule type="expression" dxfId="66" priority="23">
+    <cfRule type="expression" dxfId="34" priority="23">
       <formula>$C121="Nice to have"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="65" priority="28">
+    <cfRule type="expression" dxfId="33" priority="28">
       <formula>$C121="Deprecated"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D121">
-    <cfRule type="cellIs" dxfId="64" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="22" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="24" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="25" operator="equal">
       <formula>"Approved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="26" operator="equal">
       <formula>"On Hold"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="27" operator="equal">
       <formula>"Pending Approval"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E88:E91">
-    <cfRule type="expression" dxfId="59" priority="16">
+    <cfRule type="expression" dxfId="27" priority="16">
       <formula>$C88="Nice to have"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="21">
+    <cfRule type="expression" dxfId="26" priority="21">
       <formula>$C88="Deprecated"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D88:D91">
-    <cfRule type="cellIs" dxfId="57" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="15" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="17" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="18" operator="equal">
       <formula>"Approved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="19" operator="equal">
       <formula>"On Hold"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="20" operator="equal">
       <formula>"Pending Approval"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E87">
-    <cfRule type="expression" dxfId="52" priority="9">
+    <cfRule type="expression" dxfId="20" priority="9">
       <formula>$C87="Nice to have"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="14">
+    <cfRule type="expression" dxfId="19" priority="14">
       <formula>$C87="Deprecated"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D87">
-    <cfRule type="cellIs" dxfId="50" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="8" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="10" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="11" operator="equal">
       <formula>"Approved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="12" operator="equal">
       <formula>"On Hold"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
       <formula>"Pending Approval"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E17">
-    <cfRule type="expression" dxfId="45" priority="2">
+    <cfRule type="expression" dxfId="13" priority="2">
       <formula>$C17="Nice to have"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="7">
+    <cfRule type="expression" dxfId="12" priority="7">
       <formula>$C17="Deprecated"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D17">
-    <cfRule type="cellIs" dxfId="43" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
       <formula>"Approved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
       <formula>"On Hold"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
       <formula>"Pending Approval"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C206" xr:uid="{00000000-0002-0000-0400-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C207" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <formula1>settings.level</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D206" xr:uid="{00000000-0002-0000-0400-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D207" xr:uid="{00000000-0002-0000-0400-000001000000}">
       <formula1>settings.status</formula1>
     </dataValidation>
   </dataValidations>
@@ -13985,7 +14015,7 @@
       </c>
       <c r="E3" s="136">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F3" s="138"/>
       <c r="G3" s="141"/>
@@ -14036,7 +14066,7 @@
       </c>
       <c r="E5" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F5" s="168" t="s">
         <v>220</v>
@@ -14058,14 +14088,14 @@
         <v>218</v>
       </c>
       <c r="C6" s="169" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="D6" s="170">
         <v>44256</v>
       </c>
       <c r="E6" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F6" s="168" t="s">
         <v>221</v>
@@ -14090,7 +14120,7 @@
       </c>
       <c r="E7" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F7" s="168" t="s">
         <v>262</v>
@@ -14117,7 +14147,7 @@
       </c>
       <c r="E8" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F8" s="168" t="s">
         <v>262</v>
@@ -14142,7 +14172,7 @@
       </c>
       <c r="E9" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F9" s="175" t="s">
         <v>221</v>
@@ -14186,17 +14216,17 @@
     </row>
     <row r="11" spans="2:11" ht="30" outlineLevel="1">
       <c r="B11" s="168" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
       <c r="C11" s="169" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
       <c r="D11" s="174">
         <v>44256</v>
       </c>
       <c r="E11" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F11" s="175" t="s">
         <v>220</v>
@@ -14207,7 +14237,7 @@
       </c>
       <c r="I11" s="168"/>
       <c r="J11" s="169" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
       <c r="K11" s="173"/>
     </row>
@@ -14268,7 +14298,7 @@
       </c>
       <c r="E15" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F15" s="145"/>
       <c r="G15" s="148"/>
@@ -14292,7 +14322,7 @@
       </c>
       <c r="E16" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F16" s="162" t="s">
         <v>220</v>
@@ -14307,7 +14337,7 @@
         <v>307</v>
       </c>
       <c r="K16" s="167" t="s">
-        <v>777</v>
+        <v>773</v>
       </c>
     </row>
     <row r="17" spans="2:11" outlineLevel="1">
@@ -14322,7 +14352,7 @@
       </c>
       <c r="E17" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F17" s="162" t="s">
         <v>220</v>
@@ -14334,7 +14364,7 @@
       <c r="I17" s="162"/>
       <c r="J17" s="163"/>
       <c r="K17" s="167" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
     </row>
     <row r="18" spans="2:11" outlineLevel="1">
@@ -14342,14 +14372,14 @@
         <v>227</v>
       </c>
       <c r="C18" s="163" t="s">
-        <v>758</v>
+        <v>754</v>
       </c>
       <c r="D18" s="202">
         <v>44287</v>
       </c>
       <c r="E18" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F18" s="203"/>
       <c r="G18" s="165"/>
@@ -14359,12 +14389,12 @@
       <c r="I18" s="162"/>
       <c r="J18" s="163"/>
       <c r="K18" s="167" t="s">
-        <v>809</v>
+        <v>805</v>
       </c>
     </row>
     <row r="19" spans="2:11" outlineLevel="1">
       <c r="B19" s="162" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
       <c r="C19" s="163" t="s">
         <v>228</v>
@@ -14374,7 +14404,7 @@
       </c>
       <c r="E19" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F19" s="162" t="s">
         <v>262</v>
@@ -14388,7 +14418,7 @@
       <c r="I19" s="162"/>
       <c r="J19" s="163"/>
       <c r="K19" s="167" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
     </row>
     <row r="20" spans="2:11" outlineLevel="1">
@@ -14433,7 +14463,7 @@
       </c>
       <c r="E22" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F22" s="145"/>
       <c r="G22" s="148"/>
@@ -14467,7 +14497,7 @@
       <c r="I23" s="155"/>
       <c r="J23" s="158"/>
       <c r="K23" s="161" t="s">
-        <v>808</v>
+        <v>804</v>
       </c>
     </row>
     <row r="24" spans="2:11" ht="150" outlineLevel="1">
@@ -14482,7 +14512,7 @@
       </c>
       <c r="E24" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F24" s="155"/>
       <c r="G24" s="159"/>
@@ -14492,7 +14522,7 @@
       <c r="I24" s="155"/>
       <c r="J24" s="158"/>
       <c r="K24" s="161" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
     </row>
     <row r="25" spans="2:11" ht="30" outlineLevel="1">
@@ -14500,14 +14530,14 @@
         <v>255</v>
       </c>
       <c r="C25" s="156" t="s">
-        <v>717</v>
+        <v>713</v>
       </c>
       <c r="D25" s="157">
         <v>44256</v>
       </c>
       <c r="E25" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F25" s="155" t="s">
         <v>221</v>
@@ -14519,7 +14549,7 @@
       <c r="I25" s="155"/>
       <c r="J25" s="158"/>
       <c r="K25" s="161" t="s">
-        <v>830</v>
+        <v>826</v>
       </c>
     </row>
     <row r="26" spans="2:11" ht="60" outlineLevel="1">
@@ -14527,14 +14557,14 @@
         <v>257</v>
       </c>
       <c r="C26" s="156" t="s">
-        <v>772</v>
+        <v>768</v>
       </c>
       <c r="D26" s="176">
         <v>44256</v>
       </c>
       <c r="E26" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F26" s="177" t="s">
         <v>220</v>
@@ -14546,7 +14576,7 @@
       <c r="I26" s="155"/>
       <c r="J26" s="158"/>
       <c r="K26" s="161" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
     </row>
     <row r="27" spans="2:11" ht="30" outlineLevel="1">
@@ -14554,14 +14584,14 @@
         <v>258</v>
       </c>
       <c r="C27" s="156" t="s">
-        <v>753</v>
+        <v>749</v>
       </c>
       <c r="D27" s="176">
         <v>44262</v>
       </c>
       <c r="E27" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F27" s="177" t="s">
         <v>220</v>
@@ -14573,7 +14603,7 @@
       <c r="I27" s="155"/>
       <c r="J27" s="158"/>
       <c r="K27" s="161" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
     </row>
     <row r="28" spans="2:11" ht="30" outlineLevel="1">
@@ -14581,14 +14611,14 @@
         <v>326</v>
       </c>
       <c r="C28" s="156" t="s">
-        <v>754</v>
+        <v>750</v>
       </c>
       <c r="D28" s="176">
         <v>44270</v>
       </c>
       <c r="E28" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F28" s="177" t="s">
         <v>220</v>
@@ -14600,7 +14630,7 @@
       <c r="I28" s="155"/>
       <c r="J28" s="158"/>
       <c r="K28" s="161" t="s">
-        <v>756</v>
+        <v>752</v>
       </c>
     </row>
     <row r="29" spans="2:11" ht="60" outlineLevel="1">
@@ -14608,7 +14638,7 @@
         <v>327</v>
       </c>
       <c r="C29" s="156" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="D29" s="176">
         <v>44237</v>
@@ -14625,7 +14655,7 @@
       <c r="I29" s="155"/>
       <c r="J29" s="158"/>
       <c r="K29" s="161" t="s">
-        <v>763</v>
+        <v>759</v>
       </c>
     </row>
     <row r="30" spans="2:11" ht="135" outlineLevel="1">
@@ -14640,7 +14670,7 @@
       </c>
       <c r="E30" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F30" s="155"/>
       <c r="G30" s="159"/>
@@ -14650,7 +14680,7 @@
       <c r="I30" s="155"/>
       <c r="J30" s="158"/>
       <c r="K30" s="161" t="s">
-        <v>831</v>
+        <v>827</v>
       </c>
     </row>
     <row r="31" spans="2:11" ht="75" outlineLevel="1">
@@ -14658,14 +14688,14 @@
         <v>332</v>
       </c>
       <c r="C31" s="156" t="s">
-        <v>783</v>
+        <v>779</v>
       </c>
       <c r="D31" s="157">
         <v>44280</v>
       </c>
       <c r="E31" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F31" s="155"/>
       <c r="G31" s="159"/>
@@ -14675,7 +14705,7 @@
       <c r="I31" s="155"/>
       <c r="J31" s="158"/>
       <c r="K31" s="161" t="s">
-        <v>832</v>
+        <v>828</v>
       </c>
     </row>
     <row r="32" spans="2:11" ht="30" outlineLevel="1">
@@ -14690,7 +14720,7 @@
       </c>
       <c r="E32" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F32" s="177"/>
       <c r="G32" s="159"/>
@@ -14700,7 +14730,7 @@
       <c r="I32" s="155"/>
       <c r="J32" s="158"/>
       <c r="K32" s="161" t="s">
-        <v>774</v>
+        <v>770</v>
       </c>
     </row>
     <row r="33" spans="2:11" outlineLevel="1">
@@ -14708,14 +14738,14 @@
         <v>334</v>
       </c>
       <c r="C33" s="156" t="s">
-        <v>797</v>
+        <v>793</v>
       </c>
       <c r="D33" s="176">
         <v>44256</v>
       </c>
       <c r="E33" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F33" s="177"/>
       <c r="G33" s="159"/>
@@ -14725,7 +14755,7 @@
       <c r="I33" s="155"/>
       <c r="J33" s="158"/>
       <c r="K33" s="161" t="s">
-        <v>798</v>
+        <v>794</v>
       </c>
     </row>
     <row r="34" spans="2:11" outlineLevel="1">
@@ -14733,14 +14763,14 @@
         <v>336</v>
       </c>
       <c r="C34" s="156" t="s">
-        <v>786</v>
+        <v>782</v>
       </c>
       <c r="D34" s="176">
         <v>44256</v>
       </c>
       <c r="E34" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F34" s="177"/>
       <c r="G34" s="159"/>
@@ -14750,7 +14780,7 @@
       <c r="I34" s="155"/>
       <c r="J34" s="158"/>
       <c r="K34" s="161" t="s">
-        <v>787</v>
+        <v>783</v>
       </c>
     </row>
     <row r="35" spans="2:11" outlineLevel="1">
@@ -14765,7 +14795,7 @@
       </c>
       <c r="E35" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F35" s="155"/>
       <c r="G35" s="159"/>
@@ -14775,12 +14805,12 @@
       <c r="I35" s="155"/>
       <c r="J35" s="158"/>
       <c r="K35" s="161" t="s">
-        <v>780</v>
+        <v>776</v>
       </c>
     </row>
     <row r="36" spans="2:11" outlineLevel="1">
       <c r="B36" s="155" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="C36" s="156" t="s">
         <v>329</v>
@@ -14790,7 +14820,7 @@
       </c>
       <c r="E36" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F36" s="155"/>
       <c r="G36" s="159"/>
@@ -14800,12 +14830,12 @@
       <c r="I36" s="155"/>
       <c r="J36" s="158"/>
       <c r="K36" s="161" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
     </row>
     <row r="37" spans="2:11" ht="30" outlineLevel="1">
       <c r="B37" s="155" t="s">
-        <v>796</v>
+        <v>792</v>
       </c>
       <c r="C37" s="156" t="s">
         <v>330</v>
@@ -14815,7 +14845,7 @@
       </c>
       <c r="E37" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F37" s="155"/>
       <c r="G37" s="159"/>
@@ -14825,22 +14855,22 @@
       <c r="I37" s="155"/>
       <c r="J37" s="158"/>
       <c r="K37" s="161" t="s">
-        <v>811</v>
+        <v>807</v>
       </c>
     </row>
     <row r="38" spans="2:11" outlineLevel="1">
       <c r="B38" s="155" t="s">
-        <v>785</v>
+        <v>781</v>
       </c>
       <c r="C38" s="156" t="s">
-        <v>813</v>
+        <v>809</v>
       </c>
       <c r="D38" s="157">
         <v>44329</v>
       </c>
       <c r="E38" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F38" s="155"/>
       <c r="G38" s="159"/>
@@ -14850,12 +14880,12 @@
       <c r="I38" s="155"/>
       <c r="J38" s="158"/>
       <c r="K38" s="161" t="s">
-        <v>812</v>
+        <v>808</v>
       </c>
     </row>
     <row r="39" spans="2:11" outlineLevel="1">
       <c r="B39" s="155" t="s">
-        <v>827</v>
+        <v>823</v>
       </c>
       <c r="C39" s="156" t="s">
         <v>229</v>
@@ -14865,7 +14895,7 @@
       </c>
       <c r="E39" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F39" s="155"/>
       <c r="G39" s="159">
@@ -14903,7 +14933,7 @@
       </c>
       <c r="E41" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F41" s="155"/>
       <c r="G41" s="159">
@@ -14948,17 +14978,17 @@
     </row>
     <row r="44" spans="2:11">
       <c r="B44" s="145" t="s">
-        <v>723</v>
+        <v>719</v>
       </c>
       <c r="C44" s="146" t="s">
-        <v>726</v>
+        <v>722</v>
       </c>
       <c r="D44" s="147">
         <v>44378</v>
       </c>
       <c r="E44" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F44" s="145"/>
       <c r="G44" s="148"/>
@@ -14972,17 +15002,17 @@
     </row>
     <row r="45" spans="2:11" ht="45" outlineLevel="1">
       <c r="B45" s="194" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="C45" s="195" t="s">
-        <v>722</v>
+        <v>718</v>
       </c>
       <c r="D45" s="196">
         <v>44287</v>
       </c>
       <c r="E45" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F45" s="194"/>
       <c r="G45" s="197"/>
@@ -14992,22 +15022,22 @@
       <c r="I45" s="194"/>
       <c r="J45" s="195"/>
       <c r="K45" s="199" t="s">
-        <v>762</v>
+        <v>758</v>
       </c>
     </row>
     <row r="46" spans="2:11" ht="45" outlineLevel="1">
       <c r="B46" s="194" t="s">
-        <v>725</v>
+        <v>721</v>
       </c>
       <c r="C46" s="195" t="s">
-        <v>727</v>
+        <v>723</v>
       </c>
       <c r="D46" s="196">
         <v>44287</v>
       </c>
       <c r="E46" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F46" s="194"/>
       <c r="G46" s="197"/>
@@ -15017,22 +15047,22 @@
       <c r="I46" s="194"/>
       <c r="J46" s="195"/>
       <c r="K46" s="199" t="s">
-        <v>740</v>
+        <v>736</v>
       </c>
     </row>
     <row r="47" spans="2:11" ht="45" outlineLevel="1">
       <c r="B47" s="194" t="s">
-        <v>728</v>
+        <v>724</v>
       </c>
       <c r="C47" s="195" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="D47" s="196">
         <v>44287</v>
       </c>
       <c r="E47" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F47" s="201"/>
       <c r="G47" s="197"/>
@@ -15042,22 +15072,22 @@
       <c r="I47" s="194"/>
       <c r="J47" s="195"/>
       <c r="K47" s="199" t="s">
-        <v>740</v>
+        <v>736</v>
       </c>
     </row>
     <row r="48" spans="2:11" ht="45" outlineLevel="1">
       <c r="B48" s="194" t="s">
-        <v>730</v>
+        <v>726</v>
       </c>
       <c r="C48" s="195" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
       <c r="D48" s="196">
         <v>44287</v>
       </c>
       <c r="E48" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F48" s="201" t="s">
         <v>220</v>
@@ -15069,22 +15099,22 @@
       <c r="I48" s="194"/>
       <c r="J48" s="195"/>
       <c r="K48" s="199" t="s">
-        <v>740</v>
+        <v>736</v>
       </c>
     </row>
     <row r="49" spans="2:11" ht="60" outlineLevel="1">
       <c r="B49" s="194" t="s">
-        <v>732</v>
+        <v>728</v>
       </c>
       <c r="C49" s="195" t="s">
-        <v>733</v>
+        <v>729</v>
       </c>
       <c r="D49" s="196">
         <v>44287</v>
       </c>
       <c r="E49" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F49" s="201"/>
       <c r="G49" s="197"/>
@@ -15094,22 +15124,22 @@
       <c r="I49" s="194"/>
       <c r="J49" s="195"/>
       <c r="K49" s="199" t="s">
-        <v>761</v>
+        <v>757</v>
       </c>
     </row>
     <row r="50" spans="2:11" ht="60" outlineLevel="1">
       <c r="B50" s="194" t="s">
-        <v>734</v>
+        <v>730</v>
       </c>
       <c r="C50" s="195" t="s">
-        <v>731</v>
+        <v>727</v>
       </c>
       <c r="D50" s="196">
         <v>44287</v>
       </c>
       <c r="E50" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F50" s="201"/>
       <c r="G50" s="197"/>
@@ -15119,22 +15149,22 @@
       <c r="I50" s="194"/>
       <c r="J50" s="195"/>
       <c r="K50" s="199" t="s">
-        <v>741</v>
+        <v>737</v>
       </c>
     </row>
     <row r="51" spans="2:11" ht="60" outlineLevel="1">
       <c r="B51" s="194" t="s">
-        <v>736</v>
+        <v>732</v>
       </c>
       <c r="C51" s="195" t="s">
-        <v>742</v>
+        <v>738</v>
       </c>
       <c r="D51" s="196">
         <v>44287</v>
       </c>
       <c r="E51" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F51" s="201" t="s">
         <v>220</v>
@@ -15146,22 +15176,22 @@
       <c r="I51" s="194"/>
       <c r="J51" s="195"/>
       <c r="K51" s="199" t="s">
-        <v>741</v>
+        <v>737</v>
       </c>
     </row>
     <row r="52" spans="2:11" ht="45" outlineLevel="1">
       <c r="B52" s="194" t="s">
-        <v>738</v>
+        <v>734</v>
       </c>
       <c r="C52" s="195" t="s">
-        <v>735</v>
+        <v>731</v>
       </c>
       <c r="D52" s="196">
         <v>44287</v>
       </c>
       <c r="E52" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F52" s="194"/>
       <c r="G52" s="197"/>
@@ -15171,22 +15201,22 @@
       <c r="I52" s="194"/>
       <c r="J52" s="195"/>
       <c r="K52" s="199" t="s">
-        <v>748</v>
+        <v>744</v>
       </c>
     </row>
     <row r="53" spans="2:11" ht="30" outlineLevel="1">
       <c r="B53" s="194" t="s">
-        <v>743</v>
+        <v>739</v>
       </c>
       <c r="C53" s="195" t="s">
-        <v>746</v>
+        <v>742</v>
       </c>
       <c r="D53" s="196">
         <v>44287</v>
       </c>
       <c r="E53" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F53" s="201"/>
       <c r="G53" s="197"/>
@@ -15196,22 +15226,22 @@
       <c r="I53" s="194"/>
       <c r="J53" s="195"/>
       <c r="K53" s="199" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
     </row>
     <row r="54" spans="2:11" outlineLevel="1">
       <c r="B54" s="194" t="s">
-        <v>744</v>
+        <v>740</v>
       </c>
       <c r="C54" s="195" t="s">
-        <v>747</v>
+        <v>743</v>
       </c>
       <c r="D54" s="196">
         <v>44287</v>
       </c>
       <c r="E54" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F54" s="201"/>
       <c r="G54" s="197"/>
@@ -15221,22 +15251,22 @@
       <c r="I54" s="194"/>
       <c r="J54" s="195"/>
       <c r="K54" s="199" t="s">
-        <v>750</v>
+        <v>746</v>
       </c>
     </row>
     <row r="55" spans="2:11" outlineLevel="1">
       <c r="B55" s="194" t="s">
-        <v>745</v>
+        <v>741</v>
       </c>
       <c r="C55" s="195" t="s">
-        <v>737</v>
+        <v>733</v>
       </c>
       <c r="D55" s="196">
         <v>44287</v>
       </c>
       <c r="E55" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F55" s="201" t="s">
         <v>220</v>
@@ -15248,22 +15278,22 @@
       <c r="I55" s="194"/>
       <c r="J55" s="195"/>
       <c r="K55" s="199" t="s">
-        <v>750</v>
+        <v>746</v>
       </c>
     </row>
     <row r="56" spans="2:11" outlineLevel="1">
       <c r="B56" s="194" t="s">
-        <v>751</v>
+        <v>747</v>
       </c>
       <c r="C56" s="195" t="s">
-        <v>739</v>
+        <v>735</v>
       </c>
       <c r="D56" s="196">
         <v>44287</v>
       </c>
       <c r="E56" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F56" s="201" t="s">
         <v>220</v>
@@ -15275,7 +15305,7 @@
       <c r="I56" s="194"/>
       <c r="J56" s="195"/>
       <c r="K56" s="199" t="s">
-        <v>750</v>
+        <v>746</v>
       </c>
     </row>
     <row r="57" spans="2:11" outlineLevel="1">
@@ -15756,17 +15786,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C86">
-    <cfRule type="expression" dxfId="31" priority="4">
+    <cfRule type="expression" dxfId="6" priority="4">
       <formula>AND($E3&lt;5,$H3&lt;&gt;1,NOT(ISBLANK($H3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E85">
-    <cfRule type="expression" dxfId="30" priority="3">
+    <cfRule type="expression" dxfId="5" priority="3">
       <formula>AND(NOT(ISBLANK($H3)),$E3&lt;10,$H3&lt;&gt;1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:K86">
-    <cfRule type="expression" dxfId="29" priority="1">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>$H3=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16333,7 +16363,7 @@
         <v>66</v>
       </c>
       <c r="C40" s="43" t="s">
-        <v>773</v>
+        <v>769</v>
       </c>
       <c r="D40" s="46" t="s">
         <v>193</v>
@@ -16344,7 +16374,7 @@
         <v>75</v>
       </c>
       <c r="C41" s="36" t="s">
-        <v>773</v>
+        <v>769</v>
       </c>
       <c r="D41" s="36" t="s">
         <v>194</v>
@@ -16355,7 +16385,7 @@
         <v>162</v>
       </c>
       <c r="C42" s="44" t="s">
-        <v>773</v>
+        <v>769</v>
       </c>
       <c r="D42" s="44" t="s">
         <v>195</v>
@@ -16366,7 +16396,7 @@
         <v>163</v>
       </c>
       <c r="C43" s="36" t="s">
-        <v>773</v>
+        <v>769</v>
       </c>
       <c r="D43" s="36" t="s">
         <v>196</v>
@@ -16377,7 +16407,7 @@
         <v>129</v>
       </c>
       <c r="C44" s="44" t="s">
-        <v>773</v>
+        <v>769</v>
       </c>
       <c r="D44" s="44" t="s">
         <v>197</v>
@@ -16388,7 +16418,7 @@
         <v>164</v>
       </c>
       <c r="C45" s="36" t="s">
-        <v>773</v>
+        <v>769</v>
       </c>
       <c r="D45" s="36" t="s">
         <v>191</v>
@@ -16399,7 +16429,7 @@
         <v>165</v>
       </c>
       <c r="C46" s="44" t="s">
-        <v>773</v>
+        <v>769</v>
       </c>
       <c r="D46" s="44" t="s">
         <v>148</v>
@@ -16410,7 +16440,7 @@
         <v>133</v>
       </c>
       <c r="C47" s="36" t="s">
-        <v>773</v>
+        <v>769</v>
       </c>
       <c r="D47" s="36" t="s">
         <v>148</v>
@@ -16421,7 +16451,7 @@
         <v>166</v>
       </c>
       <c r="C48" s="44" t="s">
-        <v>773</v>
+        <v>769</v>
       </c>
       <c r="D48" s="44" t="s">
         <v>198</v>
@@ -16432,7 +16462,7 @@
         <v>167</v>
       </c>
       <c r="C49" s="36" t="s">
-        <v>773</v>
+        <v>769</v>
       </c>
       <c r="D49" s="36" t="s">
         <v>199</v>
@@ -16443,7 +16473,7 @@
         <v>168</v>
       </c>
       <c r="C50" s="44" t="s">
-        <v>773</v>
+        <v>769</v>
       </c>
       <c r="D50" s="44" t="s">
         <v>148</v>
@@ -16454,7 +16484,7 @@
         <v>169</v>
       </c>
       <c r="C51" s="37" t="s">
-        <v>773</v>
+        <v>769</v>
       </c>
       <c r="D51" s="37" t="s">
         <v>148</v>

</xml_diff>

<commit_message>
Update notes; Complete the first version of the auto test demo;
</commit_message>
<xml_diff>
--- a/BZ172Lab/BZ172Lab Notes.xlsx
+++ b/BZ172Lab/BZ172Lab Notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BZ\Projects\PLC61131Repos\BZ172Lab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3092216A-4073-4FEB-ABFB-5D686968940C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78747B41-CC2C-4229-9A26-74BDDE35BD40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="4" r:id="rId1"/>
@@ -36,22 +36,22 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Verification Tracking'!$C$2:$G$7</definedName>
     <definedName name="ALARM_BASE">Requirements!$F$16</definedName>
     <definedName name="AM_ID">Requirements!$B$27</definedName>
-    <definedName name="BO_ID">Requirements!$B$172</definedName>
-    <definedName name="CC_ID">Requirements!$B$131</definedName>
-    <definedName name="CF_ID">Requirements!$B$156</definedName>
-    <definedName name="CP_ID">Requirements!$B$162</definedName>
+    <definedName name="BO_ID">Requirements!$B$173</definedName>
+    <definedName name="CC_ID">Requirements!$B$132</definedName>
+    <definedName name="CF_ID">Requirements!$B$157</definedName>
+    <definedName name="CP_ID">Requirements!$B$163</definedName>
     <definedName name="CW_ID">Requirements!$B$90</definedName>
     <definedName name="EC_ID">Requirements!$B$98</definedName>
-    <definedName name="frs.all">Requirements!$B$3:$E$212</definedName>
-    <definedName name="frs.id">Requirements!$B$2:$B$212</definedName>
+    <definedName name="frs.all">Requirements!$B$3:$E$213</definedName>
+    <definedName name="frs.id">Requirements!$B$2:$B$213</definedName>
     <definedName name="FRS.Level" localSheetId="5">[1]Requirements!$D$4:$D$176</definedName>
-    <definedName name="FRS.Level">Requirements!$C$3:$C$212</definedName>
-    <definedName name="frs.requirement">Requirements!$E$2:$E$212</definedName>
+    <definedName name="FRS.Level">Requirements!$C$3:$C$213</definedName>
+    <definedName name="frs.requirement">Requirements!$E$2:$E$213</definedName>
     <definedName name="FRS.Status" localSheetId="5">[1]Requirements!$E$4:$E$176</definedName>
-    <definedName name="FRS.Status">Requirements!$D$3:$D$212</definedName>
-    <definedName name="FRSList">Requirements!$B$2:$F$208</definedName>
+    <definedName name="FRS.Status">Requirements!$D$3:$D$213</definedName>
+    <definedName name="FRSList">Requirements!$B$2:$F$209</definedName>
     <definedName name="GF_ID">Requirements!$B$3</definedName>
-    <definedName name="GP_ID">Requirements!$B$199</definedName>
+    <definedName name="GP_ID">Requirements!$B$200</definedName>
     <definedName name="notifications" localSheetId="5">OFFSET([2]Settings!$C$1,1,0,MATCH(REPT("z",255),[2]Settings!$C:$C),1)</definedName>
     <definedName name="notifications">OFFSET([3]Settings!$C$1,1,0,MATCH(REPT("z",255),[3]Settings!$C:$C),1)</definedName>
     <definedName name="priorities" localSheetId="5">[4]Settings!$A$2:$A$6</definedName>
@@ -64,9 +64,9 @@
     <definedName name="settings.status">Settings!$B$2:$B$9</definedName>
     <definedName name="status" localSheetId="5">[4]Settings!$B$2:$B$9</definedName>
     <definedName name="status">[5]Settings!$B$2:$B$9</definedName>
-    <definedName name="SV_ID">Requirements!$B$123</definedName>
+    <definedName name="SV_ID">Requirements!$B$124</definedName>
     <definedName name="TaskList">Tasks!$B$2:$K$80</definedName>
-    <definedName name="UO_ID">Requirements!$B$179</definedName>
+    <definedName name="UO_ID">Requirements!$B$180</definedName>
     <definedName name="valuevx">42.314159</definedName>
     <definedName name="VF_ID">Requirements!$B$51</definedName>
     <definedName name="WARNING_BASE">Requirements!$F$14</definedName>
@@ -170,7 +170,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1030" uniqueCount="577">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="579">
   <si>
     <t>Author</t>
   </si>
@@ -2437,6 +2437,14 @@
 Conditions:
     Entry  : Registers cannot be polled from Carel DI module from M172.
     Exit     : Polling success.</t>
+  </si>
+  <si>
+    <t>Varieties of types of refrigerant are supported for superheat calculation and it's configurable. 
+0 R22/1 R134a/2 R404A/3 R407C/4 R410A/5 R407A/6 R407F/7 R290/8 R507A/9 R717/10 R723/11 R1234ze/12 R744/13 R448A/14 R427A/15 R450 (N13)/16 R513A/17 R449A/18 R1234yf/19 R454B/20 R454C/21 R455A/22 R434A/23 R442A/24 R32/25 R452B/26 R452A/
+bzRefrigerantTypeCfg is from 0 to 26 as showed above and 4 is default</t>
+  </si>
+  <si>
+    <t>1.2 version</t>
   </si>
 </sst>
 </file>
@@ -4080,21 +4088,51 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="10" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="15" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="15" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -4103,36 +4141,6 @@
     </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="18" xfId="11" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="10" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="15" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="15" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="2" borderId="1" xfId="12" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5333,6 +5341,9 @@
                 <c:pt idx="2">
                   <c:v>44256</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>44287</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -5347,6 +5358,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5387,6 +5401,9 @@
                 <c:pt idx="2">
                   <c:v>44256</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>44287</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -5401,6 +5418,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5441,6 +5461,9 @@
                 <c:pt idx="2">
                   <c:v>44256</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>44287</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -5454,6 +5477,9 @@
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
@@ -5495,6 +5521,9 @@
                 <c:pt idx="2">
                   <c:v>44256</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>44287</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -5509,6 +5538,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5549,6 +5581,9 @@
                 <c:pt idx="2">
                   <c:v>44256</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>44287</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -5563,6 +5598,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>90</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7613,8 +7651,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DA4C32D8-628E-4DC9-877D-4ED51980429C}" name="Table2" displayName="Table2" ref="B2:F205" totalsRowShown="0" headerRowDxfId="129" tableBorderDxfId="128">
-  <autoFilter ref="B2:F205" xr:uid="{CDEA0ADE-0555-4D01-8A61-CFA14708222C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DA4C32D8-628E-4DC9-877D-4ED51980429C}" name="Table2" displayName="Table2" ref="B2:F206" totalsRowShown="0" headerRowDxfId="129" tableBorderDxfId="128">
+  <autoFilter ref="B2:F206" xr:uid="{CDEA0ADE-0555-4D01-8A61-CFA14708222C}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{EEC440CC-C59E-404F-9916-B7B335C0A1FA}" name="ID" dataDxfId="127"/>
     <tableColumn id="2" xr3:uid="{0D454755-1962-49B9-A9AE-DE3621F55672}" name="LEVEL" dataDxfId="126"/>
@@ -8144,7 +8182,7 @@
       </c>
       <c r="E21" s="197"/>
       <c r="F21" s="198" t="s">
-        <v>489</v>
+        <v>553</v>
       </c>
       <c r="G21" s="198"/>
       <c r="H21" s="198"/>
@@ -8156,7 +8194,7 @@
       </c>
       <c r="F22" s="196">
         <f ca="1">TODAY()</f>
-        <v>44252</v>
+        <v>44257</v>
       </c>
       <c r="G22" s="196"/>
       <c r="H22" s="196"/>
@@ -8445,7 +8483,7 @@
   <dimension ref="E3:F17"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -8497,11 +8535,17 @@
       </c>
     </row>
     <row r="8" spans="5:6">
-      <c r="E8" s="10"/>
-      <c r="F8" s="9"/>
+      <c r="E8" s="10">
+        <v>44256</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>578</v>
+      </c>
     </row>
     <row r="9" spans="5:6">
-      <c r="E9" s="10"/>
+      <c r="E9" s="10">
+        <v>44287</v>
+      </c>
       <c r="F9" s="9"/>
     </row>
     <row r="10" spans="5:6">
@@ -8548,7 +8592,7 @@
   <dimension ref="D2:S41"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22:I22"/>
+      <selection activeCell="F23" sqref="F23:G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8557,23 +8601,23 @@
   </cols>
   <sheetData>
     <row r="2" spans="4:7">
-      <c r="D2" s="208">
+      <c r="D2" s="218">
         <f ca="1">TODAY()</f>
-        <v>44252</v>
-      </c>
-      <c r="E2" s="208"/>
-      <c r="F2" s="208"/>
+        <v>44257</v>
+      </c>
+      <c r="E2" s="218"/>
+      <c r="F2" s="218"/>
     </row>
     <row r="3" spans="4:7">
-      <c r="D3" s="209"/>
-      <c r="E3" s="209"/>
-      <c r="F3" s="209"/>
+      <c r="D3" s="219"/>
+      <c r="E3" s="219"/>
+      <c r="F3" s="219"/>
     </row>
     <row r="4" spans="4:7">
-      <c r="D4" s="207" t="s">
+      <c r="D4" s="217" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="207"/>
+      <c r="E4" s="217"/>
       <c r="F4" s="27">
         <f>COUNTIF(FRS.Level, D4)</f>
         <v>139</v>
@@ -8581,10 +8625,10 @@
       <c r="G4" s="26"/>
     </row>
     <row r="5" spans="4:7">
-      <c r="D5" s="207" t="s">
+      <c r="D5" s="217" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="207"/>
+      <c r="E5" s="217"/>
       <c r="F5" s="27">
         <f>COUNTIF(FRS.Level, D5)</f>
         <v>7</v>
@@ -8592,21 +8636,21 @@
       <c r="G5" s="26"/>
     </row>
     <row r="6" spans="4:7">
-      <c r="D6" s="207" t="s">
+      <c r="D6" s="217" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="207"/>
+      <c r="E6" s="217"/>
       <c r="F6" s="27">
         <f>COUNTIF(FRS.Level, D6)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G6" s="26"/>
     </row>
     <row r="7" spans="4:7">
-      <c r="D7" s="207" t="s">
+      <c r="D7" s="217" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="207"/>
+      <c r="E7" s="217"/>
       <c r="F7" s="27">
         <f>COUNTIF(FRS.Level, D7)</f>
         <v>0</v>
@@ -8618,139 +8662,139 @@
       <c r="E8" s="25"/>
       <c r="F8" s="27">
         <f>SUM(F4:F7)</f>
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="G8" s="26"/>
     </row>
     <row r="10" spans="4:7">
-      <c r="D10" s="207" t="s">
+      <c r="D10" s="217" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="207"/>
+      <c r="E10" s="217"/>
       <c r="F10" s="27">
         <f t="shared" ref="F10:F16" si="0">COUNTIF(FRS.Status,D10)</f>
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="4:7">
-      <c r="D11" s="207" t="s">
+      <c r="D11" s="217" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="207"/>
+      <c r="E11" s="217"/>
       <c r="F11" s="27">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="4:7">
-      <c r="D12" s="207" t="s">
+      <c r="D12" s="217" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="207"/>
+      <c r="E12" s="217"/>
       <c r="F12" s="27">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="4:7">
-      <c r="D13" s="207" t="s">
+      <c r="D13" s="217" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="207"/>
+      <c r="E13" s="217"/>
       <c r="F13" s="27">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
     <row r="14" spans="4:7">
-      <c r="D14" s="207" t="s">
+      <c r="D14" s="217" t="s">
         <v>24</v>
       </c>
-      <c r="E14" s="207"/>
+      <c r="E14" s="217"/>
       <c r="F14" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="4:7">
-      <c r="D15" s="207" t="s">
+      <c r="D15" s="217" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="207"/>
+      <c r="E15" s="217"/>
       <c r="F15" s="27">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="4:7">
-      <c r="D16" s="207" t="s">
+      <c r="D16" s="217" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="207"/>
+      <c r="E16" s="217"/>
       <c r="F16" s="27">
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
     </row>
     <row r="18" spans="4:19" ht="20.25" thickBot="1">
-      <c r="D18" s="219" t="s">
+      <c r="D18" s="209" t="s">
         <v>46</v>
       </c>
-      <c r="E18" s="219"/>
-      <c r="F18" s="219"/>
-      <c r="G18" s="219"/>
-      <c r="H18" s="218" t="s">
+      <c r="E18" s="209"/>
+      <c r="F18" s="209"/>
+      <c r="G18" s="209"/>
+      <c r="H18" s="208" t="s">
         <v>47</v>
       </c>
-      <c r="I18" s="218"/>
-      <c r="J18" s="218"/>
-      <c r="K18" s="218"/>
-      <c r="L18" s="218"/>
-      <c r="M18" s="218"/>
-      <c r="N18" s="218"/>
-      <c r="O18" s="218"/>
-      <c r="P18" s="218"/>
-      <c r="Q18" s="218"/>
+      <c r="I18" s="208"/>
+      <c r="J18" s="208"/>
+      <c r="K18" s="208"/>
+      <c r="L18" s="208"/>
+      <c r="M18" s="208"/>
+      <c r="N18" s="208"/>
+      <c r="O18" s="208"/>
+      <c r="P18" s="208"/>
+      <c r="Q18" s="208"/>
     </row>
     <row r="19" spans="4:19" ht="15.75" thickTop="1">
-      <c r="D19" s="215" t="s">
+      <c r="D19" s="202" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="215"/>
-      <c r="F19" s="215" t="s">
+      <c r="E19" s="202"/>
+      <c r="F19" s="202" t="s">
         <v>2</v>
       </c>
-      <c r="G19" s="215"/>
-      <c r="H19" s="215" t="s">
+      <c r="G19" s="202"/>
+      <c r="H19" s="202" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="215"/>
-      <c r="J19" s="215" t="s">
+      <c r="I19" s="202"/>
+      <c r="J19" s="202" t="s">
         <v>18</v>
       </c>
-      <c r="K19" s="215"/>
-      <c r="L19" s="215" t="s">
+      <c r="K19" s="202"/>
+      <c r="L19" s="202" t="s">
         <v>15</v>
       </c>
-      <c r="M19" s="215"/>
-      <c r="N19" s="215" t="s">
+      <c r="M19" s="202"/>
+      <c r="N19" s="202" t="s">
         <v>21</v>
       </c>
-      <c r="O19" s="215"/>
-      <c r="P19" s="215" t="s">
+      <c r="O19" s="202"/>
+      <c r="P19" s="202" t="s">
         <v>29</v>
       </c>
-      <c r="Q19" s="215"/>
+      <c r="Q19" s="202"/>
     </row>
     <row r="20" spans="4:19">
-      <c r="D20" s="202">
+      <c r="D20" s="203">
         <v>44221</v>
       </c>
-      <c r="E20" s="203"/>
-      <c r="F20" s="204" t="s">
+      <c r="E20" s="204"/>
+      <c r="F20" s="212" t="s">
         <v>109</v>
       </c>
-      <c r="G20" s="204"/>
+      <c r="G20" s="212"/>
       <c r="H20" s="205">
         <v>8</v>
       </c>
@@ -8767,21 +8811,21 @@
         <v>0</v>
       </c>
       <c r="O20" s="205"/>
-      <c r="P20" s="216">
+      <c r="P20" s="206">
         <v>0</v>
       </c>
-      <c r="Q20" s="217"/>
+      <c r="Q20" s="207"/>
       <c r="S20" s="28"/>
     </row>
     <row r="21" spans="4:19">
-      <c r="D21" s="202">
+      <c r="D21" s="203">
         <v>44237</v>
       </c>
-      <c r="E21" s="203"/>
-      <c r="F21" s="204" t="s">
+      <c r="E21" s="204"/>
+      <c r="F21" s="212" t="s">
         <v>489</v>
       </c>
-      <c r="G21" s="204"/>
+      <c r="G21" s="212"/>
       <c r="H21" s="205">
         <v>9</v>
       </c>
@@ -8801,33 +8845,45 @@
       <c r="P21" s="205">
         <v>56</v>
       </c>
-      <c r="Q21" s="206"/>
+      <c r="Q21" s="215"/>
     </row>
     <row r="22" spans="4:19">
-      <c r="D22" s="202">
+      <c r="D22" s="203">
         <v>44256</v>
       </c>
-      <c r="E22" s="203"/>
-      <c r="F22" s="204" t="s">
+      <c r="E22" s="204"/>
+      <c r="F22" s="212" t="s">
         <v>553</v>
       </c>
-      <c r="G22" s="204"/>
-      <c r="H22" s="205"/>
+      <c r="G22" s="212"/>
+      <c r="H22" s="205">
+        <v>4</v>
+      </c>
       <c r="I22" s="205"/>
-      <c r="J22" s="205"/>
+      <c r="J22" s="205">
+        <v>32</v>
+      </c>
       <c r="K22" s="205"/>
-      <c r="L22" s="205"/>
+      <c r="L22" s="205">
+        <v>10</v>
+      </c>
       <c r="M22" s="205"/>
-      <c r="N22" s="205"/>
+      <c r="N22" s="205">
+        <v>15</v>
+      </c>
       <c r="O22" s="205"/>
-      <c r="P22" s="205"/>
-      <c r="Q22" s="206"/>
+      <c r="P22" s="205">
+        <v>90</v>
+      </c>
+      <c r="Q22" s="215"/>
     </row>
     <row r="23" spans="4:19">
-      <c r="D23" s="202"/>
-      <c r="E23" s="203"/>
-      <c r="F23" s="204"/>
-      <c r="G23" s="204"/>
+      <c r="D23" s="203">
+        <v>44287</v>
+      </c>
+      <c r="E23" s="204"/>
+      <c r="F23" s="212"/>
+      <c r="G23" s="212"/>
       <c r="H23" s="205"/>
       <c r="I23" s="205"/>
       <c r="J23" s="205"/>
@@ -8837,13 +8893,13 @@
       <c r="N23" s="205"/>
       <c r="O23" s="205"/>
       <c r="P23" s="205"/>
-      <c r="Q23" s="206"/>
+      <c r="Q23" s="215"/>
     </row>
     <row r="24" spans="4:19">
-      <c r="D24" s="202"/>
-      <c r="E24" s="203"/>
-      <c r="F24" s="204"/>
-      <c r="G24" s="204"/>
+      <c r="D24" s="203"/>
+      <c r="E24" s="204"/>
+      <c r="F24" s="212"/>
+      <c r="G24" s="212"/>
       <c r="H24" s="205"/>
       <c r="I24" s="205"/>
       <c r="J24" s="205"/>
@@ -8853,13 +8909,13 @@
       <c r="N24" s="205"/>
       <c r="O24" s="205"/>
       <c r="P24" s="205"/>
-      <c r="Q24" s="206"/>
+      <c r="Q24" s="215"/>
     </row>
     <row r="25" spans="4:19">
-      <c r="D25" s="202"/>
-      <c r="E25" s="203"/>
-      <c r="F25" s="204"/>
-      <c r="G25" s="204"/>
+      <c r="D25" s="203"/>
+      <c r="E25" s="204"/>
+      <c r="F25" s="212"/>
+      <c r="G25" s="212"/>
       <c r="H25" s="205"/>
       <c r="I25" s="205"/>
       <c r="J25" s="205"/>
@@ -8869,13 +8925,13 @@
       <c r="N25" s="205"/>
       <c r="O25" s="205"/>
       <c r="P25" s="205"/>
-      <c r="Q25" s="206"/>
+      <c r="Q25" s="215"/>
     </row>
     <row r="26" spans="4:19">
-      <c r="D26" s="202"/>
-      <c r="E26" s="203"/>
-      <c r="F26" s="204"/>
-      <c r="G26" s="204"/>
+      <c r="D26" s="203"/>
+      <c r="E26" s="204"/>
+      <c r="F26" s="212"/>
+      <c r="G26" s="212"/>
       <c r="H26" s="205"/>
       <c r="I26" s="205"/>
       <c r="J26" s="205"/>
@@ -8885,13 +8941,13 @@
       <c r="N26" s="205"/>
       <c r="O26" s="205"/>
       <c r="P26" s="205"/>
-      <c r="Q26" s="206"/>
+      <c r="Q26" s="215"/>
     </row>
     <row r="27" spans="4:19">
-      <c r="D27" s="202"/>
-      <c r="E27" s="203"/>
-      <c r="F27" s="204"/>
-      <c r="G27" s="204"/>
+      <c r="D27" s="203"/>
+      <c r="E27" s="204"/>
+      <c r="F27" s="212"/>
+      <c r="G27" s="212"/>
       <c r="H27" s="205"/>
       <c r="I27" s="205"/>
       <c r="J27" s="205"/>
@@ -8901,13 +8957,13 @@
       <c r="N27" s="205"/>
       <c r="O27" s="205"/>
       <c r="P27" s="205"/>
-      <c r="Q27" s="206"/>
+      <c r="Q27" s="215"/>
     </row>
     <row r="28" spans="4:19">
-      <c r="D28" s="202"/>
-      <c r="E28" s="203"/>
-      <c r="F28" s="204"/>
-      <c r="G28" s="204"/>
+      <c r="D28" s="203"/>
+      <c r="E28" s="204"/>
+      <c r="F28" s="212"/>
+      <c r="G28" s="212"/>
       <c r="H28" s="205"/>
       <c r="I28" s="205"/>
       <c r="J28" s="205"/>
@@ -8917,13 +8973,13 @@
       <c r="N28" s="205"/>
       <c r="O28" s="205"/>
       <c r="P28" s="205"/>
-      <c r="Q28" s="206"/>
+      <c r="Q28" s="215"/>
     </row>
     <row r="29" spans="4:19">
-      <c r="D29" s="202"/>
-      <c r="E29" s="203"/>
-      <c r="F29" s="204"/>
-      <c r="G29" s="204"/>
+      <c r="D29" s="203"/>
+      <c r="E29" s="204"/>
+      <c r="F29" s="212"/>
+      <c r="G29" s="212"/>
       <c r="H29" s="205"/>
       <c r="I29" s="205"/>
       <c r="J29" s="205"/>
@@ -8933,13 +8989,13 @@
       <c r="N29" s="205"/>
       <c r="O29" s="205"/>
       <c r="P29" s="205"/>
-      <c r="Q29" s="206"/>
+      <c r="Q29" s="215"/>
     </row>
     <row r="30" spans="4:19">
-      <c r="D30" s="202"/>
-      <c r="E30" s="203"/>
-      <c r="F30" s="204"/>
-      <c r="G30" s="204"/>
+      <c r="D30" s="203"/>
+      <c r="E30" s="204"/>
+      <c r="F30" s="212"/>
+      <c r="G30" s="212"/>
       <c r="H30" s="205"/>
       <c r="I30" s="205"/>
       <c r="J30" s="205"/>
@@ -8949,13 +9005,13 @@
       <c r="N30" s="205"/>
       <c r="O30" s="205"/>
       <c r="P30" s="205"/>
-      <c r="Q30" s="206"/>
+      <c r="Q30" s="215"/>
     </row>
     <row r="31" spans="4:19">
-      <c r="D31" s="202"/>
-      <c r="E31" s="203"/>
-      <c r="F31" s="204"/>
-      <c r="G31" s="204"/>
+      <c r="D31" s="203"/>
+      <c r="E31" s="204"/>
+      <c r="F31" s="212"/>
+      <c r="G31" s="212"/>
       <c r="H31" s="205"/>
       <c r="I31" s="205"/>
       <c r="J31" s="205"/>
@@ -8965,13 +9021,13 @@
       <c r="N31" s="205"/>
       <c r="O31" s="205"/>
       <c r="P31" s="205"/>
-      <c r="Q31" s="206"/>
+      <c r="Q31" s="215"/>
     </row>
     <row r="32" spans="4:19">
-      <c r="D32" s="202"/>
-      <c r="E32" s="203"/>
-      <c r="F32" s="204"/>
-      <c r="G32" s="204"/>
+      <c r="D32" s="203"/>
+      <c r="E32" s="204"/>
+      <c r="F32" s="212"/>
+      <c r="G32" s="212"/>
       <c r="H32" s="205"/>
       <c r="I32" s="205"/>
       <c r="J32" s="205"/>
@@ -8981,13 +9037,13 @@
       <c r="N32" s="205"/>
       <c r="O32" s="205"/>
       <c r="P32" s="205"/>
-      <c r="Q32" s="206"/>
+      <c r="Q32" s="215"/>
     </row>
     <row r="33" spans="4:17">
-      <c r="D33" s="202"/>
-      <c r="E33" s="203"/>
-      <c r="F33" s="204"/>
-      <c r="G33" s="204"/>
+      <c r="D33" s="203"/>
+      <c r="E33" s="204"/>
+      <c r="F33" s="212"/>
+      <c r="G33" s="212"/>
       <c r="H33" s="205"/>
       <c r="I33" s="205"/>
       <c r="J33" s="205"/>
@@ -8997,13 +9053,13 @@
       <c r="N33" s="205"/>
       <c r="O33" s="205"/>
       <c r="P33" s="205"/>
-      <c r="Q33" s="206"/>
+      <c r="Q33" s="215"/>
     </row>
     <row r="34" spans="4:17">
-      <c r="D34" s="202"/>
-      <c r="E34" s="203"/>
-      <c r="F34" s="204"/>
-      <c r="G34" s="204"/>
+      <c r="D34" s="203"/>
+      <c r="E34" s="204"/>
+      <c r="F34" s="212"/>
+      <c r="G34" s="212"/>
       <c r="H34" s="205"/>
       <c r="I34" s="205"/>
       <c r="J34" s="205"/>
@@ -9013,13 +9069,13 @@
       <c r="N34" s="205"/>
       <c r="O34" s="205"/>
       <c r="P34" s="205"/>
-      <c r="Q34" s="206"/>
+      <c r="Q34" s="215"/>
     </row>
     <row r="35" spans="4:17">
-      <c r="D35" s="202"/>
-      <c r="E35" s="203"/>
-      <c r="F35" s="204"/>
-      <c r="G35" s="204"/>
+      <c r="D35" s="203"/>
+      <c r="E35" s="204"/>
+      <c r="F35" s="212"/>
+      <c r="G35" s="212"/>
       <c r="H35" s="205"/>
       <c r="I35" s="205"/>
       <c r="J35" s="205"/>
@@ -9029,13 +9085,13 @@
       <c r="N35" s="205"/>
       <c r="O35" s="205"/>
       <c r="P35" s="205"/>
-      <c r="Q35" s="206"/>
+      <c r="Q35" s="215"/>
     </row>
     <row r="36" spans="4:17">
-      <c r="D36" s="202"/>
-      <c r="E36" s="203"/>
-      <c r="F36" s="204"/>
-      <c r="G36" s="204"/>
+      <c r="D36" s="203"/>
+      <c r="E36" s="204"/>
+      <c r="F36" s="212"/>
+      <c r="G36" s="212"/>
       <c r="H36" s="205"/>
       <c r="I36" s="205"/>
       <c r="J36" s="205"/>
@@ -9045,13 +9101,13 @@
       <c r="N36" s="205"/>
       <c r="O36" s="205"/>
       <c r="P36" s="205"/>
-      <c r="Q36" s="206"/>
+      <c r="Q36" s="215"/>
     </row>
     <row r="37" spans="4:17">
-      <c r="D37" s="202"/>
-      <c r="E37" s="203"/>
-      <c r="F37" s="204"/>
-      <c r="G37" s="204"/>
+      <c r="D37" s="203"/>
+      <c r="E37" s="204"/>
+      <c r="F37" s="212"/>
+      <c r="G37" s="212"/>
       <c r="H37" s="205"/>
       <c r="I37" s="205"/>
       <c r="J37" s="205"/>
@@ -9061,13 +9117,13 @@
       <c r="N37" s="205"/>
       <c r="O37" s="205"/>
       <c r="P37" s="205"/>
-      <c r="Q37" s="206"/>
+      <c r="Q37" s="215"/>
     </row>
     <row r="38" spans="4:17">
-      <c r="D38" s="202"/>
-      <c r="E38" s="203"/>
-      <c r="F38" s="204"/>
-      <c r="G38" s="204"/>
+      <c r="D38" s="203"/>
+      <c r="E38" s="204"/>
+      <c r="F38" s="212"/>
+      <c r="G38" s="212"/>
       <c r="H38" s="205"/>
       <c r="I38" s="205"/>
       <c r="J38" s="205"/>
@@ -9077,13 +9133,13 @@
       <c r="N38" s="205"/>
       <c r="O38" s="205"/>
       <c r="P38" s="205"/>
-      <c r="Q38" s="206"/>
+      <c r="Q38" s="215"/>
     </row>
     <row r="39" spans="4:17">
-      <c r="D39" s="202"/>
-      <c r="E39" s="203"/>
-      <c r="F39" s="204"/>
-      <c r="G39" s="204"/>
+      <c r="D39" s="203"/>
+      <c r="E39" s="204"/>
+      <c r="F39" s="212"/>
+      <c r="G39" s="212"/>
       <c r="H39" s="205"/>
       <c r="I39" s="205"/>
       <c r="J39" s="205"/>
@@ -9093,23 +9149,23 @@
       <c r="N39" s="205"/>
       <c r="O39" s="205"/>
       <c r="P39" s="205"/>
-      <c r="Q39" s="206"/>
+      <c r="Q39" s="215"/>
     </row>
     <row r="40" spans="4:17">
-      <c r="D40" s="213"/>
-      <c r="E40" s="214"/>
-      <c r="F40" s="212"/>
-      <c r="G40" s="212"/>
-      <c r="H40" s="210"/>
-      <c r="I40" s="210"/>
-      <c r="J40" s="210"/>
-      <c r="K40" s="210"/>
-      <c r="L40" s="210"/>
-      <c r="M40" s="210"/>
-      <c r="N40" s="210"/>
-      <c r="O40" s="210"/>
-      <c r="P40" s="210"/>
-      <c r="Q40" s="211"/>
+      <c r="D40" s="210"/>
+      <c r="E40" s="211"/>
+      <c r="F40" s="213"/>
+      <c r="G40" s="213"/>
+      <c r="H40" s="214"/>
+      <c r="I40" s="214"/>
+      <c r="J40" s="214"/>
+      <c r="K40" s="214"/>
+      <c r="L40" s="214"/>
+      <c r="M40" s="214"/>
+      <c r="N40" s="214"/>
+      <c r="O40" s="214"/>
+      <c r="P40" s="214"/>
+      <c r="Q40" s="216"/>
     </row>
     <row r="41" spans="4:17">
       <c r="D41" s="24"/>
@@ -9117,21 +9173,135 @@
     </row>
   </sheetData>
   <mergeCells count="168">
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="P19:Q19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="H18:Q18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="D18:G18"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="L34:M34"/>
+    <mergeCell ref="N34:O34"/>
+    <mergeCell ref="P34:Q34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="J35:K35"/>
+    <mergeCell ref="L35:M35"/>
+    <mergeCell ref="N35:O35"/>
+    <mergeCell ref="P35:Q35"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="L31:M31"/>
+    <mergeCell ref="N31:O31"/>
+    <mergeCell ref="P31:Q31"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="N29:O29"/>
+    <mergeCell ref="P29:Q29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="N30:O30"/>
+    <mergeCell ref="P30:Q30"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D2:F3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="P38:Q38"/>
+    <mergeCell ref="P39:Q39"/>
+    <mergeCell ref="P40:Q40"/>
+    <mergeCell ref="P26:Q26"/>
+    <mergeCell ref="P27:Q27"/>
+    <mergeCell ref="P28:Q28"/>
+    <mergeCell ref="P32:Q32"/>
+    <mergeCell ref="P33:Q33"/>
+    <mergeCell ref="P36:Q36"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="P22:Q22"/>
+    <mergeCell ref="P23:Q23"/>
+    <mergeCell ref="P24:Q24"/>
+    <mergeCell ref="P25:Q25"/>
+    <mergeCell ref="N33:O33"/>
+    <mergeCell ref="N36:O36"/>
+    <mergeCell ref="N37:O37"/>
+    <mergeCell ref="P37:Q37"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="N38:O38"/>
+    <mergeCell ref="N39:O39"/>
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="N26:O26"/>
+    <mergeCell ref="N27:O27"/>
+    <mergeCell ref="N28:O28"/>
+    <mergeCell ref="N32:O32"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="L37:M37"/>
+    <mergeCell ref="L38:M38"/>
+    <mergeCell ref="L39:M39"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="L40:M40"/>
+    <mergeCell ref="L26:M26"/>
+    <mergeCell ref="L27:M27"/>
+    <mergeCell ref="L28:M28"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="L33:M33"/>
+    <mergeCell ref="L36:M36"/>
+    <mergeCell ref="N40:O40"/>
+    <mergeCell ref="J33:K33"/>
+    <mergeCell ref="J36:K36"/>
+    <mergeCell ref="J37:K37"/>
+    <mergeCell ref="J38:K38"/>
+    <mergeCell ref="J39:K39"/>
+    <mergeCell ref="J40:K40"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="H36:I36"/>
     <mergeCell ref="D37:E37"/>
     <mergeCell ref="D38:E38"/>
     <mergeCell ref="D39:E39"/>
@@ -9156,135 +9326,21 @@
     <mergeCell ref="F37:G37"/>
     <mergeCell ref="F38:G38"/>
     <mergeCell ref="F39:G39"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="H40:I40"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="L40:M40"/>
-    <mergeCell ref="L26:M26"/>
-    <mergeCell ref="L27:M27"/>
-    <mergeCell ref="L28:M28"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="L33:M33"/>
-    <mergeCell ref="L36:M36"/>
-    <mergeCell ref="N40:O40"/>
-    <mergeCell ref="J33:K33"/>
-    <mergeCell ref="J36:K36"/>
-    <mergeCell ref="J37:K37"/>
-    <mergeCell ref="J38:K38"/>
-    <mergeCell ref="J39:K39"/>
-    <mergeCell ref="J40:K40"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="L24:M24"/>
-    <mergeCell ref="L25:M25"/>
-    <mergeCell ref="N38:O38"/>
-    <mergeCell ref="N39:O39"/>
-    <mergeCell ref="N24:O24"/>
-    <mergeCell ref="N25:O25"/>
-    <mergeCell ref="N26:O26"/>
-    <mergeCell ref="N27:O27"/>
-    <mergeCell ref="N28:O28"/>
-    <mergeCell ref="N32:O32"/>
-    <mergeCell ref="N21:O21"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="L37:M37"/>
-    <mergeCell ref="L38:M38"/>
-    <mergeCell ref="L39:M39"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="P21:Q21"/>
-    <mergeCell ref="P22:Q22"/>
-    <mergeCell ref="P23:Q23"/>
-    <mergeCell ref="P24:Q24"/>
-    <mergeCell ref="P25:Q25"/>
-    <mergeCell ref="N33:O33"/>
-    <mergeCell ref="N36:O36"/>
-    <mergeCell ref="N37:O37"/>
-    <mergeCell ref="P37:Q37"/>
-    <mergeCell ref="P38:Q38"/>
-    <mergeCell ref="P39:Q39"/>
-    <mergeCell ref="P40:Q40"/>
-    <mergeCell ref="P26:Q26"/>
-    <mergeCell ref="P27:Q27"/>
-    <mergeCell ref="P28:Q28"/>
-    <mergeCell ref="P32:Q32"/>
-    <mergeCell ref="P33:Q33"/>
-    <mergeCell ref="P36:Q36"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D2:F3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="L31:M31"/>
-    <mergeCell ref="N31:O31"/>
-    <mergeCell ref="P31:Q31"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="L29:M29"/>
-    <mergeCell ref="N29:O29"/>
-    <mergeCell ref="P29:Q29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="N30:O30"/>
-    <mergeCell ref="P30:Q30"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="J34:K34"/>
-    <mergeCell ref="L34:M34"/>
-    <mergeCell ref="N34:O34"/>
-    <mergeCell ref="P34:Q34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="J35:K35"/>
-    <mergeCell ref="L35:M35"/>
-    <mergeCell ref="N35:O35"/>
-    <mergeCell ref="P35:Q35"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="H18:Q18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="D18:G18"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="N20:O20"/>
   </mergeCells>
   <phoneticPr fontId="22" type="noConversion"/>
   <dataValidations disablePrompts="1" count="1">
@@ -9306,13 +9362,13 @@
   <sheetPr codeName="Sheet5">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:F213"/>
+  <dimension ref="B1:F214"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B99" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E20" sqref="E20"/>
+      <selection pane="bottomRight" activeCell="D108" sqref="D108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -10237,7 +10293,7 @@
       </c>
       <c r="F60" s="92"/>
     </row>
-    <row r="61" spans="2:6" ht="285" outlineLevel="1">
+    <row r="61" spans="2:6" ht="300" outlineLevel="1">
       <c r="B61" s="30" t="str">
         <f t="shared" si="3"/>
         <v>VF.010</v>
@@ -10789,7 +10845,7 @@
     </row>
     <row r="99" spans="2:6" ht="30" outlineLevel="1">
       <c r="B99" s="31" t="str">
-        <f t="shared" ref="B99:B119" si="6">_xlfn.CONCAT(EC_ID,".",TEXT(ROW()-ROW(EC_ID), "000"))</f>
+        <f t="shared" ref="B99:B120" si="6">_xlfn.CONCAT(EC_ID,".",TEXT(ROW()-ROW(EC_ID), "000"))</f>
         <v>EC.001</v>
       </c>
       <c r="C99" s="14" t="s">
@@ -10931,58 +10987,55 @@
       </c>
       <c r="F107" s="92"/>
     </row>
-    <row r="108" spans="2:6" outlineLevel="1">
+    <row r="108" spans="2:6" ht="120" outlineLevel="1">
       <c r="B108" s="31" t="str">
         <f t="shared" si="6"/>
         <v>EC.010</v>
       </c>
-      <c r="C108" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="D108" s="14" t="s">
-        <v>29</v>
+      <c r="C108" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D108" s="20" t="s">
+        <v>18</v>
       </c>
       <c r="E108" s="21" t="s">
-        <v>413</v>
-      </c>
-      <c r="F108" s="32"/>
+        <v>577</v>
+      </c>
+      <c r="F108" s="92"/>
     </row>
     <row r="109" spans="2:6" outlineLevel="1">
       <c r="B109" s="31" t="str">
         <f t="shared" si="6"/>
         <v>EC.011</v>
       </c>
-      <c r="C109" s="20" t="s">
+      <c r="C109" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="D109" s="20" t="s">
+      <c r="D109" s="14" t="s">
         <v>29</v>
       </c>
       <c r="E109" s="21" t="s">
-        <v>386</v>
-      </c>
-      <c r="F109" s="92"/>
-    </row>
-    <row r="110" spans="2:6" ht="105" outlineLevel="1">
+        <v>413</v>
+      </c>
+      <c r="F109" s="32"/>
+    </row>
+    <row r="110" spans="2:6" outlineLevel="1">
       <c r="B110" s="31" t="str">
         <f t="shared" si="6"/>
         <v>EC.012</v>
       </c>
-      <c r="C110" s="14" t="s">
+      <c r="C110" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="D110" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="E110" s="16" t="s">
-        <v>403</v>
-      </c>
-      <c r="F110" s="32">
-        <f t="shared" ref="F110:F113" si="7">WARNING_BASE + MID(E110, SEARCH("[",E110) + 1, SEARCH("]",E110) - SEARCH("[",E110) - 1)</f>
-        <v>10010</v>
-      </c>
-    </row>
-    <row r="111" spans="2:6" ht="75" outlineLevel="1">
+      <c r="D110" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="E110" s="21" t="s">
+        <v>386</v>
+      </c>
+      <c r="F110" s="92"/>
+    </row>
+    <row r="111" spans="2:6" ht="105" outlineLevel="1">
       <c r="B111" s="31" t="str">
         <f t="shared" si="6"/>
         <v>EC.013</v>
@@ -10993,31 +11046,31 @@
       <c r="D111" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="E111" s="102" t="s">
-        <v>404</v>
-      </c>
-      <c r="F111" s="32"/>
+      <c r="E111" s="16" t="s">
+        <v>403</v>
+      </c>
+      <c r="F111" s="32">
+        <f t="shared" ref="F111:F114" si="7">WARNING_BASE + MID(E111, SEARCH("[",E111) + 1, SEARCH("]",E111) - SEARCH("[",E111) - 1)</f>
+        <v>10010</v>
+      </c>
     </row>
     <row r="112" spans="2:6" ht="75" outlineLevel="1">
       <c r="B112" s="31" t="str">
         <f t="shared" si="6"/>
         <v>EC.014</v>
       </c>
-      <c r="C112" s="20" t="s">
+      <c r="C112" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="D112" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="E112" s="185" t="s">
-        <v>561</v>
-      </c>
-      <c r="F112" s="32">
-        <f t="shared" si="7"/>
-        <v>10011</v>
-      </c>
-    </row>
-    <row r="113" spans="2:6" ht="45" outlineLevel="1">
+      <c r="D112" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E112" s="102" t="s">
+        <v>404</v>
+      </c>
+      <c r="F112" s="32"/>
+    </row>
+    <row r="113" spans="2:6" ht="75" outlineLevel="1">
       <c r="B113" s="31" t="str">
         <f t="shared" si="6"/>
         <v>EC.015</v>
@@ -11026,17 +11079,17 @@
         <v>35</v>
       </c>
       <c r="D113" s="20" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="E113" s="185" t="s">
-        <v>407</v>
+        <v>561</v>
       </c>
       <c r="F113" s="32">
         <f t="shared" si="7"/>
-        <v>10012</v>
-      </c>
-    </row>
-    <row r="114" spans="2:6" outlineLevel="1">
+        <v>10011</v>
+      </c>
+    </row>
+    <row r="114" spans="2:6" ht="45" outlineLevel="1">
       <c r="B114" s="31" t="str">
         <f t="shared" si="6"/>
         <v>EC.016</v>
@@ -11045,14 +11098,17 @@
         <v>35</v>
       </c>
       <c r="D114" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="E114" s="21" t="s">
-        <v>390</v>
-      </c>
-      <c r="F114" s="92"/>
-    </row>
-    <row r="115" spans="2:6" ht="60" outlineLevel="1">
+        <v>15</v>
+      </c>
+      <c r="E114" s="185" t="s">
+        <v>407</v>
+      </c>
+      <c r="F114" s="32">
+        <f t="shared" si="7"/>
+        <v>10012</v>
+      </c>
+    </row>
+    <row r="115" spans="2:6" outlineLevel="1">
       <c r="B115" s="31" t="str">
         <f t="shared" si="6"/>
         <v>EC.017</v>
@@ -11061,15 +11117,12 @@
         <v>35</v>
       </c>
       <c r="D115" s="20" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="E115" s="21" t="s">
-        <v>394</v>
-      </c>
-      <c r="F115" s="32">
-        <f>ALARM_BASE + MID(E115, SEARCH("[",E115) + 1, SEARCH("]",E115) - SEARCH("[",E115) - 1)</f>
-        <v>10210</v>
-      </c>
+        <v>390</v>
+      </c>
+      <c r="F115" s="92"/>
     </row>
     <row r="116" spans="2:6" ht="60" outlineLevel="1">
       <c r="B116" s="31" t="str">
@@ -11080,14 +11133,14 @@
         <v>35</v>
       </c>
       <c r="D116" s="20" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="E116" s="21" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F116" s="32">
         <f>ALARM_BASE + MID(E116, SEARCH("[",E116) + 1, SEARCH("]",E116) - SEARCH("[",E116) - 1)</f>
-        <v>10211</v>
+        <v>10210</v>
       </c>
     </row>
     <row r="117" spans="2:6" ht="60" outlineLevel="1">
@@ -11095,21 +11148,21 @@
         <f t="shared" si="6"/>
         <v>EC.019</v>
       </c>
-      <c r="C117" s="14" t="s">
+      <c r="C117" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="D117" s="14" t="s">
+      <c r="D117" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="E117" s="16" t="s">
-        <v>396</v>
+      <c r="E117" s="21" t="s">
+        <v>395</v>
       </c>
       <c r="F117" s="32">
         <f>ALARM_BASE + MID(E117, SEARCH("[",E117) + 1, SEARCH("]",E117) - SEARCH("[",E117) - 1)</f>
-        <v>10212</v>
-      </c>
-    </row>
-    <row r="118" spans="2:6" ht="90" outlineLevel="1">
+        <v>10211</v>
+      </c>
+    </row>
+    <row r="118" spans="2:6" ht="60" outlineLevel="1">
       <c r="B118" s="31" t="str">
         <f t="shared" si="6"/>
         <v>EC.020</v>
@@ -11121,14 +11174,14 @@
         <v>18</v>
       </c>
       <c r="E118" s="16" t="s">
-        <v>405</v>
+        <v>396</v>
       </c>
       <c r="F118" s="32">
         <f>ALARM_BASE + MID(E118, SEARCH("[",E118) + 1, SEARCH("]",E118) - SEARCH("[",E118) - 1)</f>
-        <v>10213</v>
-      </c>
-    </row>
-    <row r="119" spans="2:6" ht="45" outlineLevel="1">
+        <v>10212</v>
+      </c>
+    </row>
+    <row r="119" spans="2:6" ht="90" outlineLevel="1">
       <c r="B119" s="31" t="str">
         <f t="shared" si="6"/>
         <v>EC.021</v>
@@ -11137,29 +11190,41 @@
         <v>35</v>
       </c>
       <c r="D119" s="14" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E119" s="16" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F119" s="32">
         <f>ALARM_BASE + MID(E119, SEARCH("[",E119) + 1, SEARCH("]",E119) - SEARCH("[",E119) - 1)</f>
+        <v>10213</v>
+      </c>
+    </row>
+    <row r="120" spans="2:6" ht="45" outlineLevel="1">
+      <c r="B120" s="31" t="str">
+        <f t="shared" si="6"/>
+        <v>EC.022</v>
+      </c>
+      <c r="C120" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D120" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E120" s="16" t="s">
+        <v>406</v>
+      </c>
+      <c r="F120" s="32">
+        <f>ALARM_BASE + MID(E120, SEARCH("[",E120) + 1, SEARCH("]",E120) - SEARCH("[",E120) - 1)</f>
         <v>10214</v>
       </c>
     </row>
-    <row r="120" spans="2:6" outlineLevel="1">
-      <c r="B120" s="91"/>
-      <c r="C120" s="20"/>
-      <c r="D120" s="20"/>
-      <c r="E120" s="21"/>
-      <c r="F120" s="92"/>
-    </row>
     <row r="121" spans="2:6" outlineLevel="1">
-      <c r="B121" s="31"/>
-      <c r="C121" s="14"/>
-      <c r="D121" s="14"/>
-      <c r="E121" s="16"/>
-      <c r="F121" s="32"/>
+      <c r="B121" s="91"/>
+      <c r="C121" s="20"/>
+      <c r="D121" s="20"/>
+      <c r="E121" s="21"/>
+      <c r="F121" s="92"/>
     </row>
     <row r="122" spans="2:6" outlineLevel="1">
       <c r="B122" s="31"/>
@@ -11168,106 +11233,106 @@
       <c r="E122" s="16"/>
       <c r="F122" s="32"/>
     </row>
-    <row r="123" spans="2:6">
-      <c r="B123" s="18" t="s">
+    <row r="123" spans="2:6" outlineLevel="1">
+      <c r="B123" s="31"/>
+      <c r="C123" s="14"/>
+      <c r="D123" s="14"/>
+      <c r="E123" s="16"/>
+      <c r="F123" s="32"/>
+    </row>
+    <row r="124" spans="2:6">
+      <c r="B124" s="18" t="s">
         <v>251</v>
       </c>
-      <c r="C123" s="19"/>
-      <c r="D123" s="19"/>
-      <c r="E123" s="96" t="s">
+      <c r="C124" s="19"/>
+      <c r="D124" s="19"/>
+      <c r="E124" s="96" t="s">
         <v>252</v>
       </c>
-      <c r="F123" s="97"/>
-    </row>
-    <row r="124" spans="2:6" outlineLevel="1">
-      <c r="B124" s="31" t="str">
+      <c r="F124" s="97"/>
+    </row>
+    <row r="125" spans="2:6" outlineLevel="1">
+      <c r="B125" s="31" t="str">
         <f>_xlfn.CONCAT(SV_ID,".",TEXT(ROW()-ROW(SV_ID), "000"))</f>
         <v>SV.001</v>
       </c>
-      <c r="C124" s="14" t="s">
+      <c r="C125" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="D124" s="14" t="s">
+      <c r="D125" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E124" s="16" t="s">
+      <c r="E125" s="16" t="s">
         <v>254</v>
       </c>
-      <c r="F124" s="32"/>
-    </row>
-    <row r="125" spans="2:6" ht="210" outlineLevel="1">
-      <c r="B125" s="31" t="str">
+      <c r="F125" s="32"/>
+    </row>
+    <row r="126" spans="2:6" ht="210" outlineLevel="1">
+      <c r="B126" s="31" t="str">
         <f>_xlfn.CONCAT(SV_ID,".",TEXT(ROW()-ROW(SV_ID), "000"))</f>
         <v>SV.002</v>
       </c>
-      <c r="C125" s="14" t="s">
+      <c r="C126" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="D125" s="14" t="s">
+      <c r="D126" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="E125" s="21" t="s">
+      <c r="E126" s="21" t="s">
         <v>501</v>
       </c>
-      <c r="F125" s="32"/>
-    </row>
-    <row r="126" spans="2:6" ht="30" outlineLevel="1">
-      <c r="B126" s="31" t="str">
+      <c r="F126" s="32"/>
+    </row>
+    <row r="127" spans="2:6" ht="30" outlineLevel="1">
+      <c r="B127" s="31" t="str">
         <f>_xlfn.CONCAT(SV_ID,".",TEXT(ROW()-ROW(SV_ID), "000"))</f>
         <v>SV.003</v>
       </c>
-      <c r="C126" s="14" t="s">
+      <c r="C127" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="D126" s="14" t="s">
+      <c r="D127" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E126" s="21" t="s">
+      <c r="E127" s="21" t="s">
         <v>525</v>
       </c>
-      <c r="F126" s="32"/>
-    </row>
-    <row r="127" spans="2:6" outlineLevel="1">
-      <c r="B127" s="31" t="str">
+      <c r="F127" s="32"/>
+    </row>
+    <row r="128" spans="2:6" outlineLevel="1">
+      <c r="B128" s="31" t="str">
         <f>_xlfn.CONCAT(SV_ID,".",TEXT(ROW()-ROW(SV_ID), "000"))</f>
         <v>SV.004</v>
       </c>
-      <c r="C127" s="20" t="s">
+      <c r="C128" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="D127" s="20" t="s">
+      <c r="D128" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="E127" s="21" t="s">
+      <c r="E128" s="21" t="s">
         <v>408</v>
       </c>
-      <c r="F127" s="92"/>
-    </row>
-    <row r="128" spans="2:6" ht="105" outlineLevel="1">
-      <c r="B128" s="31" t="str">
+      <c r="F128" s="92"/>
+    </row>
+    <row r="129" spans="2:6" ht="105" outlineLevel="1">
+      <c r="B129" s="31" t="str">
         <f>_xlfn.CONCAT(SV_ID,".",TEXT(ROW()-ROW(SV_ID), "000"))</f>
         <v>SV.005</v>
       </c>
-      <c r="C128" s="20" t="s">
+      <c r="C129" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="D128" s="20" t="s">
+      <c r="D129" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="E128" s="185" t="s">
+      <c r="E129" s="185" t="s">
         <v>526</v>
       </c>
-      <c r="F128" s="32">
-        <f t="shared" ref="F128" si="8">WARNING_BASE + MID(E128, SEARCH("[",E128) + 1, SEARCH("]",E128) - SEARCH("[",E128) - 1)</f>
+      <c r="F129" s="32">
+        <f t="shared" ref="F129" si="8">WARNING_BASE + MID(E129, SEARCH("[",E129) + 1, SEARCH("]",E129) - SEARCH("[",E129) - 1)</f>
         <v>10020</v>
       </c>
-    </row>
-    <row r="129" spans="2:6" outlineLevel="1">
-      <c r="B129" s="31"/>
-      <c r="C129" s="14"/>
-      <c r="D129" s="14"/>
-      <c r="E129" s="16"/>
-      <c r="F129" s="32"/>
     </row>
     <row r="130" spans="2:6" outlineLevel="1">
       <c r="B130" s="31"/>
@@ -11276,101 +11341,92 @@
       <c r="E130" s="16"/>
       <c r="F130" s="32"/>
     </row>
-    <row r="131" spans="2:6">
-      <c r="B131" s="18" t="s">
+    <row r="131" spans="2:6" outlineLevel="1">
+      <c r="B131" s="31"/>
+      <c r="C131" s="14"/>
+      <c r="D131" s="14"/>
+      <c r="E131" s="16"/>
+      <c r="F131" s="32"/>
+    </row>
+    <row r="132" spans="2:6">
+      <c r="B132" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="C131" s="19"/>
-      <c r="D131" s="19"/>
-      <c r="E131" s="96" t="s">
+      <c r="C132" s="19"/>
+      <c r="D132" s="19"/>
+      <c r="E132" s="96" t="s">
         <v>118</v>
       </c>
-      <c r="F131" s="97"/>
-    </row>
-    <row r="132" spans="2:6" ht="45" outlineLevel="1">
-      <c r="B132" s="91" t="str">
-        <f t="shared" ref="B132:B152" si="9">_xlfn.CONCAT(CC_ID,".",TEXT(ROW()-ROW(CC_ID), "000"))</f>
+      <c r="F132" s="97"/>
+    </row>
+    <row r="133" spans="2:6" ht="45" outlineLevel="1">
+      <c r="B133" s="91" t="str">
+        <f t="shared" ref="B133:B153" si="9">_xlfn.CONCAT(CC_ID,".",TEXT(ROW()-ROW(CC_ID), "000"))</f>
         <v>CC.001</v>
       </c>
-      <c r="C132" s="20" t="s">
+      <c r="C133" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="D132" s="20" t="s">
+      <c r="D133" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E132" s="16" t="s">
+      <c r="E133" s="16" t="s">
         <v>426</v>
       </c>
-      <c r="F132" s="92"/>
-    </row>
-    <row r="133" spans="2:6" ht="135" outlineLevel="1">
-      <c r="B133" s="91" t="str">
+      <c r="F133" s="92"/>
+    </row>
+    <row r="134" spans="2:6" ht="135" outlineLevel="1">
+      <c r="B134" s="91" t="str">
         <f t="shared" si="9"/>
         <v>CC.002</v>
       </c>
-      <c r="C133" s="20" t="s">
+      <c r="C134" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="D133" s="20" t="s">
+      <c r="D134" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E133" s="21" t="s">
+      <c r="E134" s="21" t="s">
         <v>428</v>
       </c>
-      <c r="F133" s="92"/>
-    </row>
-    <row r="134" spans="2:6" outlineLevel="1">
-      <c r="B134" s="91" t="str">
+      <c r="F134" s="92"/>
+    </row>
+    <row r="135" spans="2:6" outlineLevel="1">
+      <c r="B135" s="91" t="str">
         <f t="shared" si="9"/>
         <v>CC.003</v>
       </c>
-      <c r="C134" s="20" t="s">
+      <c r="C135" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="D134" s="20" t="s">
+      <c r="D135" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="E134" s="21" t="s">
+      <c r="E135" s="21" t="s">
         <v>323</v>
       </c>
-      <c r="F134" s="92"/>
-    </row>
-    <row r="135" spans="2:6" ht="180" outlineLevel="1">
-      <c r="B135" s="91" t="str">
+      <c r="F135" s="92"/>
+    </row>
+    <row r="136" spans="2:6" ht="180" outlineLevel="1">
+      <c r="B136" s="91" t="str">
         <f t="shared" si="9"/>
         <v>CC.004</v>
       </c>
-      <c r="C135" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="D135" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="E135" s="21" t="s">
-        <v>419</v>
-      </c>
-      <c r="F135" s="92"/>
-    </row>
-    <row r="136" spans="2:6" ht="45" outlineLevel="1">
-      <c r="B136" s="91" t="str">
-        <f t="shared" si="9"/>
-        <v>CC.005</v>
-      </c>
       <c r="C136" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D136" s="20" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="E136" s="21" t="s">
-        <v>548</v>
+        <v>419</v>
       </c>
       <c r="F136" s="92"/>
     </row>
     <row r="137" spans="2:6" ht="45" outlineLevel="1">
       <c r="B137" s="91" t="str">
         <f t="shared" si="9"/>
-        <v>CC.006</v>
+        <v>CC.005</v>
       </c>
       <c r="C137" s="20" t="s">
         <v>35</v>
@@ -11379,14 +11435,14 @@
         <v>29</v>
       </c>
       <c r="E137" s="21" t="s">
-        <v>543</v>
+        <v>548</v>
       </c>
       <c r="F137" s="92"/>
     </row>
-    <row r="138" spans="2:6" ht="90" outlineLevel="1">
+    <row r="138" spans="2:6" ht="45" outlineLevel="1">
       <c r="B138" s="91" t="str">
         <f t="shared" si="9"/>
-        <v>CC.007</v>
+        <v>CC.006</v>
       </c>
       <c r="C138" s="20" t="s">
         <v>35</v>
@@ -11395,14 +11451,14 @@
         <v>29</v>
       </c>
       <c r="E138" s="21" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="F138" s="92"/>
     </row>
-    <row r="139" spans="2:6" ht="60" outlineLevel="1">
+    <row r="139" spans="2:6" ht="90" outlineLevel="1">
       <c r="B139" s="91" t="str">
         <f t="shared" si="9"/>
-        <v>CC.008</v>
+        <v>CC.007</v>
       </c>
       <c r="C139" s="20" t="s">
         <v>35</v>
@@ -11411,14 +11467,14 @@
         <v>29</v>
       </c>
       <c r="E139" s="21" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="F139" s="92"/>
     </row>
     <row r="140" spans="2:6" ht="60" outlineLevel="1">
       <c r="B140" s="91" t="str">
         <f t="shared" si="9"/>
-        <v>CC.009</v>
+        <v>CC.008</v>
       </c>
       <c r="C140" s="20" t="s">
         <v>35</v>
@@ -11427,14 +11483,14 @@
         <v>29</v>
       </c>
       <c r="E140" s="21" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="F140" s="92"/>
     </row>
     <row r="141" spans="2:6" ht="60" outlineLevel="1">
       <c r="B141" s="91" t="str">
         <f t="shared" si="9"/>
-        <v>CC.010</v>
+        <v>CC.009</v>
       </c>
       <c r="C141" s="20" t="s">
         <v>35</v>
@@ -11443,30 +11499,30 @@
         <v>29</v>
       </c>
       <c r="E141" s="21" t="s">
-        <v>524</v>
+        <v>545</v>
       </c>
       <c r="F141" s="92"/>
     </row>
-    <row r="142" spans="2:6" ht="45" outlineLevel="1">
+    <row r="142" spans="2:6" ht="60" outlineLevel="1">
       <c r="B142" s="91" t="str">
         <f t="shared" si="9"/>
-        <v>CC.011</v>
+        <v>CC.010</v>
       </c>
       <c r="C142" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D142" s="20" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="E142" s="21" t="s">
-        <v>420</v>
+        <v>524</v>
       </c>
       <c r="F142" s="92"/>
     </row>
-    <row r="143" spans="2:6" ht="30" outlineLevel="1">
+    <row r="143" spans="2:6" ht="45" outlineLevel="1">
       <c r="B143" s="91" t="str">
         <f t="shared" si="9"/>
-        <v>CC.012</v>
+        <v>CC.011</v>
       </c>
       <c r="C143" s="20" t="s">
         <v>35</v>
@@ -11475,14 +11531,14 @@
         <v>18</v>
       </c>
       <c r="E143" s="21" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F143" s="92"/>
     </row>
     <row r="144" spans="2:6" ht="30" outlineLevel="1">
       <c r="B144" s="91" t="str">
         <f t="shared" si="9"/>
-        <v>CC.013</v>
+        <v>CC.012</v>
       </c>
       <c r="C144" s="20" t="s">
         <v>35</v>
@@ -11491,46 +11547,46 @@
         <v>18</v>
       </c>
       <c r="E144" s="21" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="F144" s="92"/>
     </row>
     <row r="145" spans="2:6" ht="30" outlineLevel="1">
       <c r="B145" s="91" t="str">
         <f t="shared" si="9"/>
-        <v>CC.014</v>
+        <v>CC.013</v>
       </c>
       <c r="C145" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D145" s="20" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E145" s="21" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="F145" s="92"/>
     </row>
     <row r="146" spans="2:6" ht="30" outlineLevel="1">
       <c r="B146" s="91" t="str">
         <f t="shared" si="9"/>
-        <v>CC.015</v>
+        <v>CC.014</v>
       </c>
       <c r="C146" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D146" s="20" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E146" s="21" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="F146" s="92"/>
     </row>
     <row r="147" spans="2:6" ht="30" outlineLevel="1">
       <c r="B147" s="91" t="str">
         <f t="shared" si="9"/>
-        <v>CC.016</v>
+        <v>CC.015</v>
       </c>
       <c r="C147" s="20" t="s">
         <v>35</v>
@@ -11539,14 +11595,14 @@
         <v>18</v>
       </c>
       <c r="E147" s="21" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="F147" s="92"/>
     </row>
-    <row r="148" spans="2:6" outlineLevel="1">
+    <row r="148" spans="2:6" ht="30" outlineLevel="1">
       <c r="B148" s="91" t="str">
         <f t="shared" si="9"/>
-        <v>CC.017</v>
+        <v>CC.016</v>
       </c>
       <c r="C148" s="20" t="s">
         <v>35</v>
@@ -11555,14 +11611,14 @@
         <v>18</v>
       </c>
       <c r="E148" s="21" t="s">
-        <v>417</v>
+        <v>425</v>
       </c>
       <c r="F148" s="92"/>
     </row>
-    <row r="149" spans="2:6" ht="45" outlineLevel="1">
+    <row r="149" spans="2:6" outlineLevel="1">
       <c r="B149" s="91" t="str">
         <f t="shared" si="9"/>
-        <v>CC.018</v>
+        <v>CC.017</v>
       </c>
       <c r="C149" s="20" t="s">
         <v>35</v>
@@ -11570,50 +11626,50 @@
       <c r="D149" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="E149" s="16" t="s">
-        <v>427</v>
-      </c>
-      <c r="F149" s="32">
-        <f>ALARM_BASE + MID(E149, SEARCH("[",E149) + 1, SEARCH("]",E149) - SEARCH("[",E149) - 1)</f>
-        <v>10230</v>
-      </c>
-    </row>
-    <row r="150" spans="2:6" ht="30" outlineLevel="1">
+      <c r="E149" s="21" t="s">
+        <v>417</v>
+      </c>
+      <c r="F149" s="92"/>
+    </row>
+    <row r="150" spans="2:6" ht="45" outlineLevel="1">
       <c r="B150" s="91" t="str">
         <f t="shared" si="9"/>
-        <v>CC.019</v>
+        <v>CC.018</v>
       </c>
       <c r="C150" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D150" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="E150" s="21" t="s">
-        <v>324</v>
-      </c>
-      <c r="F150" s="92"/>
-    </row>
-    <row r="151" spans="2:6" outlineLevel="1">
+        <v>18</v>
+      </c>
+      <c r="E150" s="16" t="s">
+        <v>427</v>
+      </c>
+      <c r="F150" s="32">
+        <f>ALARM_BASE + MID(E150, SEARCH("[",E150) + 1, SEARCH("]",E150) - SEARCH("[",E150) - 1)</f>
+        <v>10230</v>
+      </c>
+    </row>
+    <row r="151" spans="2:6" ht="30" outlineLevel="1">
       <c r="B151" s="91" t="str">
         <f t="shared" si="9"/>
-        <v>CC.020</v>
+        <v>CC.019</v>
       </c>
       <c r="C151" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D151" s="20" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="E151" s="21" t="s">
-        <v>418</v>
+        <v>324</v>
       </c>
       <c r="F151" s="92"/>
     </row>
-    <row r="152" spans="2:6" ht="75" outlineLevel="1">
+    <row r="152" spans="2:6" outlineLevel="1">
       <c r="B152" s="91" t="str">
         <f t="shared" si="9"/>
-        <v>CC.021</v>
+        <v>CC.020</v>
       </c>
       <c r="C152" s="20" t="s">
         <v>35</v>
@@ -11621,20 +11677,29 @@
       <c r="D152" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="E152" s="185" t="s">
+      <c r="E152" s="21" t="s">
+        <v>418</v>
+      </c>
+      <c r="F152" s="92"/>
+    </row>
+    <row r="153" spans="2:6" ht="75" outlineLevel="1">
+      <c r="B153" s="91" t="str">
+        <f t="shared" si="9"/>
+        <v>CC.021</v>
+      </c>
+      <c r="C153" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D153" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="E153" s="185" t="s">
         <v>562</v>
       </c>
-      <c r="F152" s="32">
-        <f t="shared" ref="F152" si="10">WARNING_BASE + MID(E152, SEARCH("[",E152) + 1, SEARCH("]",E152) - SEARCH("[",E152) - 1)</f>
+      <c r="F153" s="32">
+        <f t="shared" ref="F153" si="10">WARNING_BASE + MID(E153, SEARCH("[",E153) + 1, SEARCH("]",E153) - SEARCH("[",E153) - 1)</f>
         <v>10030</v>
       </c>
-    </row>
-    <row r="153" spans="2:6" outlineLevel="1">
-      <c r="B153" s="91"/>
-      <c r="C153" s="20"/>
-      <c r="D153" s="20"/>
-      <c r="E153" s="21"/>
-      <c r="F153" s="92"/>
     </row>
     <row r="154" spans="2:6" outlineLevel="1">
       <c r="B154" s="91"/>
@@ -11650,54 +11715,54 @@
       <c r="E155" s="21"/>
       <c r="F155" s="92"/>
     </row>
-    <row r="156" spans="2:6">
-      <c r="B156" s="18" t="s">
+    <row r="156" spans="2:6" outlineLevel="1">
+      <c r="B156" s="91"/>
+      <c r="C156" s="20"/>
+      <c r="D156" s="20"/>
+      <c r="E156" s="21"/>
+      <c r="F156" s="92"/>
+    </row>
+    <row r="157" spans="2:6">
+      <c r="B157" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="C156" s="19"/>
-      <c r="D156" s="19"/>
-      <c r="E156" s="96" t="s">
+      <c r="C157" s="19"/>
+      <c r="D157" s="19"/>
+      <c r="E157" s="96" t="s">
         <v>120</v>
       </c>
-      <c r="F156" s="97"/>
-    </row>
-    <row r="157" spans="2:6" ht="30" outlineLevel="1">
-      <c r="B157" s="91" t="str">
+      <c r="F157" s="97"/>
+    </row>
+    <row r="158" spans="2:6" ht="30" outlineLevel="1">
+      <c r="B158" s="91" t="str">
         <f>_xlfn.CONCAT(CF_ID,".",TEXT(ROW()-ROW(CF_ID), "000"))</f>
         <v>CF.001</v>
       </c>
-      <c r="C157" s="20" t="s">
+      <c r="C158" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="D157" s="20" t="s">
+      <c r="D158" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E157" s="16" t="s">
+      <c r="E158" s="16" t="s">
         <v>429</v>
       </c>
-      <c r="F157" s="92"/>
-    </row>
-    <row r="158" spans="2:6" outlineLevel="1">
-      <c r="B158" s="91" t="str">
+      <c r="F158" s="92"/>
+    </row>
+    <row r="159" spans="2:6" outlineLevel="1">
+      <c r="B159" s="91" t="str">
         <f>_xlfn.CONCAT(CF_ID,".",TEXT(ROW()-ROW(CF_ID), "000"))</f>
         <v>CF.002</v>
       </c>
-      <c r="C158" s="20" t="s">
+      <c r="C159" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="D158" s="20" t="s">
+      <c r="D159" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E158" s="21" t="s">
+      <c r="E159" s="21" t="s">
         <v>430</v>
       </c>
-      <c r="F158" s="92"/>
-    </row>
-    <row r="159" spans="2:6" outlineLevel="1">
-      <c r="B159" s="91"/>
-      <c r="C159" s="20"/>
-      <c r="D159" s="20"/>
-      <c r="E159" s="21"/>
       <c r="F159" s="92"/>
     </row>
     <row r="160" spans="2:6" outlineLevel="1">
@@ -11714,141 +11779,141 @@
       <c r="E161" s="21"/>
       <c r="F161" s="92"/>
     </row>
-    <row r="162" spans="2:6">
-      <c r="B162" s="18" t="s">
+    <row r="162" spans="2:6" outlineLevel="1">
+      <c r="B162" s="91"/>
+      <c r="C162" s="20"/>
+      <c r="D162" s="20"/>
+      <c r="E162" s="21"/>
+      <c r="F162" s="92"/>
+    </row>
+    <row r="163" spans="2:6">
+      <c r="B163" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="C162" s="19"/>
-      <c r="D162" s="19"/>
-      <c r="E162" s="96" t="s">
+      <c r="C163" s="19"/>
+      <c r="D163" s="19"/>
+      <c r="E163" s="96" t="s">
         <v>125</v>
       </c>
-      <c r="F162" s="97"/>
-    </row>
-    <row r="163" spans="2:6" ht="30" outlineLevel="1">
-      <c r="B163" s="91" t="str">
-        <f t="shared" ref="B163:B169" si="11">_xlfn.CONCAT(CP_ID,".",TEXT(ROW()-ROW(CP_ID), "000"))</f>
+      <c r="F163" s="97"/>
+    </row>
+    <row r="164" spans="2:6" ht="30" outlineLevel="1">
+      <c r="B164" s="91" t="str">
+        <f t="shared" ref="B164:B170" si="11">_xlfn.CONCAT(CP_ID,".",TEXT(ROW()-ROW(CP_ID), "000"))</f>
         <v>CP.001</v>
       </c>
-      <c r="C163" s="20" t="s">
+      <c r="C164" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="D163" s="20" t="s">
+      <c r="D164" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="E163" s="21" t="s">
+      <c r="E164" s="21" t="s">
         <v>253</v>
       </c>
-      <c r="F163" s="92"/>
-    </row>
-    <row r="164" spans="2:6" ht="195" outlineLevel="1">
-      <c r="B164" s="91" t="str">
+      <c r="F164" s="92"/>
+    </row>
+    <row r="165" spans="2:6" ht="195" outlineLevel="1">
+      <c r="B165" s="91" t="str">
         <f t="shared" si="11"/>
         <v>CP.002</v>
       </c>
-      <c r="C164" s="20" t="s">
+      <c r="C165" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="D164" s="20" t="s">
+      <c r="D165" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="E164" s="21" t="s">
+      <c r="E165" s="21" t="s">
         <v>510</v>
       </c>
-      <c r="F164" s="92"/>
-    </row>
-    <row r="165" spans="2:6" ht="45" outlineLevel="1">
-      <c r="B165" s="91" t="str">
+      <c r="F165" s="92"/>
+    </row>
+    <row r="166" spans="2:6" ht="45" outlineLevel="1">
+      <c r="B166" s="91" t="str">
         <f t="shared" si="11"/>
         <v>CP.003</v>
       </c>
-      <c r="C165" s="20" t="s">
+      <c r="C166" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="D165" s="20" t="s">
+      <c r="D166" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="E165" s="21" t="s">
+      <c r="E166" s="21" t="s">
         <v>511</v>
       </c>
-      <c r="F165" s="92"/>
-    </row>
-    <row r="166" spans="2:6" outlineLevel="1">
-      <c r="B166" s="91" t="str">
+      <c r="F166" s="92"/>
+    </row>
+    <row r="167" spans="2:6" outlineLevel="1">
+      <c r="B167" s="91" t="str">
         <f t="shared" si="11"/>
         <v>CP.004</v>
       </c>
-      <c r="C166" s="20" t="s">
+      <c r="C167" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="D166" s="20" t="s">
+      <c r="D167" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="E166" s="21" t="s">
+      <c r="E167" s="21" t="s">
         <v>409</v>
       </c>
-      <c r="F166" s="92"/>
-    </row>
-    <row r="167" spans="2:6" ht="45" outlineLevel="1">
-      <c r="B167" s="91" t="str">
+      <c r="F167" s="92"/>
+    </row>
+    <row r="168" spans="2:6" ht="45" outlineLevel="1">
+      <c r="B168" s="91" t="str">
         <f t="shared" si="11"/>
         <v>CP.005</v>
       </c>
-      <c r="C167" s="20" t="s">
+      <c r="C168" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="D167" s="20" t="s">
+      <c r="D168" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="E167" s="21" t="s">
+      <c r="E168" s="21" t="s">
         <v>509</v>
       </c>
-      <c r="F167" s="32">
-        <f>ALARM_BASE + MID(E167, SEARCH("[",E167) + 1, SEARCH("]",E167) - SEARCH("[",E167) - 1)</f>
+      <c r="F168" s="32">
+        <f>ALARM_BASE + MID(E168, SEARCH("[",E168) + 1, SEARCH("]",E168) - SEARCH("[",E168) - 1)</f>
         <v>10250</v>
       </c>
     </row>
-    <row r="168" spans="2:6" outlineLevel="1">
-      <c r="B168" s="91" t="str">
+    <row r="169" spans="2:6" outlineLevel="1">
+      <c r="B169" s="91" t="str">
         <f t="shared" si="11"/>
         <v>CP.006</v>
       </c>
-      <c r="C168" s="20" t="s">
+      <c r="C169" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="D168" s="20" t="s">
+      <c r="D169" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="E168" s="21" t="s">
+      <c r="E169" s="21" t="s">
         <v>410</v>
       </c>
-      <c r="F168" s="92"/>
-    </row>
-    <row r="169" spans="2:6" ht="120" outlineLevel="1">
-      <c r="B169" s="91" t="str">
+      <c r="F169" s="92"/>
+    </row>
+    <row r="170" spans="2:6" ht="120" outlineLevel="1">
+      <c r="B170" s="91" t="str">
         <f t="shared" si="11"/>
         <v>CP.007</v>
       </c>
-      <c r="C169" s="20" t="s">
+      <c r="C170" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="D169" s="20" t="s">
+      <c r="D170" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="E169" s="185" t="s">
+      <c r="E170" s="185" t="s">
         <v>515</v>
       </c>
-      <c r="F169" s="32">
-        <f t="shared" ref="F169" si="12">WARNING_BASE + MID(E169, SEARCH("[",E169) + 1, SEARCH("]",E169) - SEARCH("[",E169) - 1)</f>
+      <c r="F170" s="32">
+        <f t="shared" ref="F170" si="12">WARNING_BASE + MID(E170, SEARCH("[",E170) + 1, SEARCH("]",E170) - SEARCH("[",E170) - 1)</f>
         <v>10050</v>
       </c>
-    </row>
-    <row r="170" spans="2:6" outlineLevel="1">
-      <c r="B170" s="91"/>
-      <c r="C170" s="20"/>
-      <c r="D170" s="20"/>
-      <c r="E170" s="21"/>
-      <c r="F170" s="92"/>
     </row>
     <row r="171" spans="2:6" outlineLevel="1">
       <c r="B171" s="91"/>
@@ -11857,86 +11922,86 @@
       <c r="E171" s="21"/>
       <c r="F171" s="92"/>
     </row>
-    <row r="172" spans="2:6">
-      <c r="B172" s="18" t="s">
+    <row r="172" spans="2:6" outlineLevel="1">
+      <c r="B172" s="91"/>
+      <c r="C172" s="20"/>
+      <c r="D172" s="20"/>
+      <c r="E172" s="21"/>
+      <c r="F172" s="92"/>
+    </row>
+    <row r="173" spans="2:6">
+      <c r="B173" s="18" t="s">
         <v>249</v>
       </c>
-      <c r="C172" s="19"/>
-      <c r="D172" s="19"/>
-      <c r="E172" s="96" t="s">
+      <c r="C173" s="19"/>
+      <c r="D173" s="19"/>
+      <c r="E173" s="96" t="s">
         <v>248</v>
       </c>
-      <c r="F172" s="97"/>
-    </row>
-    <row r="173" spans="2:6" ht="45" outlineLevel="1">
-      <c r="B173" s="91" t="str">
+      <c r="F173" s="97"/>
+    </row>
+    <row r="174" spans="2:6" ht="45" outlineLevel="1">
+      <c r="B174" s="91" t="str">
         <f>_xlfn.CONCAT(BO_ID,".",TEXT(ROW()-ROW(BO_ID), "000"))</f>
         <v>BO.001</v>
       </c>
-      <c r="C173" s="20" t="s">
+      <c r="C174" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="D173" s="20" t="s">
+      <c r="D174" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="E173" s="21" t="s">
+      <c r="E174" s="21" t="s">
         <v>247</v>
       </c>
-      <c r="F173" s="92"/>
-    </row>
-    <row r="174" spans="2:6" ht="30" outlineLevel="1">
-      <c r="B174" s="91" t="str">
+      <c r="F174" s="92"/>
+    </row>
+    <row r="175" spans="2:6" ht="30" outlineLevel="1">
+      <c r="B175" s="91" t="str">
         <f>_xlfn.CONCAT(BO_ID,".",TEXT(ROW()-ROW(BO_ID), "000"))</f>
         <v>BO.002</v>
       </c>
-      <c r="C174" s="20" t="s">
+      <c r="C175" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="D174" s="20" t="s">
+      <c r="D175" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="E174" s="21" t="s">
+      <c r="E175" s="21" t="s">
         <v>496</v>
       </c>
-      <c r="F174" s="92"/>
-    </row>
-    <row r="175" spans="2:6" ht="45" outlineLevel="1">
-      <c r="B175" s="91" t="str">
+      <c r="F175" s="92"/>
+    </row>
+    <row r="176" spans="2:6" ht="45" outlineLevel="1">
+      <c r="B176" s="91" t="str">
         <f>_xlfn.CONCAT(BO_ID,".",TEXT(ROW()-ROW(BO_ID), "000"))</f>
         <v>BO.003</v>
       </c>
-      <c r="C175" s="20" t="s">
+      <c r="C176" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="D175" s="20" t="s">
+      <c r="D176" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="E175" s="21" t="s">
+      <c r="E176" s="21" t="s">
         <v>250</v>
       </c>
-      <c r="F175" s="92"/>
-    </row>
-    <row r="176" spans="2:6" ht="30" outlineLevel="1">
-      <c r="B176" s="91" t="str">
+      <c r="F176" s="92"/>
+    </row>
+    <row r="177" spans="2:6" ht="30" outlineLevel="1">
+      <c r="B177" s="91" t="str">
         <f>_xlfn.CONCAT(BO_ID,".",TEXT(ROW()-ROW(BO_ID), "000"))</f>
         <v>BO.004</v>
       </c>
-      <c r="C176" s="20" t="s">
+      <c r="C177" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="D176" s="20" t="s">
+      <c r="D177" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="E176" s="21" t="s">
+      <c r="E177" s="21" t="s">
         <v>495</v>
       </c>
-      <c r="F176" s="92"/>
-    </row>
-    <row r="177" spans="2:6" outlineLevel="1">
-      <c r="B177" s="91"/>
-      <c r="C177" s="20"/>
-      <c r="D177" s="20"/>
-      <c r="E177" s="21"/>
       <c r="F177" s="92"/>
     </row>
     <row r="178" spans="2:6" outlineLevel="1">
@@ -11946,70 +12011,61 @@
       <c r="E178" s="21"/>
       <c r="F178" s="92"/>
     </row>
-    <row r="179" spans="2:6">
-      <c r="B179" s="18" t="s">
+    <row r="179" spans="2:6" outlineLevel="1">
+      <c r="B179" s="91"/>
+      <c r="C179" s="20"/>
+      <c r="D179" s="20"/>
+      <c r="E179" s="21"/>
+      <c r="F179" s="92"/>
+    </row>
+    <row r="180" spans="2:6">
+      <c r="B180" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="C179" s="19"/>
-      <c r="D179" s="19"/>
-      <c r="E179" s="96" t="s">
+      <c r="C180" s="19"/>
+      <c r="D180" s="19"/>
+      <c r="E180" s="96" t="s">
         <v>123</v>
       </c>
-      <c r="F179" s="97"/>
-    </row>
-    <row r="180" spans="2:6" ht="210" outlineLevel="1">
-      <c r="B180" s="91" t="str">
-        <f t="shared" ref="B180:B196" si="13">_xlfn.CONCAT(UO_ID,".",TEXT(ROW()-ROW(UO_ID), "000"))</f>
+      <c r="F180" s="97"/>
+    </row>
+    <row r="181" spans="2:6" ht="210" outlineLevel="1">
+      <c r="B181" s="91" t="str">
+        <f t="shared" ref="B181:B197" si="13">_xlfn.CONCAT(UO_ID,".",TEXT(ROW()-ROW(UO_ID), "000"))</f>
         <v>UO.001</v>
       </c>
-      <c r="C180" s="20" t="s">
+      <c r="C181" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="D180" s="20" t="s">
+      <c r="D181" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="E180" s="21" t="s">
+      <c r="E181" s="21" t="s">
         <v>512</v>
       </c>
-      <c r="F180" s="92"/>
-    </row>
-    <row r="181" spans="2:6" ht="45" outlineLevel="1">
-      <c r="B181" s="91" t="str">
+      <c r="F181" s="92"/>
+    </row>
+    <row r="182" spans="2:6" ht="45" outlineLevel="1">
+      <c r="B182" s="91" t="str">
         <f t="shared" si="13"/>
         <v>UO.002</v>
       </c>
-      <c r="C181" s="20" t="s">
+      <c r="C182" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="D181" s="20" t="s">
+      <c r="D182" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="E181" s="21" t="s">
+      <c r="E182" s="21" t="s">
         <v>485</v>
       </c>
-      <c r="F181" s="92"/>
-    </row>
-    <row r="182" spans="2:6" outlineLevel="1">
-      <c r="B182" s="91" t="str">
+      <c r="F182" s="92"/>
+    </row>
+    <row r="183" spans="2:6" outlineLevel="1">
+      <c r="B183" s="91" t="str">
         <f t="shared" si="13"/>
         <v>UO.003</v>
       </c>
-      <c r="C182" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="D182" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="E182" s="21" t="s">
-        <v>514</v>
-      </c>
-      <c r="F182" s="92"/>
-    </row>
-    <row r="183" spans="2:6" ht="30" outlineLevel="1">
-      <c r="B183" s="91" t="str">
-        <f t="shared" si="13"/>
-        <v>UO.004</v>
-      </c>
       <c r="C183" s="20" t="s">
         <v>35</v>
       </c>
@@ -12017,14 +12073,14 @@
         <v>29</v>
       </c>
       <c r="E183" s="21" t="s">
-        <v>566</v>
+        <v>514</v>
       </c>
       <c r="F183" s="92"/>
     </row>
     <row r="184" spans="2:6" ht="30" outlineLevel="1">
       <c r="B184" s="91" t="str">
         <f t="shared" si="13"/>
-        <v>UO.005</v>
+        <v>UO.004</v>
       </c>
       <c r="C184" s="20" t="s">
         <v>35</v>
@@ -12033,14 +12089,14 @@
         <v>29</v>
       </c>
       <c r="E184" s="21" t="s">
-        <v>414</v>
+        <v>566</v>
       </c>
       <c r="F184" s="92"/>
     </row>
-    <row r="185" spans="2:6" ht="45" outlineLevel="1">
+    <row r="185" spans="2:6" ht="30" outlineLevel="1">
       <c r="B185" s="91" t="str">
         <f t="shared" si="13"/>
-        <v>UO.006</v>
+        <v>UO.005</v>
       </c>
       <c r="C185" s="20" t="s">
         <v>35</v>
@@ -12049,14 +12105,14 @@
         <v>29</v>
       </c>
       <c r="E185" s="21" t="s">
-        <v>486</v>
+        <v>414</v>
       </c>
       <c r="F185" s="92"/>
     </row>
     <row r="186" spans="2:6" ht="45" outlineLevel="1">
       <c r="B186" s="91" t="str">
         <f t="shared" si="13"/>
-        <v>UO.007</v>
+        <v>UO.006</v>
       </c>
       <c r="C186" s="20" t="s">
         <v>35</v>
@@ -12065,14 +12121,14 @@
         <v>29</v>
       </c>
       <c r="E186" s="21" t="s">
-        <v>513</v>
+        <v>486</v>
       </c>
       <c r="F186" s="92"/>
     </row>
-    <row r="187" spans="2:6" ht="30" outlineLevel="1">
+    <row r="187" spans="2:6" ht="45" outlineLevel="1">
       <c r="B187" s="91" t="str">
         <f t="shared" si="13"/>
-        <v>UO.008</v>
+        <v>UO.007</v>
       </c>
       <c r="C187" s="20" t="s">
         <v>35</v>
@@ -12081,14 +12137,14 @@
         <v>29</v>
       </c>
       <c r="E187" s="21" t="s">
-        <v>487</v>
+        <v>513</v>
       </c>
       <c r="F187" s="92"/>
     </row>
     <row r="188" spans="2:6" ht="30" outlineLevel="1">
       <c r="B188" s="91" t="str">
         <f t="shared" si="13"/>
-        <v>UO.009</v>
+        <v>UO.008</v>
       </c>
       <c r="C188" s="20" t="s">
         <v>35</v>
@@ -12097,14 +12153,14 @@
         <v>29</v>
       </c>
       <c r="E188" s="21" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="F188" s="92"/>
     </row>
-    <row r="189" spans="2:6" outlineLevel="1">
+    <row r="189" spans="2:6" ht="30" outlineLevel="1">
       <c r="B189" s="91" t="str">
         <f t="shared" si="13"/>
-        <v>UO.010</v>
+        <v>UO.009</v>
       </c>
       <c r="C189" s="20" t="s">
         <v>35</v>
@@ -12113,14 +12169,14 @@
         <v>29</v>
       </c>
       <c r="E189" s="21" t="s">
-        <v>498</v>
+        <v>488</v>
       </c>
       <c r="F189" s="92"/>
     </row>
-    <row r="190" spans="2:6" ht="45" outlineLevel="1">
+    <row r="190" spans="2:6" outlineLevel="1">
       <c r="B190" s="91" t="str">
         <f t="shared" si="13"/>
-        <v>UO.011</v>
+        <v>UO.010</v>
       </c>
       <c r="C190" s="20" t="s">
         <v>35</v>
@@ -12128,18 +12184,15 @@
       <c r="D190" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="E190" s="185" t="s">
-        <v>499</v>
-      </c>
-      <c r="F190" s="32">
-        <f t="shared" ref="F190:F191" si="14">WARNING_BASE + MID(E190, SEARCH("[",E190) + 1, SEARCH("]",E190) - SEARCH("[",E190) - 1)</f>
-        <v>10060</v>
-      </c>
-    </row>
-    <row r="191" spans="2:6" ht="75" outlineLevel="1">
+      <c r="E190" s="21" t="s">
+        <v>498</v>
+      </c>
+      <c r="F190" s="92"/>
+    </row>
+    <row r="191" spans="2:6" ht="45" outlineLevel="1">
       <c r="B191" s="91" t="str">
         <f t="shared" si="13"/>
-        <v>UO.012</v>
+        <v>UO.011</v>
       </c>
       <c r="C191" s="20" t="s">
         <v>35</v>
@@ -12148,34 +12201,37 @@
         <v>29</v>
       </c>
       <c r="E191" s="185" t="s">
+        <v>499</v>
+      </c>
+      <c r="F191" s="32">
+        <f t="shared" ref="F191:F192" si="14">WARNING_BASE + MID(E191, SEARCH("[",E191) + 1, SEARCH("]",E191) - SEARCH("[",E191) - 1)</f>
+        <v>10060</v>
+      </c>
+    </row>
+    <row r="192" spans="2:6" ht="75" outlineLevel="1">
+      <c r="B192" s="91" t="str">
+        <f t="shared" si="13"/>
+        <v>UO.012</v>
+      </c>
+      <c r="C192" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D192" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="E192" s="185" t="s">
         <v>560</v>
       </c>
-      <c r="F191" s="32">
+      <c r="F192" s="32">
         <f t="shared" si="14"/>
         <v>10061</v>
       </c>
     </row>
-    <row r="192" spans="2:6" outlineLevel="1">
-      <c r="B192" s="91" t="str">
+    <row r="193" spans="2:6" outlineLevel="1">
+      <c r="B193" s="91" t="str">
         <f t="shared" si="13"/>
         <v>UO.013</v>
       </c>
-      <c r="C192" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="D192" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="E192" s="21" t="s">
-        <v>415</v>
-      </c>
-      <c r="F192" s="92"/>
-    </row>
-    <row r="193" spans="2:6" ht="45" outlineLevel="1">
-      <c r="B193" s="91" t="str">
-        <f t="shared" si="13"/>
-        <v>UO.014</v>
-      </c>
       <c r="C193" s="20" t="s">
         <v>35</v>
       </c>
@@ -12183,17 +12239,14 @@
         <v>29</v>
       </c>
       <c r="E193" s="21" t="s">
-        <v>508</v>
-      </c>
-      <c r="F193" s="32">
-        <f>ALARM_BASE + MID(E193, SEARCH("[",E193) + 1, SEARCH("]",E193) - SEARCH("[",E193) - 1)</f>
-        <v>10260</v>
-      </c>
+        <v>415</v>
+      </c>
+      <c r="F193" s="92"/>
     </row>
     <row r="194" spans="2:6" ht="45" outlineLevel="1">
       <c r="B194" s="91" t="str">
         <f t="shared" si="13"/>
-        <v>UO.015</v>
+        <v>UO.014</v>
       </c>
       <c r="C194" s="20" t="s">
         <v>35</v>
@@ -12202,17 +12255,17 @@
         <v>29</v>
       </c>
       <c r="E194" s="21" t="s">
-        <v>416</v>
+        <v>508</v>
       </c>
       <c r="F194" s="32">
         <f>ALARM_BASE + MID(E194, SEARCH("[",E194) + 1, SEARCH("]",E194) - SEARCH("[",E194) - 1)</f>
-        <v>10261</v>
+        <v>10260</v>
       </c>
     </row>
     <row r="195" spans="2:6" ht="45" outlineLevel="1">
       <c r="B195" s="91" t="str">
         <f t="shared" si="13"/>
-        <v>UO.016</v>
+        <v>UO.015</v>
       </c>
       <c r="C195" s="20" t="s">
         <v>35</v>
@@ -12221,17 +12274,17 @@
         <v>29</v>
       </c>
       <c r="E195" s="21" t="s">
-        <v>534</v>
+        <v>416</v>
       </c>
       <c r="F195" s="32">
         <f>ALARM_BASE + MID(E195, SEARCH("[",E195) + 1, SEARCH("]",E195) - SEARCH("[",E195) - 1)</f>
-        <v>10262</v>
-      </c>
-    </row>
-    <row r="196" spans="2:6" ht="90" outlineLevel="1">
+        <v>10261</v>
+      </c>
+    </row>
+    <row r="196" spans="2:6" ht="45" outlineLevel="1">
       <c r="B196" s="91" t="str">
         <f t="shared" si="13"/>
-        <v>UO.017</v>
+        <v>UO.016</v>
       </c>
       <c r="C196" s="20" t="s">
         <v>35</v>
@@ -12240,19 +12293,31 @@
         <v>29</v>
       </c>
       <c r="E196" s="21" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="F196" s="32">
         <f>ALARM_BASE + MID(E196, SEARCH("[",E196) + 1, SEARCH("]",E196) - SEARCH("[",E196) - 1)</f>
+        <v>10262</v>
+      </c>
+    </row>
+    <row r="197" spans="2:6" ht="90" outlineLevel="1">
+      <c r="B197" s="91" t="str">
+        <f t="shared" si="13"/>
+        <v>UO.017</v>
+      </c>
+      <c r="C197" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D197" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="E197" s="21" t="s">
+        <v>535</v>
+      </c>
+      <c r="F197" s="32">
+        <f>ALARM_BASE + MID(E197, SEARCH("[",E197) + 1, SEARCH("]",E197) - SEARCH("[",E197) - 1)</f>
         <v>10263</v>
       </c>
-    </row>
-    <row r="197" spans="2:6" outlineLevel="1">
-      <c r="B197" s="91"/>
-      <c r="C197" s="20"/>
-      <c r="D197" s="20"/>
-      <c r="E197" s="21"/>
-      <c r="F197" s="92"/>
     </row>
     <row r="198" spans="2:6" outlineLevel="1">
       <c r="B198" s="91"/>
@@ -12261,29 +12326,29 @@
       <c r="E198" s="21"/>
       <c r="F198" s="92"/>
     </row>
-    <row r="199" spans="2:6">
-      <c r="B199" s="18" t="s">
+    <row r="199" spans="2:6" outlineLevel="1">
+      <c r="B199" s="91"/>
+      <c r="C199" s="20"/>
+      <c r="D199" s="20"/>
+      <c r="E199" s="21"/>
+      <c r="F199" s="92"/>
+    </row>
+    <row r="200" spans="2:6">
+      <c r="B200" s="18" t="s">
         <v>201</v>
       </c>
-      <c r="C199" s="19"/>
-      <c r="D199" s="19"/>
-      <c r="E199" s="96" t="s">
+      <c r="C200" s="19"/>
+      <c r="D200" s="19"/>
+      <c r="E200" s="96" t="s">
         <v>202</v>
       </c>
-      <c r="F199" s="97"/>
-    </row>
-    <row r="200" spans="2:6" outlineLevel="1">
-      <c r="B200" s="91" t="str">
+      <c r="F200" s="97"/>
+    </row>
+    <row r="201" spans="2:6" outlineLevel="1">
+      <c r="B201" s="91" t="str">
         <f>_xlfn.CONCAT(GP_ID,".",TEXT(ROW()-ROW(GP_ID), "000"))</f>
         <v>GP.001</v>
       </c>
-      <c r="C200" s="20"/>
-      <c r="D200" s="20"/>
-      <c r="E200" s="21"/>
-      <c r="F200" s="92"/>
-    </row>
-    <row r="201" spans="2:6" outlineLevel="1">
-      <c r="B201" s="91"/>
       <c r="C201" s="20"/>
       <c r="D201" s="20"/>
       <c r="E201" s="21"/>
@@ -12310,19 +12375,19 @@
       <c r="E204" s="21"/>
       <c r="F204" s="92"/>
     </row>
-    <row r="205" spans="2:6">
-      <c r="B205" s="181"/>
-      <c r="C205" s="182"/>
-      <c r="D205" s="182"/>
-      <c r="E205" s="183"/>
-      <c r="F205" s="184"/>
-    </row>
-    <row r="206" spans="2:6" outlineLevel="1">
-      <c r="B206" s="91"/>
-      <c r="C206" s="20"/>
-      <c r="D206" s="20"/>
-      <c r="E206" s="21"/>
-      <c r="F206" s="92"/>
+    <row r="205" spans="2:6" outlineLevel="1">
+      <c r="B205" s="91"/>
+      <c r="C205" s="20"/>
+      <c r="D205" s="20"/>
+      <c r="E205" s="21"/>
+      <c r="F205" s="92"/>
+    </row>
+    <row r="206" spans="2:6">
+      <c r="B206" s="181"/>
+      <c r="C206" s="182"/>
+      <c r="D206" s="182"/>
+      <c r="E206" s="183"/>
+      <c r="F206" s="184"/>
     </row>
     <row r="207" spans="2:6" outlineLevel="1">
       <c r="B207" s="91"/>
@@ -12359,28 +12424,35 @@
       <c r="E211" s="21"/>
       <c r="F211" s="92"/>
     </row>
-    <row r="212" spans="2:6">
-      <c r="B212" s="220" t="s">
+    <row r="212" spans="2:6" outlineLevel="1">
+      <c r="B212" s="91"/>
+      <c r="C212" s="20"/>
+      <c r="D212" s="20"/>
+      <c r="E212" s="21"/>
+      <c r="F212" s="92"/>
+    </row>
+    <row r="213" spans="2:6">
+      <c r="B213" s="220" t="s">
         <v>106</v>
       </c>
-      <c r="C212" s="220"/>
-      <c r="D212" s="220"/>
-      <c r="E212" s="220"/>
-      <c r="F212" s="220"/>
-    </row>
-    <row r="213" spans="2:6">
-      <c r="B213" s="22"/>
-      <c r="C213" s="22"/>
-      <c r="D213" s="22"/>
-      <c r="E213" s="22"/>
-      <c r="F213" s="22"/>
+      <c r="C213" s="220"/>
+      <c r="D213" s="220"/>
+      <c r="E213" s="220"/>
+      <c r="F213" s="220"/>
+    </row>
+    <row r="214" spans="2:6">
+      <c r="B214" s="22"/>
+      <c r="C214" s="22"/>
+      <c r="D214" s="22"/>
+      <c r="E214" s="22"/>
+      <c r="F214" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B212:F212"/>
+    <mergeCell ref="B213:F213"/>
   </mergeCells>
   <phoneticPr fontId="22" type="noConversion"/>
-  <conditionalFormatting sqref="E200:E204 E173:E178 E206:E211 E2:E16 E95:E122 E125:E130 E163:E171 E157:E161 E180:E198 E132:E155 E18:E89">
+  <conditionalFormatting sqref="E201:E205 E174:E179 E207:E212 E2:E16 E95:E123 E126:E131 E164:E172 E158:E162 E181:E199 E133:E156 E18:E89">
     <cfRule type="expression" dxfId="97" priority="93">
       <formula>$C2="Nice to have"</formula>
     </cfRule>
@@ -12388,7 +12460,7 @@
       <formula>$C2="Deprecated"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D200:D204 D173:D178 D206:D211 D125:D130 D3:D16 D95:D122 D163:D171 D157:D161 D180:D198 D18:D89 D132:D155">
+  <conditionalFormatting sqref="D201:D205 D174:D179 D207:D212 D126:D131 D3:D16 D95:D123 D164:D172 D158:D162 D181:D199 D18:D89 D133:D156">
     <cfRule type="cellIs" dxfId="95" priority="92" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
@@ -12405,15 +12477,15 @@
       <formula>"Pending Approval"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E131">
+  <conditionalFormatting sqref="E132">
     <cfRule type="expression" dxfId="90" priority="86">
-      <formula>$C131="Nice to have"</formula>
+      <formula>$C132="Nice to have"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="89" priority="91">
-      <formula>$C131="Deprecated"</formula>
+      <formula>$C132="Deprecated"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D131">
+  <conditionalFormatting sqref="D132">
     <cfRule type="cellIs" dxfId="88" priority="85" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
@@ -12430,15 +12502,15 @@
       <formula>"Pending Approval"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E156">
+  <conditionalFormatting sqref="E157">
     <cfRule type="expression" dxfId="83" priority="79">
-      <formula>$C156="Nice to have"</formula>
+      <formula>$C157="Nice to have"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="82" priority="84">
-      <formula>$C156="Deprecated"</formula>
+      <formula>$C157="Deprecated"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D156">
+  <conditionalFormatting sqref="D157">
     <cfRule type="cellIs" dxfId="81" priority="78" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
@@ -12455,15 +12527,15 @@
       <formula>"Pending Approval"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E162">
+  <conditionalFormatting sqref="E163">
     <cfRule type="expression" dxfId="76" priority="72">
-      <formula>$C162="Nice to have"</formula>
+      <formula>$C163="Nice to have"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="75" priority="77">
-      <formula>$C162="Deprecated"</formula>
+      <formula>$C163="Deprecated"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D162">
+  <conditionalFormatting sqref="D163">
     <cfRule type="cellIs" dxfId="74" priority="71" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
@@ -12480,15 +12552,15 @@
       <formula>"Pending Approval"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E179">
+  <conditionalFormatting sqref="E180">
     <cfRule type="expression" dxfId="69" priority="65">
-      <formula>$C179="Nice to have"</formula>
+      <formula>$C180="Nice to have"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="68" priority="70">
-      <formula>$C179="Deprecated"</formula>
+      <formula>$C180="Deprecated"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D179">
+  <conditionalFormatting sqref="D180">
     <cfRule type="cellIs" dxfId="67" priority="64" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
@@ -12505,15 +12577,15 @@
       <formula>"Pending Approval"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E199">
+  <conditionalFormatting sqref="E200">
     <cfRule type="expression" dxfId="62" priority="58">
-      <formula>$C199="Nice to have"</formula>
+      <formula>$C200="Nice to have"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="61" priority="63">
-      <formula>$C199="Deprecated"</formula>
+      <formula>$C200="Deprecated"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D199">
+  <conditionalFormatting sqref="D200">
     <cfRule type="cellIs" dxfId="60" priority="57" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
@@ -12530,15 +12602,15 @@
       <formula>"Pending Approval"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E205">
+  <conditionalFormatting sqref="E206">
     <cfRule type="expression" dxfId="55" priority="51">
-      <formula>$C205="Nice to have"</formula>
+      <formula>$C206="Nice to have"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="54" priority="56">
-      <formula>$C205="Deprecated"</formula>
+      <formula>$C206="Deprecated"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D205">
+  <conditionalFormatting sqref="D206">
     <cfRule type="cellIs" dxfId="53" priority="50" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
@@ -12555,15 +12627,15 @@
       <formula>"Pending Approval"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E172">
+  <conditionalFormatting sqref="E173">
     <cfRule type="expression" dxfId="48" priority="37">
-      <formula>$C172="Nice to have"</formula>
+      <formula>$C173="Nice to have"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="47" priority="42">
-      <formula>$C172="Deprecated"</formula>
+      <formula>$C173="Deprecated"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D172">
+  <conditionalFormatting sqref="D173">
     <cfRule type="cellIs" dxfId="46" priority="36" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
@@ -12580,15 +12652,15 @@
       <formula>"Pending Approval"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E123">
+  <conditionalFormatting sqref="E124">
     <cfRule type="expression" dxfId="41" priority="30">
-      <formula>$C123="Nice to have"</formula>
+      <formula>$C124="Nice to have"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="40" priority="35">
-      <formula>$C123="Deprecated"</formula>
+      <formula>$C124="Deprecated"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D123">
+  <conditionalFormatting sqref="D124">
     <cfRule type="cellIs" dxfId="39" priority="29" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
@@ -12605,15 +12677,15 @@
       <formula>"Pending Approval"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E124">
+  <conditionalFormatting sqref="E125">
     <cfRule type="expression" dxfId="34" priority="23">
-      <formula>$C124="Nice to have"</formula>
+      <formula>$C125="Nice to have"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="33" priority="28">
-      <formula>$C124="Deprecated"</formula>
+      <formula>$C125="Deprecated"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D124">
+  <conditionalFormatting sqref="D125">
     <cfRule type="cellIs" dxfId="32" priority="22" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
@@ -12706,10 +12778,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C211" xr:uid="{00000000-0002-0000-0400-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C212" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <formula1>settings.level</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D211" xr:uid="{00000000-0002-0000-0400-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D212" xr:uid="{00000000-0002-0000-0400-000001000000}">
       <formula1>settings.status</formula1>
     </dataValidation>
   </dataValidations>
@@ -12725,7 +12797,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04C1D18A-550F-418B-B18E-9DAD1CC7BE2C}">
   <dimension ref="B1:K86"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -12794,7 +12866,7 @@
       </c>
       <c r="E3" s="136">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F3" s="138"/>
       <c r="G3" s="141"/>
@@ -12845,7 +12917,7 @@
       </c>
       <c r="E5" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F5" s="168" t="s">
         <v>220</v>
@@ -12874,7 +12946,7 @@
       </c>
       <c r="E6" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F6" s="168" t="s">
         <v>221</v>
@@ -12899,7 +12971,7 @@
       </c>
       <c r="E7" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F7" s="168" t="s">
         <v>262</v>
@@ -12926,7 +12998,7 @@
       </c>
       <c r="E8" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F8" s="168" t="s">
         <v>262</v>
@@ -12951,7 +13023,7 @@
       </c>
       <c r="E9" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F9" s="175" t="s">
         <v>221</v>
@@ -13005,7 +13077,7 @@
       </c>
       <c r="E11" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F11" s="175" t="s">
         <v>220</v>
@@ -13077,7 +13149,7 @@
       </c>
       <c r="E15" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F15" s="145"/>
       <c r="G15" s="148"/>
@@ -13101,7 +13173,7 @@
       </c>
       <c r="E16" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F16" s="162" t="s">
         <v>220</v>
@@ -13131,7 +13203,7 @@
       </c>
       <c r="E17" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F17" s="162" t="s">
         <v>220</v>
@@ -13158,7 +13230,7 @@
       </c>
       <c r="E18" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F18" s="195"/>
       <c r="G18" s="165"/>
@@ -13183,7 +13255,7 @@
       </c>
       <c r="E19" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F19" s="162" t="s">
         <v>262</v>
@@ -13242,7 +13314,7 @@
       </c>
       <c r="E22" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F22" s="145"/>
       <c r="G22" s="148"/>
@@ -13291,7 +13363,7 @@
       </c>
       <c r="E24" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F24" s="155"/>
       <c r="G24" s="159"/>
@@ -13316,7 +13388,7 @@
       </c>
       <c r="E25" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F25" s="155" t="s">
         <v>221</v>
@@ -13343,7 +13415,7 @@
       </c>
       <c r="E26" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F26" s="177" t="s">
         <v>220</v>
@@ -13370,7 +13442,7 @@
       </c>
       <c r="E27" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F27" s="177" t="s">
         <v>220</v>
@@ -13397,7 +13469,7 @@
       </c>
       <c r="E28" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F28" s="177" t="s">
         <v>220</v>
@@ -13449,7 +13521,7 @@
       </c>
       <c r="E30" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F30" s="155"/>
       <c r="G30" s="159"/>
@@ -13474,7 +13546,7 @@
       </c>
       <c r="E31" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F31" s="155"/>
       <c r="G31" s="159"/>
@@ -13499,7 +13571,7 @@
       </c>
       <c r="E32" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F32" s="177"/>
       <c r="G32" s="159"/>
@@ -13524,7 +13596,7 @@
       </c>
       <c r="E33" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F33" s="177"/>
       <c r="G33" s="159"/>
@@ -13549,7 +13621,7 @@
       </c>
       <c r="E34" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F34" s="177"/>
       <c r="G34" s="159"/>
@@ -13574,7 +13646,7 @@
       </c>
       <c r="E35" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F35" s="155"/>
       <c r="G35" s="159"/>
@@ -13599,7 +13671,7 @@
       </c>
       <c r="E36" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F36" s="155"/>
       <c r="G36" s="159"/>
@@ -13624,7 +13696,7 @@
       </c>
       <c r="E37" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F37" s="155"/>
       <c r="G37" s="159"/>
@@ -13649,7 +13721,7 @@
       </c>
       <c r="E38" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F38" s="155"/>
       <c r="G38" s="159"/>
@@ -13674,7 +13746,7 @@
       </c>
       <c r="E39" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F39" s="155"/>
       <c r="G39" s="159">
@@ -13712,7 +13784,7 @@
       </c>
       <c r="E41" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F41" s="155"/>
       <c r="G41" s="159">
@@ -13767,7 +13839,7 @@
       </c>
       <c r="E44" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F44" s="145"/>
       <c r="G44" s="148"/>
@@ -13791,7 +13863,7 @@
       </c>
       <c r="E45" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F45" s="186"/>
       <c r="G45" s="189"/>
@@ -13816,7 +13888,7 @@
       </c>
       <c r="E46" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F46" s="186"/>
       <c r="G46" s="189"/>
@@ -13841,7 +13913,7 @@
       </c>
       <c r="E47" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F47" s="193"/>
       <c r="G47" s="189"/>
@@ -13866,7 +13938,7 @@
       </c>
       <c r="E48" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F48" s="193" t="s">
         <v>220</v>
@@ -13893,7 +13965,7 @@
       </c>
       <c r="E49" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F49" s="193"/>
       <c r="G49" s="189"/>
@@ -13918,7 +13990,7 @@
       </c>
       <c r="E50" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F50" s="193"/>
       <c r="G50" s="189"/>
@@ -13943,7 +14015,7 @@
       </c>
       <c r="E51" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F51" s="193" t="s">
         <v>220</v>
@@ -13970,7 +14042,7 @@
       </c>
       <c r="E52" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F52" s="186"/>
       <c r="G52" s="189"/>
@@ -13995,7 +14067,7 @@
       </c>
       <c r="E53" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F53" s="193"/>
       <c r="G53" s="189"/>
@@ -14020,7 +14092,7 @@
       </c>
       <c r="E54" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F54" s="193"/>
       <c r="G54" s="189"/>
@@ -14045,7 +14117,7 @@
       </c>
       <c r="E55" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F55" s="193" t="s">
         <v>220</v>
@@ -14072,7 +14144,7 @@
       </c>
       <c r="E56" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F56" s="193" t="s">
         <v>220</v>

</xml_diff>

<commit_message>
Duplicates AI/DI to my variables; Add CAREL fast DI board offline warning; Solo mode is done;
</commit_message>
<xml_diff>
--- a/BZ172Lab/BZ172Lab Notes.xlsx
+++ b/BZ172Lab/BZ172Lab Notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BZ\Projects\PLC61131Repos\BZ172Lab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C839F8-21B3-4CDB-B0C9-935C04F022CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCECF0B7-1CF9-4617-93DC-DB31D7C44EA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4089,21 +4089,51 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="10" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="15" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="15" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -4112,36 +4142,6 @@
     </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="18" xfId="11" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="10" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="15" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="15" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="2" borderId="1" xfId="12" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -8195,7 +8195,7 @@
       </c>
       <c r="F22" s="196">
         <f ca="1">TODAY()</f>
-        <v>44259</v>
+        <v>44260</v>
       </c>
       <c r="G22" s="196"/>
       <c r="H22" s="196"/>
@@ -8602,23 +8602,23 @@
   </cols>
   <sheetData>
     <row r="2" spans="4:7">
-      <c r="D2" s="208">
+      <c r="D2" s="218">
         <f ca="1">TODAY()</f>
-        <v>44259</v>
-      </c>
-      <c r="E2" s="208"/>
-      <c r="F2" s="208"/>
+        <v>44260</v>
+      </c>
+      <c r="E2" s="218"/>
+      <c r="F2" s="218"/>
     </row>
     <row r="3" spans="4:7">
-      <c r="D3" s="209"/>
-      <c r="E3" s="209"/>
-      <c r="F3" s="209"/>
+      <c r="D3" s="219"/>
+      <c r="E3" s="219"/>
+      <c r="F3" s="219"/>
     </row>
     <row r="4" spans="4:7">
-      <c r="D4" s="207" t="s">
+      <c r="D4" s="217" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="207"/>
+      <c r="E4" s="217"/>
       <c r="F4" s="27">
         <f>COUNTIF(FRS.Level, D4)</f>
         <v>139</v>
@@ -8626,10 +8626,10 @@
       <c r="G4" s="26"/>
     </row>
     <row r="5" spans="4:7">
-      <c r="D5" s="207" t="s">
+      <c r="D5" s="217" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="207"/>
+      <c r="E5" s="217"/>
       <c r="F5" s="27">
         <f>COUNTIF(FRS.Level, D5)</f>
         <v>7</v>
@@ -8637,10 +8637,10 @@
       <c r="G5" s="26"/>
     </row>
     <row r="6" spans="4:7">
-      <c r="D6" s="207" t="s">
+      <c r="D6" s="217" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="207"/>
+      <c r="E6" s="217"/>
       <c r="F6" s="27">
         <f>COUNTIF(FRS.Level, D6)</f>
         <v>6</v>
@@ -8648,10 +8648,10 @@
       <c r="G6" s="26"/>
     </row>
     <row r="7" spans="4:7">
-      <c r="D7" s="207" t="s">
+      <c r="D7" s="217" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="207"/>
+      <c r="E7" s="217"/>
       <c r="F7" s="27">
         <f>COUNTIF(FRS.Level, D7)</f>
         <v>0</v>
@@ -8668,134 +8668,134 @@
       <c r="G8" s="26"/>
     </row>
     <row r="10" spans="4:7">
-      <c r="D10" s="207" t="s">
+      <c r="D10" s="217" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="207"/>
+      <c r="E10" s="217"/>
       <c r="F10" s="27">
         <f t="shared" ref="F10:F16" si="0">COUNTIF(FRS.Status,D10)</f>
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="4:7">
-      <c r="D11" s="207" t="s">
+      <c r="D11" s="217" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="207"/>
+      <c r="E11" s="217"/>
       <c r="F11" s="27">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="4:7">
-      <c r="D12" s="207" t="s">
+      <c r="D12" s="217" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="207"/>
+      <c r="E12" s="217"/>
       <c r="F12" s="27">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="4:7">
-      <c r="D13" s="207" t="s">
+      <c r="D13" s="217" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="207"/>
+      <c r="E13" s="217"/>
       <c r="F13" s="27">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="4:7">
-      <c r="D14" s="207" t="s">
+      <c r="D14" s="217" t="s">
         <v>24</v>
       </c>
-      <c r="E14" s="207"/>
+      <c r="E14" s="217"/>
       <c r="F14" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="4:7">
-      <c r="D15" s="207" t="s">
+      <c r="D15" s="217" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="207"/>
+      <c r="E15" s="217"/>
       <c r="F15" s="27">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="4:7">
-      <c r="D16" s="207" t="s">
+      <c r="D16" s="217" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="207"/>
+      <c r="E16" s="217"/>
       <c r="F16" s="27">
         <f t="shared" si="0"/>
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="4:19" ht="20.25" thickBot="1">
-      <c r="D18" s="219" t="s">
+      <c r="D18" s="209" t="s">
         <v>46</v>
       </c>
-      <c r="E18" s="219"/>
-      <c r="F18" s="219"/>
-      <c r="G18" s="219"/>
-      <c r="H18" s="218" t="s">
+      <c r="E18" s="209"/>
+      <c r="F18" s="209"/>
+      <c r="G18" s="209"/>
+      <c r="H18" s="208" t="s">
         <v>47</v>
       </c>
-      <c r="I18" s="218"/>
-      <c r="J18" s="218"/>
-      <c r="K18" s="218"/>
-      <c r="L18" s="218"/>
-      <c r="M18" s="218"/>
-      <c r="N18" s="218"/>
-      <c r="O18" s="218"/>
-      <c r="P18" s="218"/>
-      <c r="Q18" s="218"/>
+      <c r="I18" s="208"/>
+      <c r="J18" s="208"/>
+      <c r="K18" s="208"/>
+      <c r="L18" s="208"/>
+      <c r="M18" s="208"/>
+      <c r="N18" s="208"/>
+      <c r="O18" s="208"/>
+      <c r="P18" s="208"/>
+      <c r="Q18" s="208"/>
     </row>
     <row r="19" spans="4:19" ht="15.75" thickTop="1">
-      <c r="D19" s="215" t="s">
+      <c r="D19" s="202" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="215"/>
-      <c r="F19" s="215" t="s">
+      <c r="E19" s="202"/>
+      <c r="F19" s="202" t="s">
         <v>2</v>
       </c>
-      <c r="G19" s="215"/>
-      <c r="H19" s="215" t="s">
+      <c r="G19" s="202"/>
+      <c r="H19" s="202" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="215"/>
-      <c r="J19" s="215" t="s">
+      <c r="I19" s="202"/>
+      <c r="J19" s="202" t="s">
         <v>18</v>
       </c>
-      <c r="K19" s="215"/>
-      <c r="L19" s="215" t="s">
+      <c r="K19" s="202"/>
+      <c r="L19" s="202" t="s">
         <v>15</v>
       </c>
-      <c r="M19" s="215"/>
-      <c r="N19" s="215" t="s">
+      <c r="M19" s="202"/>
+      <c r="N19" s="202" t="s">
         <v>21</v>
       </c>
-      <c r="O19" s="215"/>
-      <c r="P19" s="215" t="s">
+      <c r="O19" s="202"/>
+      <c r="P19" s="202" t="s">
         <v>29</v>
       </c>
-      <c r="Q19" s="215"/>
+      <c r="Q19" s="202"/>
     </row>
     <row r="20" spans="4:19">
-      <c r="D20" s="202">
+      <c r="D20" s="203">
         <v>44221</v>
       </c>
-      <c r="E20" s="203"/>
-      <c r="F20" s="204" t="s">
+      <c r="E20" s="204"/>
+      <c r="F20" s="212" t="s">
         <v>109</v>
       </c>
-      <c r="G20" s="204"/>
+      <c r="G20" s="212"/>
       <c r="H20" s="205">
         <v>8</v>
       </c>
@@ -8812,21 +8812,21 @@
         <v>0</v>
       </c>
       <c r="O20" s="205"/>
-      <c r="P20" s="216">
+      <c r="P20" s="206">
         <v>0</v>
       </c>
-      <c r="Q20" s="217"/>
+      <c r="Q20" s="207"/>
       <c r="S20" s="28"/>
     </row>
     <row r="21" spans="4:19">
-      <c r="D21" s="202">
+      <c r="D21" s="203">
         <v>44237</v>
       </c>
-      <c r="E21" s="203"/>
-      <c r="F21" s="204" t="s">
+      <c r="E21" s="204"/>
+      <c r="F21" s="212" t="s">
         <v>487</v>
       </c>
-      <c r="G21" s="204"/>
+      <c r="G21" s="212"/>
       <c r="H21" s="205">
         <v>9</v>
       </c>
@@ -8846,17 +8846,17 @@
       <c r="P21" s="205">
         <v>56</v>
       </c>
-      <c r="Q21" s="206"/>
+      <c r="Q21" s="215"/>
     </row>
     <row r="22" spans="4:19">
-      <c r="D22" s="202">
+      <c r="D22" s="203">
         <v>44256</v>
       </c>
-      <c r="E22" s="203"/>
-      <c r="F22" s="204" t="s">
+      <c r="E22" s="204"/>
+      <c r="F22" s="212" t="s">
         <v>551</v>
       </c>
-      <c r="G22" s="204"/>
+      <c r="G22" s="212"/>
       <c r="H22" s="205">
         <v>4</v>
       </c>
@@ -8876,15 +8876,15 @@
       <c r="P22" s="205">
         <v>90</v>
       </c>
-      <c r="Q22" s="206"/>
+      <c r="Q22" s="215"/>
     </row>
     <row r="23" spans="4:19">
-      <c r="D23" s="202">
+      <c r="D23" s="203">
         <v>44287</v>
       </c>
-      <c r="E23" s="203"/>
-      <c r="F23" s="204"/>
-      <c r="G23" s="204"/>
+      <c r="E23" s="204"/>
+      <c r="F23" s="212"/>
+      <c r="G23" s="212"/>
       <c r="H23" s="205"/>
       <c r="I23" s="205"/>
       <c r="J23" s="205"/>
@@ -8894,13 +8894,13 @@
       <c r="N23" s="205"/>
       <c r="O23" s="205"/>
       <c r="P23" s="205"/>
-      <c r="Q23" s="206"/>
+      <c r="Q23" s="215"/>
     </row>
     <row r="24" spans="4:19">
-      <c r="D24" s="202"/>
-      <c r="E24" s="203"/>
-      <c r="F24" s="204"/>
-      <c r="G24" s="204"/>
+      <c r="D24" s="203"/>
+      <c r="E24" s="204"/>
+      <c r="F24" s="212"/>
+      <c r="G24" s="212"/>
       <c r="H24" s="205"/>
       <c r="I24" s="205"/>
       <c r="J24" s="205"/>
@@ -8910,13 +8910,13 @@
       <c r="N24" s="205"/>
       <c r="O24" s="205"/>
       <c r="P24" s="205"/>
-      <c r="Q24" s="206"/>
+      <c r="Q24" s="215"/>
     </row>
     <row r="25" spans="4:19">
-      <c r="D25" s="202"/>
-      <c r="E25" s="203"/>
-      <c r="F25" s="204"/>
-      <c r="G25" s="204"/>
+      <c r="D25" s="203"/>
+      <c r="E25" s="204"/>
+      <c r="F25" s="212"/>
+      <c r="G25" s="212"/>
       <c r="H25" s="205"/>
       <c r="I25" s="205"/>
       <c r="J25" s="205"/>
@@ -8926,13 +8926,13 @@
       <c r="N25" s="205"/>
       <c r="O25" s="205"/>
       <c r="P25" s="205"/>
-      <c r="Q25" s="206"/>
+      <c r="Q25" s="215"/>
     </row>
     <row r="26" spans="4:19">
-      <c r="D26" s="202"/>
-      <c r="E26" s="203"/>
-      <c r="F26" s="204"/>
-      <c r="G26" s="204"/>
+      <c r="D26" s="203"/>
+      <c r="E26" s="204"/>
+      <c r="F26" s="212"/>
+      <c r="G26" s="212"/>
       <c r="H26" s="205"/>
       <c r="I26" s="205"/>
       <c r="J26" s="205"/>
@@ -8942,13 +8942,13 @@
       <c r="N26" s="205"/>
       <c r="O26" s="205"/>
       <c r="P26" s="205"/>
-      <c r="Q26" s="206"/>
+      <c r="Q26" s="215"/>
     </row>
     <row r="27" spans="4:19">
-      <c r="D27" s="202"/>
-      <c r="E27" s="203"/>
-      <c r="F27" s="204"/>
-      <c r="G27" s="204"/>
+      <c r="D27" s="203"/>
+      <c r="E27" s="204"/>
+      <c r="F27" s="212"/>
+      <c r="G27" s="212"/>
       <c r="H27" s="205"/>
       <c r="I27" s="205"/>
       <c r="J27" s="205"/>
@@ -8958,13 +8958,13 @@
       <c r="N27" s="205"/>
       <c r="O27" s="205"/>
       <c r="P27" s="205"/>
-      <c r="Q27" s="206"/>
+      <c r="Q27" s="215"/>
     </row>
     <row r="28" spans="4:19">
-      <c r="D28" s="202"/>
-      <c r="E28" s="203"/>
-      <c r="F28" s="204"/>
-      <c r="G28" s="204"/>
+      <c r="D28" s="203"/>
+      <c r="E28" s="204"/>
+      <c r="F28" s="212"/>
+      <c r="G28" s="212"/>
       <c r="H28" s="205"/>
       <c r="I28" s="205"/>
       <c r="J28" s="205"/>
@@ -8974,13 +8974,13 @@
       <c r="N28" s="205"/>
       <c r="O28" s="205"/>
       <c r="P28" s="205"/>
-      <c r="Q28" s="206"/>
+      <c r="Q28" s="215"/>
     </row>
     <row r="29" spans="4:19">
-      <c r="D29" s="202"/>
-      <c r="E29" s="203"/>
-      <c r="F29" s="204"/>
-      <c r="G29" s="204"/>
+      <c r="D29" s="203"/>
+      <c r="E29" s="204"/>
+      <c r="F29" s="212"/>
+      <c r="G29" s="212"/>
       <c r="H29" s="205"/>
       <c r="I29" s="205"/>
       <c r="J29" s="205"/>
@@ -8990,13 +8990,13 @@
       <c r="N29" s="205"/>
       <c r="O29" s="205"/>
       <c r="P29" s="205"/>
-      <c r="Q29" s="206"/>
+      <c r="Q29" s="215"/>
     </row>
     <row r="30" spans="4:19">
-      <c r="D30" s="202"/>
-      <c r="E30" s="203"/>
-      <c r="F30" s="204"/>
-      <c r="G30" s="204"/>
+      <c r="D30" s="203"/>
+      <c r="E30" s="204"/>
+      <c r="F30" s="212"/>
+      <c r="G30" s="212"/>
       <c r="H30" s="205"/>
       <c r="I30" s="205"/>
       <c r="J30" s="205"/>
@@ -9006,13 +9006,13 @@
       <c r="N30" s="205"/>
       <c r="O30" s="205"/>
       <c r="P30" s="205"/>
-      <c r="Q30" s="206"/>
+      <c r="Q30" s="215"/>
     </row>
     <row r="31" spans="4:19">
-      <c r="D31" s="202"/>
-      <c r="E31" s="203"/>
-      <c r="F31" s="204"/>
-      <c r="G31" s="204"/>
+      <c r="D31" s="203"/>
+      <c r="E31" s="204"/>
+      <c r="F31" s="212"/>
+      <c r="G31" s="212"/>
       <c r="H31" s="205"/>
       <c r="I31" s="205"/>
       <c r="J31" s="205"/>
@@ -9022,13 +9022,13 @@
       <c r="N31" s="205"/>
       <c r="O31" s="205"/>
       <c r="P31" s="205"/>
-      <c r="Q31" s="206"/>
+      <c r="Q31" s="215"/>
     </row>
     <row r="32" spans="4:19">
-      <c r="D32" s="202"/>
-      <c r="E32" s="203"/>
-      <c r="F32" s="204"/>
-      <c r="G32" s="204"/>
+      <c r="D32" s="203"/>
+      <c r="E32" s="204"/>
+      <c r="F32" s="212"/>
+      <c r="G32" s="212"/>
       <c r="H32" s="205"/>
       <c r="I32" s="205"/>
       <c r="J32" s="205"/>
@@ -9038,13 +9038,13 @@
       <c r="N32" s="205"/>
       <c r="O32" s="205"/>
       <c r="P32" s="205"/>
-      <c r="Q32" s="206"/>
+      <c r="Q32" s="215"/>
     </row>
     <row r="33" spans="4:17">
-      <c r="D33" s="202"/>
-      <c r="E33" s="203"/>
-      <c r="F33" s="204"/>
-      <c r="G33" s="204"/>
+      <c r="D33" s="203"/>
+      <c r="E33" s="204"/>
+      <c r="F33" s="212"/>
+      <c r="G33" s="212"/>
       <c r="H33" s="205"/>
       <c r="I33" s="205"/>
       <c r="J33" s="205"/>
@@ -9054,13 +9054,13 @@
       <c r="N33" s="205"/>
       <c r="O33" s="205"/>
       <c r="P33" s="205"/>
-      <c r="Q33" s="206"/>
+      <c r="Q33" s="215"/>
     </row>
     <row r="34" spans="4:17">
-      <c r="D34" s="202"/>
-      <c r="E34" s="203"/>
-      <c r="F34" s="204"/>
-      <c r="G34" s="204"/>
+      <c r="D34" s="203"/>
+      <c r="E34" s="204"/>
+      <c r="F34" s="212"/>
+      <c r="G34" s="212"/>
       <c r="H34" s="205"/>
       <c r="I34" s="205"/>
       <c r="J34" s="205"/>
@@ -9070,13 +9070,13 @@
       <c r="N34" s="205"/>
       <c r="O34" s="205"/>
       <c r="P34" s="205"/>
-      <c r="Q34" s="206"/>
+      <c r="Q34" s="215"/>
     </row>
     <row r="35" spans="4:17">
-      <c r="D35" s="202"/>
-      <c r="E35" s="203"/>
-      <c r="F35" s="204"/>
-      <c r="G35" s="204"/>
+      <c r="D35" s="203"/>
+      <c r="E35" s="204"/>
+      <c r="F35" s="212"/>
+      <c r="G35" s="212"/>
       <c r="H35" s="205"/>
       <c r="I35" s="205"/>
       <c r="J35" s="205"/>
@@ -9086,13 +9086,13 @@
       <c r="N35" s="205"/>
       <c r="O35" s="205"/>
       <c r="P35" s="205"/>
-      <c r="Q35" s="206"/>
+      <c r="Q35" s="215"/>
     </row>
     <row r="36" spans="4:17">
-      <c r="D36" s="202"/>
-      <c r="E36" s="203"/>
-      <c r="F36" s="204"/>
-      <c r="G36" s="204"/>
+      <c r="D36" s="203"/>
+      <c r="E36" s="204"/>
+      <c r="F36" s="212"/>
+      <c r="G36" s="212"/>
       <c r="H36" s="205"/>
       <c r="I36" s="205"/>
       <c r="J36" s="205"/>
@@ -9102,13 +9102,13 @@
       <c r="N36" s="205"/>
       <c r="O36" s="205"/>
       <c r="P36" s="205"/>
-      <c r="Q36" s="206"/>
+      <c r="Q36" s="215"/>
     </row>
     <row r="37" spans="4:17">
-      <c r="D37" s="202"/>
-      <c r="E37" s="203"/>
-      <c r="F37" s="204"/>
-      <c r="G37" s="204"/>
+      <c r="D37" s="203"/>
+      <c r="E37" s="204"/>
+      <c r="F37" s="212"/>
+      <c r="G37" s="212"/>
       <c r="H37" s="205"/>
       <c r="I37" s="205"/>
       <c r="J37" s="205"/>
@@ -9118,13 +9118,13 @@
       <c r="N37" s="205"/>
       <c r="O37" s="205"/>
       <c r="P37" s="205"/>
-      <c r="Q37" s="206"/>
+      <c r="Q37" s="215"/>
     </row>
     <row r="38" spans="4:17">
-      <c r="D38" s="202"/>
-      <c r="E38" s="203"/>
-      <c r="F38" s="204"/>
-      <c r="G38" s="204"/>
+      <c r="D38" s="203"/>
+      <c r="E38" s="204"/>
+      <c r="F38" s="212"/>
+      <c r="G38" s="212"/>
       <c r="H38" s="205"/>
       <c r="I38" s="205"/>
       <c r="J38" s="205"/>
@@ -9134,13 +9134,13 @@
       <c r="N38" s="205"/>
       <c r="O38" s="205"/>
       <c r="P38" s="205"/>
-      <c r="Q38" s="206"/>
+      <c r="Q38" s="215"/>
     </row>
     <row r="39" spans="4:17">
-      <c r="D39" s="202"/>
-      <c r="E39" s="203"/>
-      <c r="F39" s="204"/>
-      <c r="G39" s="204"/>
+      <c r="D39" s="203"/>
+      <c r="E39" s="204"/>
+      <c r="F39" s="212"/>
+      <c r="G39" s="212"/>
       <c r="H39" s="205"/>
       <c r="I39" s="205"/>
       <c r="J39" s="205"/>
@@ -9150,23 +9150,23 @@
       <c r="N39" s="205"/>
       <c r="O39" s="205"/>
       <c r="P39" s="205"/>
-      <c r="Q39" s="206"/>
+      <c r="Q39" s="215"/>
     </row>
     <row r="40" spans="4:17">
-      <c r="D40" s="213"/>
-      <c r="E40" s="214"/>
-      <c r="F40" s="212"/>
-      <c r="G40" s="212"/>
-      <c r="H40" s="210"/>
-      <c r="I40" s="210"/>
-      <c r="J40" s="210"/>
-      <c r="K40" s="210"/>
-      <c r="L40" s="210"/>
-      <c r="M40" s="210"/>
-      <c r="N40" s="210"/>
-      <c r="O40" s="210"/>
-      <c r="P40" s="210"/>
-      <c r="Q40" s="211"/>
+      <c r="D40" s="210"/>
+      <c r="E40" s="211"/>
+      <c r="F40" s="213"/>
+      <c r="G40" s="213"/>
+      <c r="H40" s="214"/>
+      <c r="I40" s="214"/>
+      <c r="J40" s="214"/>
+      <c r="K40" s="214"/>
+      <c r="L40" s="214"/>
+      <c r="M40" s="214"/>
+      <c r="N40" s="214"/>
+      <c r="O40" s="214"/>
+      <c r="P40" s="214"/>
+      <c r="Q40" s="216"/>
     </row>
     <row r="41" spans="4:17">
       <c r="D41" s="24"/>
@@ -9174,21 +9174,135 @@
     </row>
   </sheetData>
   <mergeCells count="168">
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="P19:Q19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="H18:Q18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="D18:G18"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="L34:M34"/>
+    <mergeCell ref="N34:O34"/>
+    <mergeCell ref="P34:Q34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="J35:K35"/>
+    <mergeCell ref="L35:M35"/>
+    <mergeCell ref="N35:O35"/>
+    <mergeCell ref="P35:Q35"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="L31:M31"/>
+    <mergeCell ref="N31:O31"/>
+    <mergeCell ref="P31:Q31"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="N29:O29"/>
+    <mergeCell ref="P29:Q29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="N30:O30"/>
+    <mergeCell ref="P30:Q30"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D2:F3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="P38:Q38"/>
+    <mergeCell ref="P39:Q39"/>
+    <mergeCell ref="P40:Q40"/>
+    <mergeCell ref="P26:Q26"/>
+    <mergeCell ref="P27:Q27"/>
+    <mergeCell ref="P28:Q28"/>
+    <mergeCell ref="P32:Q32"/>
+    <mergeCell ref="P33:Q33"/>
+    <mergeCell ref="P36:Q36"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="P22:Q22"/>
+    <mergeCell ref="P23:Q23"/>
+    <mergeCell ref="P24:Q24"/>
+    <mergeCell ref="P25:Q25"/>
+    <mergeCell ref="N33:O33"/>
+    <mergeCell ref="N36:O36"/>
+    <mergeCell ref="N37:O37"/>
+    <mergeCell ref="P37:Q37"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="N38:O38"/>
+    <mergeCell ref="N39:O39"/>
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="N26:O26"/>
+    <mergeCell ref="N27:O27"/>
+    <mergeCell ref="N28:O28"/>
+    <mergeCell ref="N32:O32"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="L37:M37"/>
+    <mergeCell ref="L38:M38"/>
+    <mergeCell ref="L39:M39"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="L40:M40"/>
+    <mergeCell ref="L26:M26"/>
+    <mergeCell ref="L27:M27"/>
+    <mergeCell ref="L28:M28"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="L33:M33"/>
+    <mergeCell ref="L36:M36"/>
+    <mergeCell ref="N40:O40"/>
+    <mergeCell ref="J33:K33"/>
+    <mergeCell ref="J36:K36"/>
+    <mergeCell ref="J37:K37"/>
+    <mergeCell ref="J38:K38"/>
+    <mergeCell ref="J39:K39"/>
+    <mergeCell ref="J40:K40"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="H36:I36"/>
     <mergeCell ref="D37:E37"/>
     <mergeCell ref="D38:E38"/>
     <mergeCell ref="D39:E39"/>
@@ -9213,135 +9327,21 @@
     <mergeCell ref="F37:G37"/>
     <mergeCell ref="F38:G38"/>
     <mergeCell ref="F39:G39"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="H40:I40"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="L40:M40"/>
-    <mergeCell ref="L26:M26"/>
-    <mergeCell ref="L27:M27"/>
-    <mergeCell ref="L28:M28"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="L33:M33"/>
-    <mergeCell ref="L36:M36"/>
-    <mergeCell ref="N40:O40"/>
-    <mergeCell ref="J33:K33"/>
-    <mergeCell ref="J36:K36"/>
-    <mergeCell ref="J37:K37"/>
-    <mergeCell ref="J38:K38"/>
-    <mergeCell ref="J39:K39"/>
-    <mergeCell ref="J40:K40"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="L24:M24"/>
-    <mergeCell ref="L25:M25"/>
-    <mergeCell ref="N38:O38"/>
-    <mergeCell ref="N39:O39"/>
-    <mergeCell ref="N24:O24"/>
-    <mergeCell ref="N25:O25"/>
-    <mergeCell ref="N26:O26"/>
-    <mergeCell ref="N27:O27"/>
-    <mergeCell ref="N28:O28"/>
-    <mergeCell ref="N32:O32"/>
-    <mergeCell ref="N21:O21"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="L37:M37"/>
-    <mergeCell ref="L38:M38"/>
-    <mergeCell ref="L39:M39"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="P21:Q21"/>
-    <mergeCell ref="P22:Q22"/>
-    <mergeCell ref="P23:Q23"/>
-    <mergeCell ref="P24:Q24"/>
-    <mergeCell ref="P25:Q25"/>
-    <mergeCell ref="N33:O33"/>
-    <mergeCell ref="N36:O36"/>
-    <mergeCell ref="N37:O37"/>
-    <mergeCell ref="P37:Q37"/>
-    <mergeCell ref="P38:Q38"/>
-    <mergeCell ref="P39:Q39"/>
-    <mergeCell ref="P40:Q40"/>
-    <mergeCell ref="P26:Q26"/>
-    <mergeCell ref="P27:Q27"/>
-    <mergeCell ref="P28:Q28"/>
-    <mergeCell ref="P32:Q32"/>
-    <mergeCell ref="P33:Q33"/>
-    <mergeCell ref="P36:Q36"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D2:F3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="L31:M31"/>
-    <mergeCell ref="N31:O31"/>
-    <mergeCell ref="P31:Q31"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="L29:M29"/>
-    <mergeCell ref="N29:O29"/>
-    <mergeCell ref="P29:Q29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="N30:O30"/>
-    <mergeCell ref="P30:Q30"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="J34:K34"/>
-    <mergeCell ref="L34:M34"/>
-    <mergeCell ref="N34:O34"/>
-    <mergeCell ref="P34:Q34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="J35:K35"/>
-    <mergeCell ref="L35:M35"/>
-    <mergeCell ref="N35:O35"/>
-    <mergeCell ref="P35:Q35"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="H18:Q18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="D18:G18"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="N20:O20"/>
   </mergeCells>
   <phoneticPr fontId="22" type="noConversion"/>
   <dataValidations disablePrompts="1" count="1">
@@ -9369,7 +9369,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomRight" activeCell="D83" sqref="D83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -9418,7 +9418,7 @@
         <v>35</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="E4" s="29" t="s">
         <v>578</v>
@@ -10294,7 +10294,7 @@
       </c>
       <c r="F60" s="92"/>
     </row>
-    <row r="61" spans="2:6" ht="285" outlineLevel="1">
+    <row r="61" spans="2:6" ht="300" outlineLevel="1">
       <c r="B61" s="30" t="str">
         <f t="shared" si="3"/>
         <v>VF.010</v>
@@ -10691,7 +10691,7 @@
         <v>35</v>
       </c>
       <c r="D83" s="14" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="E83" s="16" t="s">
         <v>574</v>
@@ -12867,7 +12867,7 @@
       </c>
       <c r="E3" s="136">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F3" s="138"/>
       <c r="G3" s="141"/>
@@ -12918,7 +12918,7 @@
       </c>
       <c r="E5" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F5" s="168" t="s">
         <v>219</v>
@@ -12947,7 +12947,7 @@
       </c>
       <c r="E6" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F6" s="168" t="s">
         <v>220</v>
@@ -12972,7 +12972,7 @@
       </c>
       <c r="E7" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F7" s="168" t="s">
         <v>261</v>
@@ -12999,7 +12999,7 @@
       </c>
       <c r="E8" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F8" s="168" t="s">
         <v>261</v>
@@ -13024,7 +13024,7 @@
       </c>
       <c r="E9" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F9" s="175" t="s">
         <v>220</v>
@@ -13078,7 +13078,7 @@
       </c>
       <c r="E11" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F11" s="175" t="s">
         <v>219</v>
@@ -13150,7 +13150,7 @@
       </c>
       <c r="E15" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F15" s="145"/>
       <c r="G15" s="148"/>
@@ -13174,7 +13174,7 @@
       </c>
       <c r="E16" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F16" s="162" t="s">
         <v>219</v>
@@ -13204,7 +13204,7 @@
       </c>
       <c r="E17" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F17" s="162" t="s">
         <v>219</v>
@@ -13231,7 +13231,7 @@
       </c>
       <c r="E18" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F18" s="195"/>
       <c r="G18" s="165"/>
@@ -13256,7 +13256,7 @@
       </c>
       <c r="E19" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F19" s="162" t="s">
         <v>261</v>
@@ -13315,7 +13315,7 @@
       </c>
       <c r="E22" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F22" s="145"/>
       <c r="G22" s="148"/>
@@ -13416,7 +13416,7 @@
       </c>
       <c r="E26" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F26" s="177" t="s">
         <v>219</v>
@@ -13443,7 +13443,7 @@
       </c>
       <c r="E27" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F27" s="177" t="s">
         <v>219</v>
@@ -13470,7 +13470,7 @@
       </c>
       <c r="E28" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F28" s="177" t="s">
         <v>219</v>
@@ -13522,7 +13522,7 @@
       </c>
       <c r="E30" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F30" s="155"/>
       <c r="G30" s="159"/>
@@ -13547,7 +13547,7 @@
       </c>
       <c r="E31" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F31" s="155"/>
       <c r="G31" s="159"/>
@@ -13597,7 +13597,7 @@
       </c>
       <c r="E33" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F33" s="177"/>
       <c r="G33" s="159"/>
@@ -13647,7 +13647,7 @@
       </c>
       <c r="E35" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F35" s="155"/>
       <c r="G35" s="159"/>
@@ -13672,7 +13672,7 @@
       </c>
       <c r="E36" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F36" s="155"/>
       <c r="G36" s="159"/>
@@ -13697,7 +13697,7 @@
       </c>
       <c r="E37" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F37" s="155"/>
       <c r="G37" s="159"/>
@@ -13722,7 +13722,7 @@
       </c>
       <c r="E38" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F38" s="155"/>
       <c r="G38" s="159"/>
@@ -13747,7 +13747,7 @@
       </c>
       <c r="E39" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F39" s="155"/>
       <c r="G39" s="159">
@@ -13785,7 +13785,7 @@
       </c>
       <c r="E41" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F41" s="155"/>
       <c r="G41" s="159">
@@ -13840,7 +13840,7 @@
       </c>
       <c r="E44" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F44" s="145"/>
       <c r="G44" s="148"/>
@@ -13864,7 +13864,7 @@
       </c>
       <c r="E45" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F45" s="186"/>
       <c r="G45" s="189"/>
@@ -13889,7 +13889,7 @@
       </c>
       <c r="E46" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F46" s="186"/>
       <c r="G46" s="189"/>
@@ -13914,7 +13914,7 @@
       </c>
       <c r="E47" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F47" s="193"/>
       <c r="G47" s="189"/>
@@ -13939,7 +13939,7 @@
       </c>
       <c r="E48" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F48" s="193" t="s">
         <v>219</v>
@@ -13966,7 +13966,7 @@
       </c>
       <c r="E49" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F49" s="193"/>
       <c r="G49" s="189"/>
@@ -13991,7 +13991,7 @@
       </c>
       <c r="E50" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F50" s="193"/>
       <c r="G50" s="189"/>
@@ -14016,7 +14016,7 @@
       </c>
       <c r="E51" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F51" s="193" t="s">
         <v>219</v>
@@ -14043,7 +14043,7 @@
       </c>
       <c r="E52" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F52" s="186"/>
       <c r="G52" s="189"/>
@@ -14068,7 +14068,7 @@
       </c>
       <c r="E53" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F53" s="193"/>
       <c r="G53" s="189"/>
@@ -14093,7 +14093,7 @@
       </c>
       <c r="E54" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F54" s="193"/>
       <c r="G54" s="189"/>
@@ -14118,7 +14118,7 @@
       </c>
       <c r="E55" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F55" s="193" t="s">
         <v>219</v>
@@ -14145,7 +14145,7 @@
       </c>
       <c r="E56" s="137">
         <f ca="1">IF(OR(ISBLANK(Table1[[#This Row],[Due]]),TODAY()&gt;Table1[[#This Row],[Due]]),0,NETWORKDAYS(TODAY(),Table1[[#This Row],[Due]]))</f>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F56" s="193" t="s">
         <v>219</v>

</xml_diff>